<commit_message>
updated Tier 2 MWWS
</commit_message>
<xml_diff>
--- a/PIT4/Schema Publication Changelog.xlsx
+++ b/PIT4/Schema Publication Changelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\paye-employers-documentation\src\main\resources\PIT4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8580A0-DEFE-4B9A-BCB7-6DF196C41006}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D08015D-38CF-41EA-AB8E-137DEEB6B6D9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3397,10 +3397,10 @@
     <t>Added section on TWSS</t>
   </si>
   <si>
-    <t>Tier 1</t>
-  </si>
-  <si>
     <t>Updated description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier 1 &amp; Tier 2 MWWS </t>
   </si>
 </sst>
 </file>
@@ -4450,38 +4450,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4504,6 +4474,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4525,79 +4555,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4609,47 +4615,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5663,7 +5663,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5673,7 +5673,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5783,10 +5783,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="161" t="s">
+      <c r="A7" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5797,8 +5797,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="161"/>
-      <c r="B8" s="162"/>
+      <c r="A8" s="176"/>
+      <c r="B8" s="175"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5807,8 +5807,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="161"/>
-      <c r="B9" s="162"/>
+      <c r="A9" s="176"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5817,8 +5817,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="161"/>
-      <c r="B10" s="162"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="175"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5827,8 +5827,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="161"/>
-      <c r="B11" s="162"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="175"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5837,8 +5837,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="161"/>
-      <c r="B12" s="162"/>
+      <c r="A12" s="176"/>
+      <c r="B12" s="175"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5847,10 +5847,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="164" t="s">
+      <c r="A13" s="178" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5861,8 +5861,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="164"/>
-      <c r="B14" s="162"/>
+      <c r="A14" s="178"/>
+      <c r="B14" s="175"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5871,8 +5871,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="164"/>
-      <c r="B15" s="162"/>
+      <c r="A15" s="178"/>
+      <c r="B15" s="175"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5881,10 +5881,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="165" t="s">
+      <c r="A16" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="166" t="s">
+      <c r="B16" s="170" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5895,8 +5895,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="165"/>
-      <c r="B17" s="166"/>
+      <c r="A17" s="161"/>
+      <c r="B17" s="170"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5905,8 +5905,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="165"/>
-      <c r="B18" s="166"/>
+      <c r="A18" s="161"/>
+      <c r="B18" s="170"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5915,8 +5915,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="165"/>
-      <c r="B19" s="166"/>
+      <c r="A19" s="161"/>
+      <c r="B19" s="170"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5925,8 +5925,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="165"/>
-      <c r="B20" s="166"/>
+      <c r="A20" s="161"/>
+      <c r="B20" s="170"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5935,8 +5935,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="165"/>
-      <c r="B21" s="166"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="170"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5945,8 +5945,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="165"/>
-      <c r="B22" s="166"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="170"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5955,8 +5955,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="165"/>
-      <c r="B23" s="166"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="170"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5965,26 +5965,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="165"/>
-      <c r="B24" s="166"/>
-      <c r="C24" s="165" t="s">
+      <c r="A24" s="161"/>
+      <c r="B24" s="170"/>
+      <c r="C24" s="161" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="172" t="s">
+      <c r="D24" s="162" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="165"/>
-      <c r="B25" s="166"/>
-      <c r="C25" s="165"/>
-      <c r="D25" s="172"/>
+      <c r="A25" s="161"/>
+      <c r="B25" s="170"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="162"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="161" t="s">
+      <c r="A26" s="176" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="162" t="s">
+      <c r="B26" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5995,8 +5995,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="161"/>
-      <c r="B27" s="162"/>
+      <c r="A27" s="176"/>
+      <c r="B27" s="175"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -6023,28 +6023,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="163" t="s">
+      <c r="A30" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="162" t="s">
+      <c r="B30" s="175" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="165" t="s">
+      <c r="C30" s="161" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="175" t="s">
+      <c r="D30" s="165" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="163"/>
-      <c r="B31" s="162"/>
-      <c r="C31" s="165"/>
-      <c r="D31" s="175"/>
+      <c r="A31" s="177"/>
+      <c r="B31" s="175"/>
+      <c r="C31" s="161"/>
+      <c r="D31" s="165"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="163"/>
-      <c r="B32" s="162"/>
+      <c r="A32" s="177"/>
+      <c r="B32" s="175"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -6053,8 +6053,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="163"/>
-      <c r="B33" s="162"/>
+      <c r="A33" s="177"/>
+      <c r="B33" s="175"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -6063,8 +6063,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="163"/>
-      <c r="B34" s="162"/>
+      <c r="A34" s="177"/>
+      <c r="B34" s="175"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -6073,8 +6073,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="163"/>
-      <c r="B35" s="162"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="175"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -6083,8 +6083,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="163"/>
-      <c r="B36" s="162"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="175"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -6093,26 +6093,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="163"/>
-      <c r="B37" s="162"/>
-      <c r="C37" s="176" t="s">
+      <c r="A37" s="177"/>
+      <c r="B37" s="175"/>
+      <c r="C37" s="166" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="178" t="s">
+      <c r="D37" s="168" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="163"/>
-      <c r="B38" s="162"/>
-      <c r="C38" s="177"/>
-      <c r="D38" s="178"/>
+      <c r="A38" s="177"/>
+      <c r="B38" s="175"/>
+      <c r="C38" s="167"/>
+      <c r="D38" s="168"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="161" t="s">
+      <c r="A39" s="176" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="162" t="s">
+      <c r="B39" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6123,8 +6123,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="161"/>
-      <c r="B40" s="162"/>
+      <c r="A40" s="176"/>
+      <c r="B40" s="175"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6151,10 +6151,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="163" t="s">
+      <c r="A43" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="162" t="s">
+      <c r="B43" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6163,8 +6163,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="163"/>
-      <c r="B44" s="162"/>
+      <c r="A44" s="177"/>
+      <c r="B44" s="175"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6173,10 +6173,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="169" t="s">
+      <c r="A45" s="172" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="162" t="s">
+      <c r="B45" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6185,8 +6185,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="170"/>
-      <c r="B46" s="162"/>
+      <c r="A46" s="173"/>
+      <c r="B46" s="175"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6195,8 +6195,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="170"/>
-      <c r="B47" s="162"/>
+      <c r="A47" s="173"/>
+      <c r="B47" s="175"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6205,8 +6205,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="171"/>
-      <c r="B48" s="162"/>
+      <c r="A48" s="174"/>
+      <c r="B48" s="175"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -6215,10 +6215,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="166" t="s">
+      <c r="A49" s="170" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="166" t="s">
+      <c r="B49" s="170" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10322,8 +10322,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="166"/>
-      <c r="B50" s="166"/>
+      <c r="A50" s="170"/>
+      <c r="B50" s="170"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14427,8 +14427,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="166"/>
-      <c r="B51" s="166"/>
+      <c r="A51" s="170"/>
+      <c r="B51" s="170"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18532,8 +18532,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="166"/>
-      <c r="B52" s="166"/>
+      <c r="A52" s="170"/>
+      <c r="B52" s="170"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22637,12 +22637,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="166"/>
-      <c r="B53" s="166"/>
-      <c r="C53" s="174" t="s">
+      <c r="A53" s="170"/>
+      <c r="B53" s="170"/>
+      <c r="C53" s="164" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="175" t="s">
+      <c r="D53" s="165" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26742,10 +26742,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="166"/>
-      <c r="B54" s="166"/>
-      <c r="C54" s="174"/>
-      <c r="D54" s="175"/>
+      <c r="A54" s="170"/>
+      <c r="B54" s="170"/>
+      <c r="C54" s="164"/>
+      <c r="D54" s="165"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30863,10 +30863,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="167" t="s">
+      <c r="A57" s="169" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="166" t="s">
+      <c r="B57" s="170" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30877,8 +30877,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="167"/>
-      <c r="B58" s="166"/>
+      <c r="A58" s="169"/>
+      <c r="B58" s="170"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30887,8 +30887,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="167"/>
-      <c r="B59" s="166"/>
+      <c r="A59" s="169"/>
+      <c r="B59" s="170"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30897,8 +30897,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="167"/>
-      <c r="B60" s="166"/>
+      <c r="A60" s="169"/>
+      <c r="B60" s="170"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30907,8 +30907,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="167"/>
-      <c r="B61" s="166"/>
+      <c r="A61" s="169"/>
+      <c r="B61" s="170"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30917,8 +30917,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="167"/>
-      <c r="B62" s="166"/>
+      <c r="A62" s="169"/>
+      <c r="B62" s="170"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30927,8 +30927,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="167"/>
-      <c r="B63" s="166"/>
+      <c r="A63" s="169"/>
+      <c r="B63" s="170"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30937,16 +30937,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="167"/>
-      <c r="B64" s="166"/>
+      <c r="A64" s="169"/>
+      <c r="B64" s="170"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="167"/>
-      <c r="B65" s="166"/>
+      <c r="A65" s="169"/>
+      <c r="B65" s="170"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30955,16 +30955,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="167"/>
-      <c r="B66" s="166"/>
+      <c r="A66" s="169"/>
+      <c r="B66" s="170"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="167"/>
-      <c r="B67" s="166"/>
+      <c r="A67" s="169"/>
+      <c r="B67" s="170"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30973,8 +30973,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="167"/>
-      <c r="B68" s="166"/>
+      <c r="A68" s="169"/>
+      <c r="B68" s="170"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30983,8 +30983,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="167"/>
-      <c r="B69" s="166"/>
+      <c r="A69" s="169"/>
+      <c r="B69" s="170"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30993,8 +30993,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="167"/>
-      <c r="B70" s="166"/>
+      <c r="A70" s="169"/>
+      <c r="B70" s="170"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -31003,8 +31003,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="167"/>
-      <c r="B71" s="166"/>
+      <c r="A71" s="169"/>
+      <c r="B71" s="170"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -31013,8 +31013,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="167"/>
-      <c r="B72" s="166"/>
+      <c r="A72" s="169"/>
+      <c r="B72" s="170"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -31023,16 +31023,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="167"/>
-      <c r="B73" s="166"/>
+      <c r="A73" s="169"/>
+      <c r="B73" s="170"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="167"/>
-      <c r="B74" s="166"/>
+      <c r="A74" s="169"/>
+      <c r="B74" s="170"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -31041,18 +31041,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="167"/>
-      <c r="B75" s="166"/>
-      <c r="C75" s="173"/>
-      <c r="D75" s="168" t="s">
+      <c r="A75" s="169"/>
+      <c r="B75" s="170"/>
+      <c r="C75" s="163"/>
+      <c r="D75" s="171" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="167"/>
-      <c r="B76" s="166"/>
-      <c r="C76" s="173"/>
-      <c r="D76" s="168"/>
+      <c r="A76" s="169"/>
+      <c r="B76" s="170"/>
+      <c r="C76" s="163"/>
+      <c r="D76" s="171"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -31076,8 +31076,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -31086,29 +31086,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -31123,6 +31107,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -31176,10 +31176,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="175" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31190,133 +31190,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="161"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="188" t="s">
+      <c r="A5" s="176"/>
+      <c r="B5" s="175"/>
+      <c r="C5" s="186" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="187" t="s">
+      <c r="D5" s="185" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="161"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="188"/>
-      <c r="D6" s="187"/>
+      <c r="A6" s="176"/>
+      <c r="B6" s="175"/>
+      <c r="C6" s="186"/>
+      <c r="D6" s="185"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="161"/>
-      <c r="B7" s="162"/>
+      <c r="A7" s="176"/>
+      <c r="B7" s="175"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="161"/>
-      <c r="B8" s="162"/>
+      <c r="A8" s="176"/>
+      <c r="B8" s="175"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="161"/>
-      <c r="B9" s="162"/>
+      <c r="A9" s="176"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="178" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="162" t="s">
+      <c r="B10" s="175" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="186"/>
-      <c r="D10" s="187" t="s">
+      <c r="C10" s="188"/>
+      <c r="D10" s="185" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="164"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="186"/>
-      <c r="D11" s="187"/>
+      <c r="A11" s="178"/>
+      <c r="B11" s="175"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="185"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="164"/>
-      <c r="B12" s="162"/>
-      <c r="C12" s="186"/>
-      <c r="D12" s="187"/>
+      <c r="A12" s="178"/>
+      <c r="B12" s="175"/>
+      <c r="C12" s="188"/>
+      <c r="D12" s="185"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="165" t="s">
+      <c r="A13" s="161" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="170" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="189"/>
-      <c r="D13" s="187" t="s">
+      <c r="C13" s="187"/>
+      <c r="D13" s="185" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="165"/>
-      <c r="B14" s="166"/>
-      <c r="C14" s="189"/>
-      <c r="D14" s="187"/>
+      <c r="A14" s="161"/>
+      <c r="B14" s="170"/>
+      <c r="C14" s="187"/>
+      <c r="D14" s="185"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="165"/>
-      <c r="B15" s="166"/>
-      <c r="C15" s="189"/>
+      <c r="A15" s="161"/>
+      <c r="B15" s="170"/>
+      <c r="C15" s="187"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="165"/>
-      <c r="B16" s="166"/>
-      <c r="C16" s="189"/>
+      <c r="A16" s="161"/>
+      <c r="B16" s="170"/>
+      <c r="C16" s="187"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="165"/>
-      <c r="B17" s="166"/>
-      <c r="C17" s="189"/>
+      <c r="A17" s="161"/>
+      <c r="B17" s="170"/>
+      <c r="C17" s="187"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="165"/>
-      <c r="B18" s="166"/>
-      <c r="C18" s="189"/>
+      <c r="A18" s="161"/>
+      <c r="B18" s="170"/>
+      <c r="C18" s="187"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="165"/>
-      <c r="B19" s="166"/>
-      <c r="C19" s="189"/>
+      <c r="A19" s="161"/>
+      <c r="B19" s="170"/>
+      <c r="C19" s="187"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="165"/>
-      <c r="B20" s="166"/>
-      <c r="C20" s="189"/>
+      <c r="A20" s="161"/>
+      <c r="B20" s="170"/>
+      <c r="C20" s="187"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="165"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="189"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="170"/>
+      <c r="C21" s="187"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="165"/>
-      <c r="B22" s="166"/>
-      <c r="C22" s="189"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="170"/>
+      <c r="C22" s="187"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="165"/>
-      <c r="B23" s="166"/>
-      <c r="C23" s="189"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="170"/>
+      <c r="C23" s="187"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31414,10 +31414,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="190" t="s">
+      <c r="A32" s="179" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="193" t="s">
+      <c r="B32" s="182" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31428,26 +31428,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="191"/>
-      <c r="B33" s="194"/>
+      <c r="A33" s="180"/>
+      <c r="B33" s="183"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="191"/>
-      <c r="B34" s="194"/>
+      <c r="A34" s="180"/>
+      <c r="B34" s="183"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="191"/>
-      <c r="B35" s="194"/>
+      <c r="A35" s="180"/>
+      <c r="B35" s="183"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="192"/>
-      <c r="B36" s="195"/>
+      <c r="A36" s="181"/>
+      <c r="B36" s="184"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31476,10 +31476,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="163" t="s">
+      <c r="A39" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="162" t="s">
+      <c r="B39" s="175" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31490,8 +31490,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="163"/>
-      <c r="B40" s="162"/>
+      <c r="A40" s="177"/>
+      <c r="B40" s="175"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31500,84 +31500,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="161" t="s">
+      <c r="A41" s="176" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="162" t="s">
+      <c r="B41" s="175" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="186" t="s">
+      <c r="C41" s="188" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="165" t="s">
+      <c r="D41" s="161" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="161"/>
-      <c r="B42" s="162"/>
-      <c r="C42" s="186"/>
-      <c r="D42" s="165"/>
+      <c r="A42" s="176"/>
+      <c r="B42" s="175"/>
+      <c r="C42" s="188"/>
+      <c r="D42" s="161"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="161"/>
-      <c r="B43" s="162"/>
-      <c r="C43" s="186" t="s">
+      <c r="A43" s="176"/>
+      <c r="B43" s="175"/>
+      <c r="C43" s="188" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="168" t="s">
+      <c r="D43" s="171" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="161"/>
-      <c r="B44" s="162"/>
-      <c r="C44" s="186"/>
-      <c r="D44" s="168"/>
+      <c r="A44" s="176"/>
+      <c r="B44" s="175"/>
+      <c r="C44" s="188"/>
+      <c r="D44" s="171"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="167" t="s">
+      <c r="A45" s="169" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="166" t="s">
+      <c r="B45" s="170" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="182"/>
+      <c r="C45" s="192"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="167"/>
-      <c r="B46" s="166"/>
-      <c r="C46" s="183"/>
-      <c r="D46" s="179" t="s">
+      <c r="A46" s="169"/>
+      <c r="B46" s="170"/>
+      <c r="C46" s="193"/>
+      <c r="D46" s="189" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="167"/>
-      <c r="B47" s="166"/>
-      <c r="C47" s="183"/>
-      <c r="D47" s="180"/>
+      <c r="A47" s="169"/>
+      <c r="B47" s="170"/>
+      <c r="C47" s="193"/>
+      <c r="D47" s="190"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="167"/>
-      <c r="B48" s="166"/>
-      <c r="C48" s="184"/>
-      <c r="D48" s="180"/>
+      <c r="A48" s="169"/>
+      <c r="B48" s="170"/>
+      <c r="C48" s="194"/>
+      <c r="D48" s="190"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="167"/>
-      <c r="B49" s="166"/>
-      <c r="C49" s="174"/>
-      <c r="D49" s="180"/>
+      <c r="A49" s="169"/>
+      <c r="B49" s="170"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="190"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="167"/>
-      <c r="B50" s="166"/>
-      <c r="C50" s="174"/>
-      <c r="D50" s="181"/>
+      <c r="A50" s="169"/>
+      <c r="B50" s="170"/>
+      <c r="C50" s="164"/>
+      <c r="D50" s="191"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31600,10 +31600,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="166" t="s">
+      <c r="A53" s="170" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="166" t="s">
+      <c r="B53" s="170" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31614,8 +31614,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="166"/>
-      <c r="B54" s="166"/>
+      <c r="A54" s="170"/>
+      <c r="B54" s="170"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31624,8 +31624,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="166"/>
-      <c r="B55" s="166"/>
+      <c r="A55" s="170"/>
+      <c r="B55" s="170"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31634,9 +31634,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="166"/>
-      <c r="B56" s="166"/>
-      <c r="C56" s="185" t="s">
+      <c r="A56" s="170"/>
+      <c r="B56" s="170"/>
+      <c r="C56" s="195" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31644,16 +31644,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="166"/>
-      <c r="B57" s="166"/>
-      <c r="C57" s="185"/>
+      <c r="A57" s="170"/>
+      <c r="B57" s="170"/>
+      <c r="C57" s="195"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="166"/>
-      <c r="B58" s="166"/>
+      <c r="A58" s="170"/>
+      <c r="B58" s="170"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31662,8 +31662,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="166"/>
-      <c r="B59" s="166"/>
+      <c r="A59" s="170"/>
+      <c r="B59" s="170"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31672,9 +31672,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="166"/>
-      <c r="B60" s="166"/>
-      <c r="C60" s="185" t="s">
+      <c r="A60" s="170"/>
+      <c r="B60" s="170"/>
+      <c r="C60" s="195" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31682,25 +31682,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="166"/>
-      <c r="B61" s="166"/>
-      <c r="C61" s="185"/>
+      <c r="A61" s="170"/>
+      <c r="B61" s="170"/>
+      <c r="C61" s="195"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="166"/>
-      <c r="B62" s="166"/>
-      <c r="C62" s="185"/>
+      <c r="A62" s="170"/>
+      <c r="B62" s="170"/>
+      <c r="C62" s="195"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="166"/>
-      <c r="B63" s="166"/>
-      <c r="C63" s="186" t="s">
+      <c r="A63" s="170"/>
+      <c r="B63" s="170"/>
+      <c r="C63" s="188" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31708,30 +31708,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="166"/>
-      <c r="B64" s="166"/>
-      <c r="C64" s="186"/>
-      <c r="D64" s="168" t="s">
+      <c r="A64" s="170"/>
+      <c r="B64" s="170"/>
+      <c r="C64" s="188"/>
+      <c r="D64" s="171" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="166"/>
-      <c r="B65" s="166"/>
-      <c r="C65" s="186"/>
-      <c r="D65" s="168"/>
+      <c r="A65" s="170"/>
+      <c r="B65" s="170"/>
+      <c r="C65" s="188"/>
+      <c r="D65" s="171"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="166"/>
-      <c r="B66" s="166"/>
-      <c r="C66" s="186"/>
-      <c r="D66" s="168"/>
+      <c r="A66" s="170"/>
+      <c r="B66" s="170"/>
+      <c r="C66" s="188"/>
+      <c r="D66" s="171"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="166"/>
-      <c r="B67" s="166"/>
-      <c r="C67" s="186"/>
-      <c r="D67" s="168"/>
+      <c r="A67" s="170"/>
+      <c r="B67" s="170"/>
+      <c r="C67" s="188"/>
+      <c r="D67" s="171"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31787,23 +31787,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31820,6 +31803,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31831,7 +31831,7 @@
   <dimension ref="A1:D223"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A31"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31868,7 +31868,7 @@
       <c r="A3" s="198" t="s">
         <v>432</v>
       </c>
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="218" t="s">
         <v>433</v>
       </c>
       <c r="C3" s="101" t="s">
@@ -31879,8 +31879,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="199"/>
-      <c r="B4" s="197"/>
+      <c r="A4" s="200"/>
+      <c r="B4" s="220"/>
       <c r="C4" s="100" t="s">
         <v>436</v>
       </c>
@@ -31892,7 +31892,7 @@
       <c r="A5" s="198" t="s">
         <v>438</v>
       </c>
-      <c r="B5" s="202" t="s">
+      <c r="B5" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C5" s="100"/>
@@ -31901,31 +31901,31 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="223"/>
-      <c r="B6" s="210"/>
+      <c r="A6" s="199"/>
+      <c r="B6" s="202"/>
       <c r="C6" s="100"/>
       <c r="D6" s="58" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="223"/>
-      <c r="B7" s="210"/>
+      <c r="A7" s="199"/>
+      <c r="B7" s="202"/>
       <c r="C7" s="100"/>
       <c r="D7" s="140" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="223"/>
-      <c r="B8" s="210"/>
+      <c r="A8" s="199"/>
+      <c r="B8" s="202"/>
       <c r="C8" s="100"/>
       <c r="D8" s="140" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="199"/>
+      <c r="A9" s="200"/>
       <c r="B9" s="203"/>
       <c r="C9" s="100" t="s">
         <v>498</v>
@@ -31943,10 +31943,10 @@
       <c r="D10" s="104"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="211" t="s">
+      <c r="A11" s="213" t="s">
         <v>247</v>
       </c>
-      <c r="B11" s="202" t="s">
+      <c r="B11" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C11" s="128" t="s">
@@ -31957,7 +31957,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="213"/>
+      <c r="A12" s="215"/>
       <c r="B12" s="203"/>
       <c r="C12" s="128" t="s">
         <v>474</v>
@@ -31993,10 +31993,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="196" t="s">
+      <c r="A15" s="218" t="s">
         <v>279</v>
       </c>
-      <c r="B15" s="202" t="s">
+      <c r="B15" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C15" s="95" t="s">
@@ -32007,8 +32007,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="216"/>
-      <c r="B16" s="210"/>
+      <c r="A16" s="219"/>
+      <c r="B16" s="202"/>
       <c r="C16" s="106" t="s">
         <v>299</v>
       </c>
@@ -32017,8 +32017,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="216"/>
-      <c r="B17" s="210"/>
+      <c r="A17" s="219"/>
+      <c r="B17" s="202"/>
       <c r="C17" s="128" t="s">
         <v>280</v>
       </c>
@@ -32027,8 +32027,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="216"/>
-      <c r="B18" s="210"/>
+      <c r="A18" s="219"/>
+      <c r="B18" s="202"/>
       <c r="C18" s="128" t="s">
         <v>21</v>
       </c>
@@ -32037,8 +32037,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="216"/>
-      <c r="B19" s="210"/>
+      <c r="A19" s="219"/>
+      <c r="B19" s="202"/>
       <c r="C19" s="100" t="s">
         <v>434</v>
       </c>
@@ -32047,8 +32047,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="216"/>
-      <c r="B20" s="210"/>
+      <c r="A20" s="219"/>
+      <c r="B20" s="202"/>
       <c r="C20" s="100" t="s">
         <v>444</v>
       </c>
@@ -32057,8 +32057,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="216"/>
-      <c r="B21" s="210"/>
+      <c r="A21" s="219"/>
+      <c r="B21" s="202"/>
       <c r="C21" s="100" t="s">
         <v>446</v>
       </c>
@@ -32067,8 +32067,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="216"/>
-      <c r="B22" s="210"/>
+      <c r="A22" s="219"/>
+      <c r="B22" s="202"/>
       <c r="C22" s="100" t="s">
         <v>434</v>
       </c>
@@ -32077,7 +32077,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="197"/>
+      <c r="A23" s="220"/>
       <c r="B23" s="203"/>
       <c r="C23" s="142" t="s">
         <v>453</v>
@@ -32090,7 +32090,7 @@
       <c r="A24" s="198" t="s">
         <v>452</v>
       </c>
-      <c r="B24" s="202" t="s">
+      <c r="B24" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C24" s="100" t="s">
@@ -32101,8 +32101,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="223"/>
-      <c r="B25" s="210"/>
+      <c r="A25" s="199"/>
+      <c r="B25" s="202"/>
       <c r="C25" s="100" t="s">
         <v>453</v>
       </c>
@@ -32111,8 +32111,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="223"/>
-      <c r="B26" s="210"/>
+      <c r="A26" s="199"/>
+      <c r="B26" s="202"/>
       <c r="C26" s="100">
         <v>3.3</v>
       </c>
@@ -32121,8 +32121,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="223"/>
-      <c r="B27" s="210"/>
+      <c r="A27" s="199"/>
+      <c r="B27" s="202"/>
       <c r="C27" s="130">
         <v>3</v>
       </c>
@@ -32131,7 +32131,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="199"/>
+      <c r="A28" s="200"/>
       <c r="B28" s="203"/>
       <c r="C28" s="130">
         <v>3.5</v>
@@ -32156,7 +32156,7 @@
       <c r="A30" s="198" t="s">
         <v>501</v>
       </c>
-      <c r="B30" s="202" t="s">
+      <c r="B30" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C30" s="100"/>
@@ -32165,13 +32165,13 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="199"/>
+      <c r="A31" s="200"/>
       <c r="B31" s="203"/>
       <c r="C31" s="100" t="s">
+        <v>507</v>
+      </c>
+      <c r="D31" t="s">
         <v>506</v>
-      </c>
-      <c r="D31" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -32195,10 +32195,10 @@
       <c r="D33" s="104"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="204" t="s">
+      <c r="A34" s="223" t="s">
         <v>336</v>
       </c>
-      <c r="B34" s="205" t="s">
+      <c r="B34" s="224" t="s">
         <v>439</v>
       </c>
       <c r="C34" s="100" t="s">
@@ -32209,8 +32209,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="204"/>
-      <c r="B35" s="205"/>
+      <c r="A35" s="223"/>
+      <c r="B35" s="224"/>
       <c r="C35" s="100" t="s">
         <v>341</v>
       </c>
@@ -32219,8 +32219,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="204"/>
-      <c r="B36" s="205"/>
+      <c r="A36" s="223"/>
+      <c r="B36" s="224"/>
       <c r="C36" s="100" t="s">
         <v>337</v>
       </c>
@@ -32237,10 +32237,10 @@
       <c r="D37" s="104"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="218" t="s">
+      <c r="A38" s="216" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="206" t="s">
+      <c r="B38" s="217" t="s">
         <v>439</v>
       </c>
       <c r="C38" s="106"/>
@@ -32249,8 +32249,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="218"/>
-      <c r="B39" s="206"/>
+      <c r="A39" s="216"/>
+      <c r="B39" s="217"/>
       <c r="C39" s="136" t="s">
         <v>234</v>
       </c>
@@ -32259,8 +32259,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="218"/>
-      <c r="B40" s="206"/>
+      <c r="A40" s="216"/>
+      <c r="B40" s="217"/>
       <c r="C40" s="139" t="s">
         <v>484</v>
       </c>
@@ -32269,8 +32269,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="218"/>
-      <c r="B41" s="206"/>
+      <c r="A41" s="216"/>
+      <c r="B41" s="217"/>
       <c r="C41" s="141" t="s">
         <v>484</v>
       </c>
@@ -32279,8 +32279,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="218"/>
-      <c r="B42" s="206"/>
+      <c r="A42" s="216"/>
+      <c r="B42" s="217"/>
       <c r="C42" s="139" t="s">
         <v>498</v>
       </c>
@@ -32289,10 +32289,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="211" t="s">
+      <c r="A43" s="213" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="202" t="s">
+      <c r="B43" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C43" s="107" t="s">
@@ -32303,8 +32303,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="212"/>
-      <c r="B44" s="210"/>
+      <c r="A44" s="214"/>
+      <c r="B44" s="202"/>
       <c r="C44" s="136" t="s">
         <v>463</v>
       </c>
@@ -32313,7 +32313,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="213"/>
+      <c r="A45" s="215"/>
       <c r="B45" s="203"/>
       <c r="C45" s="137" t="s">
         <v>481</v>
@@ -32363,10 +32363,10 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="218" t="s">
+      <c r="A49" s="216" t="s">
         <v>269</v>
       </c>
-      <c r="B49" s="206" t="s">
+      <c r="B49" s="217" t="s">
         <v>439</v>
       </c>
       <c r="C49" s="106"/>
@@ -32375,16 +32375,16 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="218"/>
-      <c r="B50" s="206"/>
+      <c r="A50" s="216"/>
+      <c r="B50" s="217"/>
       <c r="C50" s="106"/>
       <c r="D50" s="106" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="218"/>
-      <c r="B51" s="206"/>
+      <c r="A51" s="216"/>
+      <c r="B51" s="217"/>
       <c r="C51" s="111" t="s">
         <v>319</v>
       </c>
@@ -32393,8 +32393,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="218"/>
-      <c r="B52" s="206"/>
+      <c r="A52" s="216"/>
+      <c r="B52" s="217"/>
       <c r="C52" s="112" t="s">
         <v>398</v>
       </c>
@@ -32415,10 +32415,10 @@
       <c r="D53" s="106"/>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="207" t="s">
+      <c r="A54" s="225" t="s">
         <v>165</v>
       </c>
-      <c r="B54" s="202" t="s">
+      <c r="B54" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C54" s="106"/>
@@ -32427,8 +32427,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="208"/>
-      <c r="B55" s="210"/>
+      <c r="A55" s="226"/>
+      <c r="B55" s="202"/>
       <c r="C55" s="112" t="s">
         <v>355</v>
       </c>
@@ -32437,8 +32437,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="208"/>
-      <c r="B56" s="210"/>
+      <c r="A56" s="226"/>
+      <c r="B56" s="202"/>
       <c r="C56" s="112" t="s">
         <v>353</v>
       </c>
@@ -32447,8 +32447,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="208"/>
-      <c r="B57" s="210"/>
+      <c r="A57" s="226"/>
+      <c r="B57" s="202"/>
       <c r="C57" s="115" t="s">
         <v>361</v>
       </c>
@@ -32457,8 +32457,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="208"/>
-      <c r="B58" s="210"/>
+      <c r="A58" s="226"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="112" t="s">
         <v>353</v>
       </c>
@@ -32467,8 +32467,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="208"/>
-      <c r="B59" s="210"/>
+      <c r="A59" s="226"/>
+      <c r="B59" s="202"/>
       <c r="C59" s="112" t="s">
         <v>365</v>
       </c>
@@ -32477,8 +32477,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="208"/>
-      <c r="B60" s="210"/>
+      <c r="A60" s="226"/>
+      <c r="B60" s="202"/>
       <c r="C60" s="112" t="s">
         <v>353</v>
       </c>
@@ -32487,8 +32487,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="208"/>
-      <c r="B61" s="210"/>
+      <c r="A61" s="226"/>
+      <c r="B61" s="202"/>
       <c r="C61" s="112" t="s">
         <v>464</v>
       </c>
@@ -32497,8 +32497,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="208"/>
-      <c r="B62" s="210"/>
+      <c r="A62" s="226"/>
+      <c r="B62" s="202"/>
       <c r="C62" s="133" t="s">
         <v>466</v>
       </c>
@@ -32507,8 +32507,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="208"/>
-      <c r="B63" s="210"/>
+      <c r="A63" s="226"/>
+      <c r="B63" s="202"/>
       <c r="C63" s="133" t="s">
         <v>353</v>
       </c>
@@ -32517,8 +32517,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="208"/>
-      <c r="B64" s="210"/>
+      <c r="A64" s="226"/>
+      <c r="B64" s="202"/>
       <c r="C64" s="138" t="s">
         <v>466</v>
       </c>
@@ -32527,8 +32527,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="208"/>
-      <c r="B65" s="210"/>
+      <c r="A65" s="226"/>
+      <c r="B65" s="202"/>
       <c r="C65" s="112" t="s">
         <v>353</v>
       </c>
@@ -32537,7 +32537,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="209"/>
+      <c r="A66" s="227"/>
       <c r="B66" s="203"/>
       <c r="C66" s="112" t="s">
         <v>498</v>
@@ -32587,10 +32587,10 @@
       <c r="D69" s="113"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="219" t="s">
+      <c r="A70" s="204" t="s">
         <v>363</v>
       </c>
-      <c r="B70" s="202" t="s">
+      <c r="B70" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C70" s="112" t="s">
@@ -32599,7 +32599,7 @@
       <c r="D70" s="113"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="224"/>
+      <c r="A71" s="205"/>
       <c r="B71" s="203"/>
       <c r="C71" s="112" t="s">
         <v>398</v>
@@ -32617,10 +32617,10 @@
       <c r="D72" s="103"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="219" t="s">
+      <c r="A73" s="204" t="s">
         <v>236</v>
       </c>
-      <c r="B73" s="202" t="s">
+      <c r="B73" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C73" s="106"/>
@@ -32629,24 +32629,24 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="220"/>
-      <c r="B74" s="210"/>
+      <c r="A74" s="206"/>
+      <c r="B74" s="202"/>
       <c r="C74" s="106"/>
       <c r="D74" s="106" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="220"/>
-      <c r="B75" s="210"/>
+      <c r="A75" s="206"/>
+      <c r="B75" s="202"/>
       <c r="C75" s="106"/>
       <c r="D75" s="106" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="220"/>
-      <c r="B76" s="210"/>
+      <c r="A76" s="206"/>
+      <c r="B76" s="202"/>
       <c r="C76" s="106" t="s">
         <v>294</v>
       </c>
@@ -32655,8 +32655,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="220"/>
-      <c r="B77" s="210"/>
+      <c r="A77" s="206"/>
+      <c r="B77" s="202"/>
       <c r="C77" s="106" t="s">
         <v>322</v>
       </c>
@@ -32665,8 +32665,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="220"/>
-      <c r="B78" s="210"/>
+      <c r="A78" s="206"/>
+      <c r="B78" s="202"/>
       <c r="C78" s="106" t="s">
         <v>367</v>
       </c>
@@ -32675,8 +32675,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="220"/>
-      <c r="B79" s="210"/>
+      <c r="A79" s="206"/>
+      <c r="B79" s="202"/>
       <c r="C79" s="119" t="s">
         <v>468</v>
       </c>
@@ -32685,8 +32685,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="220"/>
-      <c r="B80" s="210"/>
+      <c r="A80" s="206"/>
+      <c r="B80" s="202"/>
       <c r="C80" s="58" t="s">
         <v>37</v>
       </c>
@@ -32695,8 +32695,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="220"/>
-      <c r="B81" s="210"/>
+      <c r="A81" s="206"/>
+      <c r="B81" s="202"/>
       <c r="C81" s="130" t="s">
         <v>353</v>
       </c>
@@ -32705,8 +32705,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="220"/>
-      <c r="B82" s="210"/>
+      <c r="A82" s="206"/>
+      <c r="B82" s="202"/>
       <c r="C82" s="130" t="s">
         <v>466</v>
       </c>
@@ -32715,8 +32715,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="220"/>
-      <c r="B83" s="210"/>
+      <c r="A83" s="206"/>
+      <c r="B83" s="202"/>
       <c r="C83" s="130" t="s">
         <v>367</v>
       </c>
@@ -32725,8 +32725,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="220"/>
-      <c r="B84" s="210"/>
+      <c r="A84" s="206"/>
+      <c r="B84" s="202"/>
       <c r="C84" s="130" t="s">
         <v>353</v>
       </c>
@@ -32735,7 +32735,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="224"/>
+      <c r="A85" s="205"/>
       <c r="B85" s="203"/>
       <c r="C85" s="130" t="s">
         <v>498</v>
@@ -32745,10 +32745,10 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="214" t="s">
+      <c r="A86" s="207" t="s">
         <v>27</v>
       </c>
-      <c r="B86" s="202" t="s">
+      <c r="B86" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C86" s="106" t="s">
@@ -32759,16 +32759,16 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="215"/>
-      <c r="B87" s="210"/>
+      <c r="A87" s="208"/>
+      <c r="B87" s="202"/>
       <c r="C87" s="106"/>
       <c r="D87" s="106" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="215"/>
-      <c r="B88" s="210"/>
+      <c r="A88" s="208"/>
+      <c r="B88" s="202"/>
       <c r="C88" s="117" t="s">
         <v>323</v>
       </c>
@@ -32777,8 +32777,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="215"/>
-      <c r="B89" s="210"/>
+      <c r="A89" s="208"/>
+      <c r="B89" s="202"/>
       <c r="C89" s="117" t="s">
         <v>353</v>
       </c>
@@ -32787,8 +32787,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="215"/>
-      <c r="B90" s="210"/>
+      <c r="A90" s="208"/>
+      <c r="B90" s="202"/>
       <c r="C90" s="117" t="s">
         <v>361</v>
       </c>
@@ -32797,8 +32797,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="215"/>
-      <c r="B91" s="210"/>
+      <c r="A91" s="208"/>
+      <c r="B91" s="202"/>
       <c r="C91" s="117" t="s">
         <v>365</v>
       </c>
@@ -32807,8 +32807,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="215"/>
-      <c r="B92" s="210"/>
+      <c r="A92" s="208"/>
+      <c r="B92" s="202"/>
       <c r="C92" s="117" t="s">
         <v>375</v>
       </c>
@@ -32817,8 +32817,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="215"/>
-      <c r="B93" s="210"/>
+      <c r="A93" s="208"/>
+      <c r="B93" s="202"/>
       <c r="C93" s="109" t="s">
         <v>353</v>
       </c>
@@ -32827,8 +32827,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="215"/>
-      <c r="B94" s="210"/>
+      <c r="A94" s="208"/>
+      <c r="B94" s="202"/>
       <c r="C94" s="109" t="s">
         <v>464</v>
       </c>
@@ -32837,8 +32837,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="215"/>
-      <c r="B95" s="210"/>
+      <c r="A95" s="208"/>
+      <c r="B95" s="202"/>
       <c r="C95" s="130" t="s">
         <v>466</v>
       </c>
@@ -32847,8 +32847,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="215"/>
-      <c r="B96" s="210"/>
+      <c r="A96" s="208"/>
+      <c r="B96" s="202"/>
       <c r="C96" s="130" t="s">
         <v>353</v>
       </c>
@@ -32857,8 +32857,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="215"/>
-      <c r="B97" s="210"/>
+      <c r="A97" s="208"/>
+      <c r="B97" s="202"/>
       <c r="C97" s="130" t="s">
         <v>466</v>
       </c>
@@ -32867,8 +32867,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="215"/>
-      <c r="B98" s="210"/>
+      <c r="A98" s="208"/>
+      <c r="B98" s="202"/>
       <c r="C98" s="130" t="s">
         <v>367</v>
       </c>
@@ -32877,8 +32877,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="215"/>
-      <c r="B99" s="210"/>
+      <c r="A99" s="208"/>
+      <c r="B99" s="202"/>
       <c r="C99" s="130" t="s">
         <v>353</v>
       </c>
@@ -32887,7 +32887,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="217"/>
+      <c r="A100" s="209"/>
       <c r="B100" s="203"/>
       <c r="C100" s="130" t="s">
         <v>498</v>
@@ -32897,13 +32897,13 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="211" t="s">
+      <c r="A101" s="213" t="s">
         <v>222</v>
       </c>
-      <c r="B101" s="202" t="s">
+      <c r="B101" s="201" t="s">
         <v>439</v>
       </c>
-      <c r="C101" s="225" t="s">
+      <c r="C101" s="210" t="s">
         <v>238</v>
       </c>
       <c r="D101" s="96" t="s">
@@ -32911,17 +32911,17 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="212"/>
-      <c r="B102" s="210"/>
-      <c r="C102" s="226"/>
+      <c r="A102" s="214"/>
+      <c r="B102" s="202"/>
+      <c r="C102" s="211"/>
       <c r="D102" s="113" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="212"/>
-      <c r="B103" s="210"/>
-      <c r="C103" s="227" t="s">
+      <c r="A103" s="214"/>
+      <c r="B103" s="202"/>
+      <c r="C103" s="212" t="s">
         <v>239</v>
       </c>
       <c r="D103" s="106" t="s">
@@ -32929,16 +32929,16 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="212"/>
-      <c r="B104" s="210"/>
-      <c r="C104" s="227"/>
+      <c r="A104" s="214"/>
+      <c r="B104" s="202"/>
+      <c r="C104" s="212"/>
       <c r="D104" s="119" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="212"/>
-      <c r="B105" s="210"/>
+      <c r="A105" s="214"/>
+      <c r="B105" s="202"/>
       <c r="C105" s="112" t="s">
         <v>301</v>
       </c>
@@ -32947,8 +32947,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="212"/>
-      <c r="B106" s="210"/>
+      <c r="A106" s="214"/>
+      <c r="B106" s="202"/>
       <c r="C106" s="112">
         <v>2.1</v>
       </c>
@@ -32957,8 +32957,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="212"/>
-      <c r="B107" s="210"/>
+      <c r="A107" s="214"/>
+      <c r="B107" s="202"/>
       <c r="C107" s="112" t="s">
         <v>238</v>
       </c>
@@ -32967,8 +32967,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="212"/>
-      <c r="B108" s="210"/>
+      <c r="A108" s="214"/>
+      <c r="B108" s="202"/>
       <c r="C108" s="112" t="s">
         <v>238</v>
       </c>
@@ -32977,8 +32977,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="212"/>
-      <c r="B109" s="210"/>
+      <c r="A109" s="214"/>
+      <c r="B109" s="202"/>
       <c r="C109" s="112" t="s">
         <v>238</v>
       </c>
@@ -32987,8 +32987,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="212"/>
-      <c r="B110" s="210"/>
+      <c r="A110" s="214"/>
+      <c r="B110" s="202"/>
       <c r="C110" s="120" t="s">
         <v>372</v>
       </c>
@@ -32997,8 +32997,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="212"/>
-      <c r="B111" s="210"/>
+      <c r="A111" s="214"/>
+      <c r="B111" s="202"/>
       <c r="C111" s="112">
         <v>2.1</v>
       </c>
@@ -33007,8 +33007,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="212"/>
-      <c r="B112" s="210"/>
+      <c r="A112" s="214"/>
+      <c r="B112" s="202"/>
       <c r="C112" s="112" t="s">
         <v>238</v>
       </c>
@@ -33017,8 +33017,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="212"/>
-      <c r="B113" s="210"/>
+      <c r="A113" s="214"/>
+      <c r="B113" s="202"/>
       <c r="C113" s="112" t="s">
         <v>238</v>
       </c>
@@ -33027,8 +33027,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="212"/>
-      <c r="B114" s="210"/>
+      <c r="A114" s="214"/>
+      <c r="B114" s="202"/>
       <c r="C114" s="112">
         <v>2.1</v>
       </c>
@@ -33037,10 +33037,10 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="214" t="s">
+      <c r="A115" s="207" t="s">
         <v>290</v>
       </c>
-      <c r="B115" s="202" t="s">
+      <c r="B115" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C115" s="106" t="s">
@@ -33051,8 +33051,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A116" s="215"/>
-      <c r="B116" s="210"/>
+      <c r="A116" s="208"/>
+      <c r="B116" s="202"/>
       <c r="C116" s="119" t="s">
         <v>275</v>
       </c>
@@ -33061,7 +33061,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="217"/>
+      <c r="A117" s="209"/>
       <c r="B117" s="203"/>
       <c r="C117" s="106" t="s">
         <v>344</v>
@@ -33071,10 +33071,10 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="219" t="s">
+      <c r="A118" s="204" t="s">
         <v>364</v>
       </c>
-      <c r="B118" s="202" t="s">
+      <c r="B118" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C118" s="112" t="s">
@@ -33083,8 +33083,8 @@
       <c r="D118" s="106"/>
     </row>
     <row r="119" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="220"/>
-      <c r="B119" s="210"/>
+      <c r="A119" s="206"/>
+      <c r="B119" s="202"/>
       <c r="C119" s="112" t="s">
         <v>372</v>
       </c>
@@ -33093,8 +33093,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="220"/>
-      <c r="B120" s="210"/>
+      <c r="A120" s="206"/>
+      <c r="B120" s="202"/>
       <c r="C120" s="112">
         <v>2.1</v>
       </c>
@@ -33103,8 +33103,8 @@
       </c>
     </row>
     <row r="121" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="220"/>
-      <c r="B121" s="210"/>
+      <c r="A121" s="206"/>
+      <c r="B121" s="202"/>
       <c r="C121" s="112" t="s">
         <v>239</v>
       </c>
@@ -33113,8 +33113,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="220"/>
-      <c r="B122" s="210"/>
+      <c r="A122" s="206"/>
+      <c r="B122" s="202"/>
       <c r="C122" s="112" t="s">
         <v>238</v>
       </c>
@@ -33143,10 +33143,10 @@
       <c r="D124" s="113"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="211" t="s">
+      <c r="A125" s="213" t="s">
         <v>255</v>
       </c>
-      <c r="B125" s="202" t="s">
+      <c r="B125" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C125" s="106"/>
@@ -33155,24 +33155,24 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="212"/>
-      <c r="B126" s="210"/>
+      <c r="A126" s="214"/>
+      <c r="B126" s="202"/>
       <c r="C126" s="106"/>
       <c r="D126" s="106" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="212"/>
-      <c r="B127" s="210"/>
+      <c r="A127" s="214"/>
+      <c r="B127" s="202"/>
       <c r="C127" s="106"/>
       <c r="D127" s="113" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="212"/>
-      <c r="B128" s="210"/>
+      <c r="A128" s="214"/>
+      <c r="B128" s="202"/>
       <c r="C128" s="106" t="s">
         <v>418</v>
       </c>
@@ -33181,8 +33181,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="212"/>
-      <c r="B129" s="210"/>
+      <c r="A129" s="214"/>
+      <c r="B129" s="202"/>
       <c r="C129" s="106" t="s">
         <v>423</v>
       </c>
@@ -33191,8 +33191,8 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="212"/>
-      <c r="B130" s="210"/>
+      <c r="A130" s="214"/>
+      <c r="B130" s="202"/>
       <c r="C130" s="106" t="s">
         <v>484</v>
       </c>
@@ -33201,8 +33201,8 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="212"/>
-      <c r="B131" s="210"/>
+      <c r="A131" s="214"/>
+      <c r="B131" s="202"/>
       <c r="C131" s="106" t="s">
         <v>498</v>
       </c>
@@ -33211,10 +33211,10 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="218" t="s">
+      <c r="A132" s="216" t="s">
         <v>328</v>
       </c>
-      <c r="B132" s="206" t="s">
+      <c r="B132" s="217" t="s">
         <v>439</v>
       </c>
       <c r="C132" s="80" t="s">
@@ -33225,8 +33225,8 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="218"/>
-      <c r="B133" s="206"/>
+      <c r="A133" s="216"/>
+      <c r="B133" s="217"/>
       <c r="C133" s="106" t="s">
         <v>405</v>
       </c>
@@ -33235,42 +33235,42 @@
       </c>
     </row>
     <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="218"/>
-      <c r="B134" s="206"/>
+      <c r="A134" s="216"/>
+      <c r="B134" s="217"/>
       <c r="C134" s="122" t="s">
         <v>408</v>
       </c>
-      <c r="D134" s="221" t="s">
+      <c r="D134" s="196" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="218"/>
-      <c r="B135" s="206"/>
+      <c r="A135" s="216"/>
+      <c r="B135" s="217"/>
       <c r="C135" s="122" t="s">
         <v>409</v>
       </c>
-      <c r="D135" s="222"/>
+      <c r="D135" s="197"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="218"/>
-      <c r="B136" s="206"/>
+      <c r="A136" s="216"/>
+      <c r="B136" s="217"/>
       <c r="C136" s="122" t="s">
         <v>410</v>
       </c>
-      <c r="D136" s="222"/>
+      <c r="D136" s="197"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="218"/>
-      <c r="B137" s="206"/>
+      <c r="A137" s="216"/>
+      <c r="B137" s="217"/>
       <c r="C137" s="122" t="s">
         <v>411</v>
       </c>
-      <c r="D137" s="222"/>
+      <c r="D137" s="197"/>
     </row>
     <row r="138" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A138" s="218"/>
-      <c r="B138" s="206"/>
+      <c r="A138" s="216"/>
+      <c r="B138" s="217"/>
       <c r="C138" s="122" t="s">
         <v>470</v>
       </c>
@@ -33293,10 +33293,10 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="214" t="s">
+      <c r="A140" s="207" t="s">
         <v>32</v>
       </c>
-      <c r="B140" s="202" t="s">
+      <c r="B140" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C140" s="106" t="s">
@@ -33307,8 +33307,8 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="215"/>
-      <c r="B141" s="210"/>
+      <c r="A141" s="208"/>
+      <c r="B141" s="202"/>
       <c r="C141" s="106" t="s">
         <v>264</v>
       </c>
@@ -33317,8 +33317,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="215"/>
-      <c r="B142" s="210"/>
+      <c r="A142" s="208"/>
+      <c r="B142" s="202"/>
       <c r="C142" s="106" t="s">
         <v>263</v>
       </c>
@@ -33327,8 +33327,8 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="215"/>
-      <c r="B143" s="210"/>
+      <c r="A143" s="208"/>
+      <c r="B143" s="202"/>
       <c r="C143" s="113" t="s">
         <v>271</v>
       </c>
@@ -33337,8 +33337,8 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="215"/>
-      <c r="B144" s="210"/>
+      <c r="A144" s="208"/>
+      <c r="B144" s="202"/>
       <c r="C144" s="106" t="s">
         <v>276</v>
       </c>
@@ -33347,8 +33347,8 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="215"/>
-      <c r="B145" s="210"/>
+      <c r="A145" s="208"/>
+      <c r="B145" s="202"/>
       <c r="C145" s="106" t="s">
         <v>277</v>
       </c>
@@ -33357,8 +33357,8 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="215"/>
-      <c r="B146" s="210"/>
+      <c r="A146" s="208"/>
+      <c r="B146" s="202"/>
       <c r="C146" s="113" t="s">
         <v>282</v>
       </c>
@@ -33367,8 +33367,8 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="215"/>
-      <c r="B147" s="210"/>
+      <c r="A147" s="208"/>
+      <c r="B147" s="202"/>
       <c r="C147" s="113" t="s">
         <v>296</v>
       </c>
@@ -33377,8 +33377,8 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="215"/>
-      <c r="B148" s="210"/>
+      <c r="A148" s="208"/>
+      <c r="B148" s="202"/>
       <c r="C148" s="113" t="s">
         <v>283</v>
       </c>
@@ -33387,8 +33387,8 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="215"/>
-      <c r="B149" s="210"/>
+      <c r="A149" s="208"/>
+      <c r="B149" s="202"/>
       <c r="C149" s="123" t="s">
         <v>243</v>
       </c>
@@ -33397,8 +33397,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A150" s="215"/>
-      <c r="B150" s="210"/>
+      <c r="A150" s="208"/>
+      <c r="B150" s="202"/>
       <c r="C150" s="117" t="s">
         <v>305</v>
       </c>
@@ -33407,8 +33407,8 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="215"/>
-      <c r="B151" s="210"/>
+      <c r="A151" s="208"/>
+      <c r="B151" s="202"/>
       <c r="C151" s="106" t="s">
         <v>306</v>
       </c>
@@ -33417,8 +33417,8 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="215"/>
-      <c r="B152" s="210"/>
+      <c r="A152" s="208"/>
+      <c r="B152" s="202"/>
       <c r="C152" s="113" t="s">
         <v>307</v>
       </c>
@@ -33427,8 +33427,8 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="215"/>
-      <c r="B153" s="210"/>
+      <c r="A153" s="208"/>
+      <c r="B153" s="202"/>
       <c r="C153" s="113" t="s">
         <v>309</v>
       </c>
@@ -33437,8 +33437,8 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="215"/>
-      <c r="B154" s="210"/>
+      <c r="A154" s="208"/>
+      <c r="B154" s="202"/>
       <c r="C154" s="113" t="s">
         <v>262</v>
       </c>
@@ -33447,8 +33447,8 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="215"/>
-      <c r="B155" s="210"/>
+      <c r="A155" s="208"/>
+      <c r="B155" s="202"/>
       <c r="C155" s="106" t="s">
         <v>312</v>
       </c>
@@ -33457,8 +33457,8 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="215"/>
-      <c r="B156" s="210"/>
+      <c r="A156" s="208"/>
+      <c r="B156" s="202"/>
       <c r="C156" s="113" t="s">
         <v>277</v>
       </c>
@@ -33467,8 +33467,8 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="215"/>
-      <c r="B157" s="210"/>
+      <c r="A157" s="208"/>
+      <c r="B157" s="202"/>
       <c r="C157" s="113" t="s">
         <v>313</v>
       </c>
@@ -33477,16 +33477,16 @@
       </c>
     </row>
     <row r="158" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A158" s="215"/>
-      <c r="B158" s="210"/>
+      <c r="A158" s="208"/>
+      <c r="B158" s="202"/>
       <c r="C158" s="106"/>
       <c r="D158" s="97" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="215"/>
-      <c r="B159" s="210"/>
+      <c r="A159" s="208"/>
+      <c r="B159" s="202"/>
       <c r="C159" s="113" t="s">
         <v>316</v>
       </c>
@@ -33495,8 +33495,8 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="215"/>
-      <c r="B160" s="210"/>
+      <c r="A160" s="208"/>
+      <c r="B160" s="202"/>
       <c r="C160" s="113" t="s">
         <v>262</v>
       </c>
@@ -33505,8 +33505,8 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="215"/>
-      <c r="B161" s="210"/>
+      <c r="A161" s="208"/>
+      <c r="B161" s="202"/>
       <c r="C161" s="113" t="s">
         <v>333</v>
       </c>
@@ -33515,8 +33515,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="215"/>
-      <c r="B162" s="210"/>
+      <c r="A162" s="208"/>
+      <c r="B162" s="202"/>
       <c r="C162" s="113" t="s">
         <v>334</v>
       </c>
@@ -33525,8 +33525,8 @@
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="215"/>
-      <c r="B163" s="210"/>
+      <c r="A163" s="208"/>
+      <c r="B163" s="202"/>
       <c r="C163" s="113" t="s">
         <v>318</v>
       </c>
@@ -33535,8 +33535,8 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="215"/>
-      <c r="B164" s="210"/>
+      <c r="A164" s="208"/>
+      <c r="B164" s="202"/>
       <c r="C164" s="113" t="s">
         <v>339</v>
       </c>
@@ -33545,8 +33545,8 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="215"/>
-      <c r="B165" s="210"/>
+      <c r="A165" s="208"/>
+      <c r="B165" s="202"/>
       <c r="C165" s="113" t="s">
         <v>332</v>
       </c>
@@ -33555,8 +33555,8 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="215"/>
-      <c r="B166" s="210"/>
+      <c r="A166" s="208"/>
+      <c r="B166" s="202"/>
       <c r="C166" s="113" t="s">
         <v>347</v>
       </c>
@@ -33565,8 +33565,8 @@
       </c>
     </row>
     <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="215"/>
-      <c r="B167" s="210"/>
+      <c r="A167" s="208"/>
+      <c r="B167" s="202"/>
       <c r="C167" s="101" t="s">
         <v>350</v>
       </c>
@@ -33575,8 +33575,8 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="215"/>
-      <c r="B168" s="210"/>
+      <c r="A168" s="208"/>
+      <c r="B168" s="202"/>
       <c r="C168" s="113" t="s">
         <v>351</v>
       </c>
@@ -33585,8 +33585,8 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="215"/>
-      <c r="B169" s="210"/>
+      <c r="A169" s="208"/>
+      <c r="B169" s="202"/>
       <c r="C169" s="113" t="s">
         <v>352</v>
       </c>
@@ -33595,8 +33595,8 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="215"/>
-      <c r="B170" s="210"/>
+      <c r="A170" s="208"/>
+      <c r="B170" s="202"/>
       <c r="C170" s="113" t="s">
         <v>358</v>
       </c>
@@ -33605,8 +33605,8 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="215"/>
-      <c r="B171" s="210"/>
+      <c r="A171" s="208"/>
+      <c r="B171" s="202"/>
       <c r="C171" s="113" t="s">
         <v>360</v>
       </c>
@@ -33615,8 +33615,8 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="215"/>
-      <c r="B172" s="210"/>
+      <c r="A172" s="208"/>
+      <c r="B172" s="202"/>
       <c r="C172" s="113" t="s">
         <v>366</v>
       </c>
@@ -33625,8 +33625,8 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="215"/>
-      <c r="B173" s="210"/>
+      <c r="A173" s="208"/>
+      <c r="B173" s="202"/>
       <c r="C173" s="113" t="s">
         <v>358</v>
       </c>
@@ -33635,8 +33635,8 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="215"/>
-      <c r="B174" s="210"/>
+      <c r="A174" s="208"/>
+      <c r="B174" s="202"/>
       <c r="C174" s="118" t="s">
         <v>379</v>
       </c>
@@ -33645,8 +33645,8 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="215"/>
-      <c r="B175" s="210"/>
+      <c r="A175" s="208"/>
+      <c r="B175" s="202"/>
       <c r="C175" s="106" t="s">
         <v>383</v>
       </c>
@@ -33655,8 +33655,8 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="215"/>
-      <c r="B176" s="210"/>
+      <c r="A176" s="208"/>
+      <c r="B176" s="202"/>
       <c r="C176" s="106" t="s">
         <v>386</v>
       </c>
@@ -33665,8 +33665,8 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="215"/>
-      <c r="B177" s="210"/>
+      <c r="A177" s="208"/>
+      <c r="B177" s="202"/>
       <c r="C177" s="106" t="s">
         <v>387</v>
       </c>
@@ -33675,8 +33675,8 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="215"/>
-      <c r="B178" s="210"/>
+      <c r="A178" s="208"/>
+      <c r="B178" s="202"/>
       <c r="C178" s="106" t="s">
         <v>388</v>
       </c>
@@ -33685,8 +33685,8 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="215"/>
-      <c r="B179" s="210"/>
+      <c r="A179" s="208"/>
+      <c r="B179" s="202"/>
       <c r="C179" s="106" t="s">
         <v>389</v>
       </c>
@@ -33695,8 +33695,8 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="215"/>
-      <c r="B180" s="210"/>
+      <c r="A180" s="208"/>
+      <c r="B180" s="202"/>
       <c r="C180" s="106" t="s">
         <v>390</v>
       </c>
@@ -33705,8 +33705,8 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="215"/>
-      <c r="B181" s="210"/>
+      <c r="A181" s="208"/>
+      <c r="B181" s="202"/>
       <c r="C181" s="106" t="s">
         <v>393</v>
       </c>
@@ -33715,8 +33715,8 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="215"/>
-      <c r="B182" s="210"/>
+      <c r="A182" s="208"/>
+      <c r="B182" s="202"/>
       <c r="C182" s="106" t="s">
         <v>403</v>
       </c>
@@ -33725,8 +33725,8 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="215"/>
-      <c r="B183" s="210"/>
+      <c r="A183" s="208"/>
+      <c r="B183" s="202"/>
       <c r="C183" s="106" t="s">
         <v>404</v>
       </c>
@@ -33735,8 +33735,8 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="215"/>
-      <c r="B184" s="210"/>
+      <c r="A184" s="208"/>
+      <c r="B184" s="202"/>
       <c r="C184" s="106" t="s">
         <v>421</v>
       </c>
@@ -33745,8 +33745,8 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="215"/>
-      <c r="B185" s="210"/>
+      <c r="A185" s="208"/>
+      <c r="B185" s="202"/>
       <c r="C185" s="106" t="s">
         <v>422</v>
       </c>
@@ -33755,8 +33755,8 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="215"/>
-      <c r="B186" s="210"/>
+      <c r="A186" s="208"/>
+      <c r="B186" s="202"/>
       <c r="C186" s="106" t="s">
         <v>425</v>
       </c>
@@ -33765,8 +33765,8 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="215"/>
-      <c r="B187" s="210"/>
+      <c r="A187" s="208"/>
+      <c r="B187" s="202"/>
       <c r="C187" s="58" t="s">
         <v>471</v>
       </c>
@@ -33775,8 +33775,8 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="215"/>
-      <c r="B188" s="210"/>
+      <c r="A188" s="208"/>
+      <c r="B188" s="202"/>
       <c r="C188" s="58" t="s">
         <v>421</v>
       </c>
@@ -33785,8 +33785,8 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="215"/>
-      <c r="B189" s="210"/>
+      <c r="A189" s="208"/>
+      <c r="B189" s="202"/>
       <c r="C189" s="58" t="s">
         <v>497</v>
       </c>
@@ -33795,10 +33795,10 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="214" t="s">
+      <c r="A190" s="207" t="s">
         <v>415</v>
       </c>
-      <c r="B190" s="202" t="s">
+      <c r="B190" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C190" s="106" t="s">
@@ -33809,7 +33809,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="217"/>
+      <c r="A191" s="209"/>
       <c r="B191" s="203"/>
       <c r="C191" s="118" t="s">
         <v>491</v>
@@ -33855,10 +33855,10 @@
       <c r="D194" s="104"/>
     </row>
     <row r="195" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="211" t="s">
+      <c r="A195" s="213" t="s">
         <v>84</v>
       </c>
-      <c r="B195" s="202" t="s">
+      <c r="B195" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C195" s="106"/>
@@ -33867,8 +33867,8 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="212"/>
-      <c r="B196" s="210"/>
+      <c r="A196" s="214"/>
+      <c r="B196" s="202"/>
       <c r="C196" s="107" t="s">
         <v>245</v>
       </c>
@@ -33877,8 +33877,8 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="212"/>
-      <c r="B197" s="210"/>
+      <c r="A197" s="214"/>
+      <c r="B197" s="202"/>
       <c r="C197" s="107">
         <v>10.1</v>
       </c>
@@ -33887,8 +33887,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="212"/>
-      <c r="B198" s="210"/>
+      <c r="A198" s="214"/>
+      <c r="B198" s="202"/>
       <c r="C198" s="107">
         <v>10.199999999999999</v>
       </c>
@@ -33897,8 +33897,8 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="212"/>
-      <c r="B199" s="210"/>
+      <c r="A199" s="214"/>
+      <c r="B199" s="202"/>
       <c r="C199" s="98" t="s">
         <v>287</v>
       </c>
@@ -33907,8 +33907,8 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="212"/>
-      <c r="B200" s="210"/>
+      <c r="A200" s="214"/>
+      <c r="B200" s="202"/>
       <c r="C200" s="98" t="s">
         <v>369</v>
       </c>
@@ -33917,8 +33917,8 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="212"/>
-      <c r="B201" s="210"/>
+      <c r="A201" s="214"/>
+      <c r="B201" s="202"/>
       <c r="C201" s="98" t="s">
         <v>117</v>
       </c>
@@ -33927,8 +33927,8 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="212"/>
-      <c r="B202" s="210"/>
+      <c r="A202" s="214"/>
+      <c r="B202" s="202"/>
       <c r="C202" s="98" t="s">
         <v>416</v>
       </c>
@@ -33937,8 +33937,8 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="212"/>
-      <c r="B203" s="210"/>
+      <c r="A203" s="214"/>
+      <c r="B203" s="202"/>
       <c r="C203" s="98" t="s">
         <v>17</v>
       </c>
@@ -33947,8 +33947,8 @@
       </c>
     </row>
     <row r="204" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A204" s="212"/>
-      <c r="B204" s="210"/>
+      <c r="A204" s="214"/>
+      <c r="B204" s="202"/>
       <c r="C204" s="98" t="s">
         <v>496</v>
       </c>
@@ -33957,7 +33957,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A205" s="213"/>
+      <c r="A205" s="215"/>
       <c r="B205" s="203"/>
       <c r="C205" s="98" t="s">
         <v>496</v>
@@ -33967,10 +33967,10 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="211" t="s">
+      <c r="A206" s="213" t="s">
         <v>246</v>
       </c>
-      <c r="B206" s="202" t="s">
+      <c r="B206" s="201" t="s">
         <v>439</v>
       </c>
       <c r="C206" s="98"/>
@@ -33979,8 +33979,8 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="212"/>
-      <c r="B207" s="210"/>
+      <c r="A207" s="214"/>
+      <c r="B207" s="202"/>
       <c r="C207" s="126" t="s">
         <v>427</v>
       </c>
@@ -34011,10 +34011,10 @@
       <c r="D209" s="127"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="211" t="s">
+      <c r="A210" s="213" t="s">
         <v>58</v>
       </c>
-      <c r="B210" s="202" t="s">
+      <c r="B210" s="201" t="s">
         <v>265</v>
       </c>
       <c r="C210" s="128" t="s">
@@ -34025,8 +34025,8 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="212"/>
-      <c r="B211" s="210"/>
+      <c r="A211" s="214"/>
+      <c r="B211" s="202"/>
       <c r="C211" s="128" t="s">
         <v>259</v>
       </c>
@@ -34035,7 +34035,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="213"/>
+      <c r="A212" s="215"/>
       <c r="B212" s="203"/>
       <c r="C212" s="106"/>
       <c r="D212" s="106" t="s">
@@ -34043,10 +34043,10 @@
       </c>
     </row>
     <row r="213" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A213" s="200" t="s">
+      <c r="A213" s="221" t="s">
         <v>59</v>
       </c>
-      <c r="B213" s="202" t="s">
+      <c r="B213" s="201" t="s">
         <v>265</v>
       </c>
       <c r="C213" s="119" t="s">
@@ -34057,7 +34057,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="201"/>
+      <c r="A214" s="222"/>
       <c r="B214" s="203"/>
       <c r="C214" s="119"/>
       <c r="D214" s="106" t="s">
@@ -34065,10 +34065,10 @@
       </c>
     </row>
     <row r="215" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A215" s="200" t="s">
+      <c r="A215" s="221" t="s">
         <v>285</v>
       </c>
-      <c r="B215" s="202" t="s">
+      <c r="B215" s="201" t="s">
         <v>265</v>
       </c>
       <c r="C215" s="119"/>
@@ -34077,7 +34077,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="201"/>
+      <c r="A216" s="222"/>
       <c r="B216" s="203"/>
       <c r="C216" s="106"/>
       <c r="D216" s="106" t="s">
@@ -34085,10 +34085,10 @@
       </c>
     </row>
     <row r="217" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A217" s="200" t="s">
+      <c r="A217" s="221" t="s">
         <v>60</v>
       </c>
-      <c r="B217" s="202" t="s">
+      <c r="B217" s="201" t="s">
         <v>265</v>
       </c>
       <c r="C217" s="119" t="s">
@@ -34099,7 +34099,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="201"/>
+      <c r="A218" s="222"/>
       <c r="B218" s="203"/>
       <c r="C218" s="106"/>
       <c r="D218" s="106" t="s">
@@ -34158,6 +34158,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="B217:B218"/>
+    <mergeCell ref="A213:A214"/>
+    <mergeCell ref="B213:B214"/>
+    <mergeCell ref="A215:A216"/>
+    <mergeCell ref="B215:B216"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A54:A66"/>
+    <mergeCell ref="B54:B66"/>
+    <mergeCell ref="A210:A212"/>
+    <mergeCell ref="B210:B212"/>
+    <mergeCell ref="A206:A207"/>
+    <mergeCell ref="B206:B207"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A140:A189"/>
+    <mergeCell ref="B140:B189"/>
+    <mergeCell ref="A101:A114"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="A195:A205"/>
+    <mergeCell ref="B195:B205"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B101:B114"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B132:B138"/>
+    <mergeCell ref="A118:A122"/>
+    <mergeCell ref="B118:B122"/>
+    <mergeCell ref="A125:A131"/>
+    <mergeCell ref="B125:B131"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="D134:D137"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="B24:B28"/>
@@ -34174,47 +34215,6 @@
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="A132:A138"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="B132:B138"/>
-    <mergeCell ref="A118:A122"/>
-    <mergeCell ref="B118:B122"/>
-    <mergeCell ref="A125:A131"/>
-    <mergeCell ref="B125:B131"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A206:A207"/>
-    <mergeCell ref="B206:B207"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A140:A189"/>
-    <mergeCell ref="B140:B189"/>
-    <mergeCell ref="A101:A114"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="B15:B23"/>
-    <mergeCell ref="A195:A205"/>
-    <mergeCell ref="B195:B205"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="B101:B114"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="B217:B218"/>
-    <mergeCell ref="A213:A214"/>
-    <mergeCell ref="B213:B214"/>
-    <mergeCell ref="A215:A216"/>
-    <mergeCell ref="B215:B216"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="A54:A66"/>
-    <mergeCell ref="B54:B66"/>
-    <mergeCell ref="A210:A212"/>
-    <mergeCell ref="B210:B212"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Format Changes / paye-employers-rest-api-pit4.json changes
</commit_message>
<xml_diff>
--- a/PIT4/Schema Publication Changelog.xlsx
+++ b/PIT4/Schema Publication Changelog.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ademps03\IdeaProjects\paye-employers-documentation\src\main\resources\PIT4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ymathieu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444F1246-0151-4B76-9731-F8DB4FBBBB00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2567AE-E989-4F40-8DB0-396B725A61DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28485" windowHeight="14535" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
     <sheet name="v1.0 Milestone 1" sheetId="2" r:id="rId2"/>
     <sheet name="v1.0Milestone 2" sheetId="3" r:id="rId3"/>
     <sheet name="1.0 Release Candidate 2" sheetId="4" r:id="rId4"/>
+    <sheet name="ERR Milestone 1" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc520203303" localSheetId="3">'1.0 Release Candidate 2'!$C$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="535">
   <si>
     <t>Document</t>
   </si>
@@ -3483,6 +3484,9 @@
   </si>
   <si>
     <t>Added note re. upper limit</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Submission Request: Data Items</t>
   </si>
 </sst>
 </file>
@@ -4106,7 +4110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="246">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -4514,6 +4518,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4559,8 +4575,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4583,66 +4629,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4664,6 +4650,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4682,11 +4698,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4697,13 +4716,61 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4723,63 +4790,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5154,7 +5164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -5184,12 +5194,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="155" t="s">
+      <c r="A2" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="157"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="161"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5212,12 +5222,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="155" t="s">
+      <c r="A4" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="156"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="157"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="161"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5257,10 +5267,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="158" t="s">
+      <c r="A7" s="162" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="161">
+      <c r="B7" s="165">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -5274,8 +5284,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="159"/>
-      <c r="B8" s="162"/>
+      <c r="A8" s="163"/>
+      <c r="B8" s="166"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -5287,8 +5297,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="159"/>
-      <c r="B9" s="162"/>
+      <c r="A9" s="163"/>
+      <c r="B9" s="166"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -5300,8 +5310,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="159"/>
-      <c r="B10" s="162"/>
+      <c r="A10" s="163"/>
+      <c r="B10" s="166"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -5313,8 +5323,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="159"/>
-      <c r="B11" s="162"/>
+      <c r="A11" s="163"/>
+      <c r="B11" s="166"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -5326,8 +5336,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="160"/>
-      <c r="B12" s="163"/>
+      <c r="A12" s="164"/>
+      <c r="B12" s="167"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5339,10 +5349,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="166" t="s">
+      <c r="A13" s="170" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="161">
+      <c r="B13" s="165">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -5356,8 +5366,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="167"/>
-      <c r="B14" s="163"/>
+      <c r="A14" s="171"/>
+      <c r="B14" s="167"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5403,12 +5413,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="155" t="s">
+      <c r="A17" s="159" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="156"/>
-      <c r="C17" s="156"/>
-      <c r="D17" s="157"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="160"/>
+      <c r="D17" s="161"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5448,21 +5458,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="155" t="s">
+      <c r="A20" s="159" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="156"/>
-      <c r="C20" s="156"/>
-      <c r="D20" s="157"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="160"/>
+      <c r="D20" s="161"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="168" t="s">
+      <c r="A21" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="165">
+      <c r="B21" s="169">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -5476,8 +5486,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="169"/>
-      <c r="B22" s="163"/>
+      <c r="A22" s="173"/>
+      <c r="B22" s="167"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -5500,18 +5510,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="159" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="157"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="160"/>
+      <c r="D24" s="161"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="164" t="s">
+      <c r="A25" s="168" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="165">
+      <c r="B25" s="169">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5525,8 +5535,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="159"/>
-      <c r="B26" s="162"/>
+      <c r="A26" s="163"/>
+      <c r="B26" s="166"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5538,8 +5548,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="159"/>
-      <c r="B27" s="162"/>
+      <c r="A27" s="163"/>
+      <c r="B27" s="166"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5551,8 +5561,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="159"/>
-      <c r="B28" s="162"/>
+      <c r="A28" s="163"/>
+      <c r="B28" s="166"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5564,8 +5574,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="159"/>
-      <c r="B29" s="162"/>
+      <c r="A29" s="163"/>
+      <c r="B29" s="166"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5577,8 +5587,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="159"/>
-      <c r="B30" s="162"/>
+      <c r="A30" s="163"/>
+      <c r="B30" s="166"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5590,8 +5600,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="159"/>
-      <c r="B31" s="162"/>
+      <c r="A31" s="163"/>
+      <c r="B31" s="166"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5603,8 +5613,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="160"/>
-      <c r="B32" s="163"/>
+      <c r="A32" s="164"/>
+      <c r="B32" s="167"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5728,12 +5738,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="155" t="s">
+      <c r="A41" s="159" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="156"/>
-      <c r="C41" s="156"/>
-      <c r="D41" s="157"/>
+      <c r="B41" s="160"/>
+      <c r="C41" s="160"/>
+      <c r="D41" s="161"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5793,7 +5803,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5803,7 +5813,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5834,7 +5844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC79"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A30" sqref="A30:A38"/>
     </sheetView>
   </sheetViews>
@@ -5913,10 +5923,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="184" t="s">
+      <c r="B7" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5927,8 +5937,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="185"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="175"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5937,8 +5947,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="185"/>
-      <c r="B9" s="184"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5947,8 +5957,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="185"/>
-      <c r="B10" s="184"/>
+      <c r="A10" s="174"/>
+      <c r="B10" s="175"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5957,8 +5967,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="185"/>
-      <c r="B11" s="184"/>
+      <c r="A11" s="174"/>
+      <c r="B11" s="175"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5967,8 +5977,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="185"/>
-      <c r="B12" s="184"/>
+      <c r="A12" s="174"/>
+      <c r="B12" s="175"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5977,10 +5987,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="187" t="s">
+      <c r="A13" s="177" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="184" t="s">
+      <c r="B13" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5991,8 +6001,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="187"/>
-      <c r="B14" s="184"/>
+      <c r="A14" s="177"/>
+      <c r="B14" s="175"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -6001,8 +6011,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="187"/>
-      <c r="B15" s="184"/>
+      <c r="A15" s="177"/>
+      <c r="B15" s="175"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -6011,7 +6021,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="170" t="s">
+      <c r="A16" s="178" t="s">
         <v>74</v>
       </c>
       <c r="B16" s="179" t="s">
@@ -6025,7 +6035,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="170"/>
+      <c r="A17" s="178"/>
       <c r="B17" s="179"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
@@ -6035,7 +6045,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="170"/>
+      <c r="A18" s="178"/>
       <c r="B18" s="179"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
@@ -6045,7 +6055,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="170"/>
+      <c r="A19" s="178"/>
       <c r="B19" s="179"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
@@ -6055,7 +6065,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="170"/>
+      <c r="A20" s="178"/>
       <c r="B20" s="179"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
@@ -6065,7 +6075,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="170"/>
+      <c r="A21" s="178"/>
       <c r="B21" s="179"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
@@ -6075,7 +6085,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="170"/>
+      <c r="A22" s="178"/>
       <c r="B22" s="179"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
@@ -6085,7 +6095,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="170"/>
+      <c r="A23" s="178"/>
       <c r="B23" s="179"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
@@ -6095,26 +6105,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="170"/>
+      <c r="A24" s="178"/>
       <c r="B24" s="179"/>
-      <c r="C24" s="170" t="s">
+      <c r="C24" s="178" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="171" t="s">
+      <c r="D24" s="185" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="170"/>
+      <c r="A25" s="178"/>
       <c r="B25" s="179"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="171"/>
+      <c r="C25" s="178"/>
+      <c r="D25" s="185"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="185" t="s">
+      <c r="A26" s="174" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="184" t="s">
+      <c r="B26" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -6125,8 +6135,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="185"/>
-      <c r="B27" s="184"/>
+      <c r="A27" s="174"/>
+      <c r="B27" s="175"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -6153,28 +6163,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="186" t="s">
+      <c r="A30" s="176" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="184" t="s">
+      <c r="B30" s="175" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="170" t="s">
+      <c r="C30" s="178" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="174" t="s">
+      <c r="D30" s="188" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="186"/>
-      <c r="B31" s="184"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="174"/>
+      <c r="A31" s="176"/>
+      <c r="B31" s="175"/>
+      <c r="C31" s="178"/>
+      <c r="D31" s="188"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="186"/>
-      <c r="B32" s="184"/>
+      <c r="A32" s="176"/>
+      <c r="B32" s="175"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -6183,8 +6193,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="186"/>
-      <c r="B33" s="184"/>
+      <c r="A33" s="176"/>
+      <c r="B33" s="175"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -6193,8 +6203,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="186"/>
-      <c r="B34" s="184"/>
+      <c r="A34" s="176"/>
+      <c r="B34" s="175"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -6203,8 +6213,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="186"/>
-      <c r="B35" s="184"/>
+      <c r="A35" s="176"/>
+      <c r="B35" s="175"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -6213,8 +6223,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="186"/>
-      <c r="B36" s="184"/>
+      <c r="A36" s="176"/>
+      <c r="B36" s="175"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -6223,26 +6233,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="186"/>
-      <c r="B37" s="184"/>
-      <c r="C37" s="175" t="s">
+      <c r="A37" s="176"/>
+      <c r="B37" s="175"/>
+      <c r="C37" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="177" t="s">
+      <c r="D37" s="191" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="186"/>
-      <c r="B38" s="184"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="177"/>
+      <c r="A38" s="176"/>
+      <c r="B38" s="175"/>
+      <c r="C38" s="190"/>
+      <c r="D38" s="191"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="185" t="s">
+      <c r="A39" s="174" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="184" t="s">
+      <c r="B39" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6253,8 +6263,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="185"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="174"/>
+      <c r="B40" s="175"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6281,10 +6291,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="186" t="s">
+      <c r="A43" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="184" t="s">
+      <c r="B43" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6293,8 +6303,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="186"/>
-      <c r="B44" s="184"/>
+      <c r="A44" s="176"/>
+      <c r="B44" s="175"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6303,10 +6313,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="181" t="s">
+      <c r="A45" s="182" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="184" t="s">
+      <c r="B45" s="175" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6315,8 +6325,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="182"/>
-      <c r="B46" s="184"/>
+      <c r="A46" s="183"/>
+      <c r="B46" s="175"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6325,8 +6335,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="182"/>
-      <c r="B47" s="184"/>
+      <c r="A47" s="183"/>
+      <c r="B47" s="175"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6335,8 +6345,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="183"/>
-      <c r="B48" s="184"/>
+      <c r="A48" s="184"/>
+      <c r="B48" s="175"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -22769,10 +22779,10 @@
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A53" s="179"/>
       <c r="B53" s="179"/>
-      <c r="C53" s="173" t="s">
+      <c r="C53" s="187" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="174" t="s">
+      <c r="D53" s="188" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26874,8 +26884,8 @@
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="179"/>
       <c r="B54" s="179"/>
-      <c r="C54" s="173"/>
-      <c r="D54" s="174"/>
+      <c r="C54" s="187"/>
+      <c r="D54" s="188"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30993,7 +31003,7 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="178" t="s">
+      <c r="A57" s="180" t="s">
         <v>84</v>
       </c>
       <c r="B57" s="179" t="s">
@@ -31007,7 +31017,7 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="178"/>
+      <c r="A58" s="180"/>
       <c r="B58" s="179"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
@@ -31017,7 +31027,7 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="178"/>
+      <c r="A59" s="180"/>
       <c r="B59" s="179"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
@@ -31027,7 +31037,7 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="178"/>
+      <c r="A60" s="180"/>
       <c r="B60" s="179"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
@@ -31037,7 +31047,7 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="178"/>
+      <c r="A61" s="180"/>
       <c r="B61" s="179"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
@@ -31047,7 +31057,7 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="178"/>
+      <c r="A62" s="180"/>
       <c r="B62" s="179"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
@@ -31057,7 +31067,7 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="178"/>
+      <c r="A63" s="180"/>
       <c r="B63" s="179"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
@@ -31067,7 +31077,7 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="178"/>
+      <c r="A64" s="180"/>
       <c r="B64" s="179"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
@@ -31075,7 +31085,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="178"/>
+      <c r="A65" s="180"/>
       <c r="B65" s="179"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
@@ -31085,7 +31095,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="178"/>
+      <c r="A66" s="180"/>
       <c r="B66" s="179"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
@@ -31093,7 +31103,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="178"/>
+      <c r="A67" s="180"/>
       <c r="B67" s="179"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
@@ -31103,7 +31113,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="178"/>
+      <c r="A68" s="180"/>
       <c r="B68" s="179"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
@@ -31113,7 +31123,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="178"/>
+      <c r="A69" s="180"/>
       <c r="B69" s="179"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
@@ -31123,7 +31133,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="178"/>
+      <c r="A70" s="180"/>
       <c r="B70" s="179"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
@@ -31133,7 +31143,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="178"/>
+      <c r="A71" s="180"/>
       <c r="B71" s="179"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
@@ -31143,7 +31153,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="178"/>
+      <c r="A72" s="180"/>
       <c r="B72" s="179"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
@@ -31153,7 +31163,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="178"/>
+      <c r="A73" s="180"/>
       <c r="B73" s="179"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
@@ -31161,7 +31171,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="178"/>
+      <c r="A74" s="180"/>
       <c r="B74" s="179"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
@@ -31171,18 +31181,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="178"/>
+      <c r="A75" s="180"/>
       <c r="B75" s="179"/>
-      <c r="C75" s="172"/>
-      <c r="D75" s="180" t="s">
+      <c r="C75" s="186"/>
+      <c r="D75" s="181" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="178"/>
+      <c r="A76" s="180"/>
       <c r="B76" s="179"/>
-      <c r="C76" s="172"/>
-      <c r="D76" s="180"/>
+      <c r="C76" s="186"/>
+      <c r="D76" s="181"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -31206,8 +31216,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -31216,13 +31226,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -31237,22 +31263,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -31306,10 +31316,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="185" t="s">
+      <c r="A4" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="175" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31320,133 +31330,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="185"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="195" t="s">
+      <c r="A5" s="174"/>
+      <c r="B5" s="175"/>
+      <c r="C5" s="201" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="194" t="s">
+      <c r="D5" s="200" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="185"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="195"/>
-      <c r="D6" s="194"/>
+      <c r="A6" s="174"/>
+      <c r="B6" s="175"/>
+      <c r="C6" s="201"/>
+      <c r="D6" s="200"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="185"/>
-      <c r="B7" s="184"/>
+      <c r="A7" s="174"/>
+      <c r="B7" s="175"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="185"/>
-      <c r="B8" s="184"/>
+      <c r="A8" s="174"/>
+      <c r="B8" s="175"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="185"/>
-      <c r="B9" s="184"/>
+      <c r="A9" s="174"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="187" t="s">
+      <c r="A10" s="177" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="184" t="s">
+      <c r="B10" s="175" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="197"/>
-      <c r="D10" s="194" t="s">
+      <c r="C10" s="199"/>
+      <c r="D10" s="200" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="187"/>
-      <c r="B11" s="184"/>
-      <c r="C11" s="197"/>
-      <c r="D11" s="194"/>
+      <c r="A11" s="177"/>
+      <c r="B11" s="175"/>
+      <c r="C11" s="199"/>
+      <c r="D11" s="200"/>
     </row>
     <row r="12" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="187"/>
-      <c r="B12" s="184"/>
-      <c r="C12" s="197"/>
-      <c r="D12" s="194"/>
+      <c r="A12" s="177"/>
+      <c r="B12" s="175"/>
+      <c r="C12" s="199"/>
+      <c r="D12" s="200"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="170" t="s">
+      <c r="A13" s="178" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="179" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="196"/>
-      <c r="D13" s="194" t="s">
+      <c r="C13" s="202"/>
+      <c r="D13" s="200" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="170"/>
+      <c r="A14" s="178"/>
       <c r="B14" s="179"/>
-      <c r="C14" s="196"/>
-      <c r="D14" s="194"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="200"/>
     </row>
     <row r="15" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="170"/>
+      <c r="A15" s="178"/>
       <c r="B15" s="179"/>
-      <c r="C15" s="196"/>
+      <c r="C15" s="202"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="170"/>
+      <c r="A16" s="178"/>
       <c r="B16" s="179"/>
-      <c r="C16" s="196"/>
+      <c r="C16" s="202"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="170"/>
+      <c r="A17" s="178"/>
       <c r="B17" s="179"/>
-      <c r="C17" s="196"/>
+      <c r="C17" s="202"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="170"/>
+      <c r="A18" s="178"/>
       <c r="B18" s="179"/>
-      <c r="C18" s="196"/>
+      <c r="C18" s="202"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="170"/>
+      <c r="A19" s="178"/>
       <c r="B19" s="179"/>
-      <c r="C19" s="196"/>
+      <c r="C19" s="202"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="170"/>
+      <c r="A20" s="178"/>
       <c r="B20" s="179"/>
-      <c r="C20" s="196"/>
+      <c r="C20" s="202"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="170"/>
+      <c r="A21" s="178"/>
       <c r="B21" s="179"/>
-      <c r="C21" s="196"/>
+      <c r="C21" s="202"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="170"/>
+      <c r="A22" s="178"/>
       <c r="B22" s="179"/>
-      <c r="C22" s="196"/>
+      <c r="C22" s="202"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="170"/>
+      <c r="A23" s="178"/>
       <c r="B23" s="179"/>
-      <c r="C23" s="196"/>
+      <c r="C23" s="202"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31544,10 +31554,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="188" t="s">
+      <c r="A32" s="203" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="191" t="s">
+      <c r="B32" s="206" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31558,26 +31568,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="189"/>
-      <c r="B33" s="192"/>
+      <c r="A33" s="204"/>
+      <c r="B33" s="207"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="189"/>
-      <c r="B34" s="192"/>
+      <c r="A34" s="204"/>
+      <c r="B34" s="207"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="189"/>
-      <c r="B35" s="192"/>
+      <c r="A35" s="204"/>
+      <c r="B35" s="207"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="190"/>
-      <c r="B36" s="193"/>
+      <c r="A36" s="205"/>
+      <c r="B36" s="208"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31606,10 +31616,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="186" t="s">
+      <c r="A39" s="176" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="184" t="s">
+      <c r="B39" s="175" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31620,8 +31630,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="186"/>
-      <c r="B40" s="184"/>
+      <c r="A40" s="176"/>
+      <c r="B40" s="175"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31630,84 +31640,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="185" t="s">
+      <c r="A41" s="174" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="184" t="s">
+      <c r="B41" s="175" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="197" t="s">
+      <c r="C41" s="199" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="170" t="s">
+      <c r="D41" s="178" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="185"/>
-      <c r="B42" s="184"/>
-      <c r="C42" s="197"/>
-      <c r="D42" s="170"/>
+      <c r="A42" s="174"/>
+      <c r="B42" s="175"/>
+      <c r="C42" s="199"/>
+      <c r="D42" s="178"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="185"/>
-      <c r="B43" s="184"/>
-      <c r="C43" s="197" t="s">
+      <c r="A43" s="174"/>
+      <c r="B43" s="175"/>
+      <c r="C43" s="199" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="180" t="s">
+      <c r="D43" s="181" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="185"/>
-      <c r="B44" s="184"/>
-      <c r="C44" s="197"/>
-      <c r="D44" s="180"/>
+      <c r="A44" s="174"/>
+      <c r="B44" s="175"/>
+      <c r="C44" s="199"/>
+      <c r="D44" s="181"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="178" t="s">
+      <c r="A45" s="180" t="s">
         <v>32</v>
       </c>
       <c r="B45" s="179" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="201"/>
+      <c r="C45" s="195"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="178"/>
+      <c r="A46" s="180"/>
       <c r="B46" s="179"/>
-      <c r="C46" s="202"/>
-      <c r="D46" s="198" t="s">
+      <c r="C46" s="196"/>
+      <c r="D46" s="192" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="178"/>
+      <c r="A47" s="180"/>
       <c r="B47" s="179"/>
-      <c r="C47" s="202"/>
-      <c r="D47" s="199"/>
+      <c r="C47" s="196"/>
+      <c r="D47" s="193"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="178"/>
+      <c r="A48" s="180"/>
       <c r="B48" s="179"/>
-      <c r="C48" s="203"/>
-      <c r="D48" s="199"/>
+      <c r="C48" s="197"/>
+      <c r="D48" s="193"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="178"/>
+      <c r="A49" s="180"/>
       <c r="B49" s="179"/>
-      <c r="C49" s="173"/>
-      <c r="D49" s="199"/>
+      <c r="C49" s="187"/>
+      <c r="D49" s="193"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="178"/>
+      <c r="A50" s="180"/>
       <c r="B50" s="179"/>
-      <c r="C50" s="173"/>
-      <c r="D50" s="200"/>
+      <c r="C50" s="187"/>
+      <c r="D50" s="194"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31766,7 +31776,7 @@
     <row r="56" spans="1:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="179"/>
       <c r="B56" s="179"/>
-      <c r="C56" s="204" t="s">
+      <c r="C56" s="198" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31776,7 +31786,7 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="179"/>
       <c r="B57" s="179"/>
-      <c r="C57" s="204"/>
+      <c r="C57" s="198"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
@@ -31804,7 +31814,7 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="179"/>
       <c r="B60" s="179"/>
-      <c r="C60" s="204" t="s">
+      <c r="C60" s="198" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31814,7 +31824,7 @@
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="179"/>
       <c r="B61" s="179"/>
-      <c r="C61" s="204"/>
+      <c r="C61" s="198"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
@@ -31822,7 +31832,7 @@
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="179"/>
       <c r="B62" s="179"/>
-      <c r="C62" s="204"/>
+      <c r="C62" s="198"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
@@ -31830,7 +31840,7 @@
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="179"/>
       <c r="B63" s="179"/>
-      <c r="C63" s="197" t="s">
+      <c r="C63" s="199" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31840,28 +31850,28 @@
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="179"/>
       <c r="B64" s="179"/>
-      <c r="C64" s="197"/>
-      <c r="D64" s="180" t="s">
+      <c r="C64" s="199"/>
+      <c r="D64" s="181" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="179"/>
       <c r="B65" s="179"/>
-      <c r="C65" s="197"/>
-      <c r="D65" s="180"/>
+      <c r="C65" s="199"/>
+      <c r="D65" s="181"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="179"/>
       <c r="B66" s="179"/>
-      <c r="C66" s="197"/>
-      <c r="D66" s="180"/>
+      <c r="C66" s="199"/>
+      <c r="D66" s="181"/>
     </row>
     <row r="67" spans="1:4" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="179"/>
       <c r="B67" s="179"/>
-      <c r="C67" s="197"/>
-      <c r="D67" s="180"/>
+      <c r="C67" s="199"/>
+      <c r="D67" s="181"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31917,6 +31927,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31933,23 +31960,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31960,8 +31970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111:A129"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A95" sqref="A95:A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31995,10 +32005,10 @@
       <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="205" t="s">
+      <c r="A3" s="209" t="s">
         <v>432</v>
       </c>
-      <c r="B3" s="205" t="s">
+      <c r="B3" s="209" t="s">
         <v>433</v>
       </c>
       <c r="C3" s="101" t="s">
@@ -32009,8 +32019,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="206"/>
-      <c r="B4" s="206"/>
+      <c r="A4" s="210"/>
+      <c r="B4" s="210"/>
       <c r="C4" s="100" t="s">
         <v>436</v>
       </c>
@@ -32019,8 +32029,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="207"/>
-      <c r="B5" s="207"/>
+      <c r="A5" s="211"/>
+      <c r="B5" s="211"/>
       <c r="C5" s="100" t="s">
         <v>436</v>
       </c>
@@ -32029,10 +32039,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="213" t="s">
+      <c r="A6" s="218" t="s">
         <v>438</v>
       </c>
-      <c r="B6" s="208" t="s">
+      <c r="B6" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C6" s="100"/>
@@ -32041,32 +32051,32 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="214"/>
-      <c r="B7" s="209"/>
+      <c r="A7" s="219"/>
+      <c r="B7" s="213"/>
       <c r="C7" s="100"/>
       <c r="D7" s="58" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="214"/>
-      <c r="B8" s="209"/>
+      <c r="A8" s="219"/>
+      <c r="B8" s="213"/>
       <c r="C8" s="100"/>
       <c r="D8" s="140" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="214"/>
-      <c r="B9" s="209"/>
+      <c r="A9" s="219"/>
+      <c r="B9" s="213"/>
       <c r="C9" s="100"/>
       <c r="D9" s="140" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="215"/>
-      <c r="B10" s="210"/>
+      <c r="A10" s="220"/>
+      <c r="B10" s="214"/>
       <c r="C10" s="100" t="s">
         <v>498</v>
       </c>
@@ -32075,10 +32085,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="205" t="s">
+      <c r="A11" s="209" t="s">
         <v>525</v>
       </c>
-      <c r="B11" s="208" t="s">
+      <c r="B11" s="212" t="s">
         <v>433</v>
       </c>
       <c r="C11" s="100" t="s">
@@ -32089,8 +32099,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="206"/>
-      <c r="B12" s="209"/>
+      <c r="A12" s="210"/>
+      <c r="B12" s="213"/>
       <c r="C12" s="100" t="s">
         <v>526</v>
       </c>
@@ -32099,8 +32109,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
-      <c r="B13" s="210"/>
+      <c r="A13" s="211"/>
+      <c r="B13" s="214"/>
       <c r="C13" s="100" t="s">
         <v>529</v>
       </c>
@@ -32117,10 +32127,10 @@
       <c r="D14" s="104"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="225" t="s">
+      <c r="A15" s="222" t="s">
         <v>247</v>
       </c>
-      <c r="B15" s="208" t="s">
+      <c r="B15" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C15" s="128" t="s">
@@ -32131,8 +32141,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="227"/>
-      <c r="B16" s="210"/>
+      <c r="A16" s="223"/>
+      <c r="B16" s="214"/>
       <c r="C16" s="128" t="s">
         <v>474</v>
       </c>
@@ -32167,10 +32177,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="205" t="s">
+      <c r="A19" s="209" t="s">
         <v>279</v>
       </c>
-      <c r="B19" s="208" t="s">
+      <c r="B19" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C19" s="95" t="s">
@@ -32181,8 +32191,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="206"/>
-      <c r="B20" s="209"/>
+      <c r="A20" s="210"/>
+      <c r="B20" s="213"/>
       <c r="C20" s="106" t="s">
         <v>299</v>
       </c>
@@ -32191,8 +32201,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="206"/>
-      <c r="B21" s="209"/>
+      <c r="A21" s="210"/>
+      <c r="B21" s="213"/>
       <c r="C21" s="128" t="s">
         <v>280</v>
       </c>
@@ -32201,8 +32211,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="206"/>
-      <c r="B22" s="209"/>
+      <c r="A22" s="210"/>
+      <c r="B22" s="213"/>
       <c r="C22" s="128" t="s">
         <v>21</v>
       </c>
@@ -32211,8 +32221,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="206"/>
-      <c r="B23" s="209"/>
+      <c r="A23" s="210"/>
+      <c r="B23" s="213"/>
       <c r="C23" s="100" t="s">
         <v>434</v>
       </c>
@@ -32221,8 +32231,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="206"/>
-      <c r="B24" s="209"/>
+      <c r="A24" s="210"/>
+      <c r="B24" s="213"/>
       <c r="C24" s="100" t="s">
         <v>444</v>
       </c>
@@ -32231,8 +32241,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="206"/>
-      <c r="B25" s="209"/>
+      <c r="A25" s="210"/>
+      <c r="B25" s="213"/>
       <c r="C25" s="100" t="s">
         <v>446</v>
       </c>
@@ -32241,8 +32251,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="206"/>
-      <c r="B26" s="209"/>
+      <c r="A26" s="210"/>
+      <c r="B26" s="213"/>
       <c r="C26" s="100" t="s">
         <v>434</v>
       </c>
@@ -32251,8 +32261,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="206"/>
-      <c r="B27" s="209"/>
+      <c r="A27" s="210"/>
+      <c r="B27" s="213"/>
       <c r="C27" s="142" t="s">
         <v>453</v>
       </c>
@@ -32261,8 +32271,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="207"/>
-      <c r="B28" s="210"/>
+      <c r="A28" s="211"/>
+      <c r="B28" s="214"/>
       <c r="C28" s="142">
         <v>1.1000000000000001</v>
       </c>
@@ -32271,10 +32281,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="213" t="s">
+      <c r="A29" s="218" t="s">
         <v>452</v>
       </c>
-      <c r="B29" s="208" t="s">
+      <c r="B29" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C29" s="100" t="s">
@@ -32285,8 +32295,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="214"/>
-      <c r="B30" s="209"/>
+      <c r="A30" s="219"/>
+      <c r="B30" s="213"/>
       <c r="C30" s="100" t="s">
         <v>453</v>
       </c>
@@ -32295,8 +32305,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="214"/>
-      <c r="B31" s="209"/>
+      <c r="A31" s="219"/>
+      <c r="B31" s="213"/>
       <c r="C31" s="100">
         <v>3.3</v>
       </c>
@@ -32305,8 +32315,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="214"/>
-      <c r="B32" s="209"/>
+      <c r="A32" s="219"/>
+      <c r="B32" s="213"/>
       <c r="C32" s="130">
         <v>3</v>
       </c>
@@ -32315,8 +32325,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="215"/>
-      <c r="B33" s="210"/>
+      <c r="A33" s="220"/>
+      <c r="B33" s="214"/>
       <c r="C33" s="130">
         <v>3.5</v>
       </c>
@@ -32325,10 +32335,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="213" t="s">
+      <c r="A34" s="218" t="s">
         <v>457</v>
       </c>
-      <c r="B34" s="208" t="s">
+      <c r="B34" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C34" s="130"/>
@@ -32337,18 +32347,18 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="215"/>
-      <c r="B35" s="210"/>
+      <c r="A35" s="220"/>
+      <c r="B35" s="214"/>
       <c r="C35" s="100"/>
       <c r="D35" s="67" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="237" t="s">
+      <c r="A36" s="221" t="s">
         <v>501</v>
       </c>
-      <c r="B36" s="208" t="s">
+      <c r="B36" s="212" t="s">
         <v>439</v>
       </c>
       <c r="D36" s="67" t="s">
@@ -32356,8 +32366,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="237"/>
-      <c r="B37" s="209"/>
+      <c r="A37" s="221"/>
+      <c r="B37" s="213"/>
       <c r="C37" s="144" t="s">
         <v>508</v>
       </c>
@@ -32366,8 +32376,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="237"/>
-      <c r="B38" s="209"/>
+      <c r="A38" s="221"/>
+      <c r="B38" s="213"/>
       <c r="C38" s="58" t="s">
         <v>506</v>
       </c>
@@ -32376,8 +32386,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="237"/>
-      <c r="B39" s="209"/>
+      <c r="A39" s="221"/>
+      <c r="B39" s="213"/>
       <c r="C39" s="61" t="s">
         <v>509</v>
       </c>
@@ -32389,7 +32399,7 @@
       <c r="A40" s="146" t="s">
         <v>511</v>
       </c>
-      <c r="B40" s="208" t="s">
+      <c r="B40" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C40" s="100"/>
@@ -32399,7 +32409,7 @@
     </row>
     <row r="41" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="147"/>
-      <c r="B41" s="209"/>
+      <c r="B41" s="213"/>
       <c r="C41" s="100" t="s">
         <v>512</v>
       </c>
@@ -32409,7 +32419,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="148"/>
-      <c r="B42" s="210"/>
+      <c r="B42" s="214"/>
       <c r="C42" s="100"/>
       <c r="D42" s="145" t="s">
         <v>514</v>
@@ -32419,7 +32429,7 @@
       <c r="A43" s="146" t="s">
         <v>502</v>
       </c>
-      <c r="B43" s="208" t="s">
+      <c r="B43" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C43" s="100"/>
@@ -32429,28 +32439,28 @@
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="148"/>
-      <c r="B44" s="210"/>
+      <c r="B44" s="214"/>
       <c r="C44" s="100"/>
       <c r="D44" s="145" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="205" t="s">
+      <c r="A45" s="209" t="s">
         <v>517</v>
       </c>
-      <c r="B45" s="208" t="s">
+      <c r="B45" s="212" t="s">
         <v>439</v>
       </c>
-      <c r="C45" s="232"/>
+      <c r="C45" s="224"/>
       <c r="D45" s="145" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="207"/>
-      <c r="B46" s="210"/>
-      <c r="C46" s="233"/>
+      <c r="A46" s="211"/>
+      <c r="B46" s="214"/>
+      <c r="C46" s="225"/>
       <c r="D46" s="145" t="s">
         <v>518</v>
       </c>
@@ -32500,10 +32510,10 @@
       <c r="D50" s="104"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="237" t="s">
+      <c r="A51" s="221" t="s">
         <v>336</v>
       </c>
-      <c r="B51" s="238" t="s">
+      <c r="B51" s="230" t="s">
         <v>439</v>
       </c>
       <c r="C51" s="100" t="s">
@@ -32514,8 +32524,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="237"/>
-      <c r="B52" s="238"/>
+      <c r="A52" s="221"/>
+      <c r="B52" s="230"/>
       <c r="C52" s="100" t="s">
         <v>341</v>
       </c>
@@ -32524,8 +32534,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="237"/>
-      <c r="B53" s="238"/>
+      <c r="A53" s="221"/>
+      <c r="B53" s="230"/>
       <c r="C53" s="100" t="s">
         <v>337</v>
       </c>
@@ -32542,10 +32552,10 @@
       <c r="D54" s="104"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="228" t="s">
+      <c r="A55" s="231" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="229" t="s">
+      <c r="B55" s="226" t="s">
         <v>439</v>
       </c>
       <c r="C55" s="106"/>
@@ -32554,8 +32564,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="228"/>
-      <c r="B56" s="229"/>
+      <c r="A56" s="231"/>
+      <c r="B56" s="226"/>
       <c r="C56" s="136" t="s">
         <v>234</v>
       </c>
@@ -32564,8 +32574,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="228"/>
-      <c r="B57" s="229"/>
+      <c r="A57" s="231"/>
+      <c r="B57" s="226"/>
       <c r="C57" s="139" t="s">
         <v>484</v>
       </c>
@@ -32574,8 +32584,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="228"/>
-      <c r="B58" s="229"/>
+      <c r="A58" s="231"/>
+      <c r="B58" s="226"/>
       <c r="C58" s="141" t="s">
         <v>484</v>
       </c>
@@ -32584,8 +32594,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="228"/>
-      <c r="B59" s="229"/>
+      <c r="A59" s="231"/>
+      <c r="B59" s="226"/>
       <c r="C59" s="139" t="s">
         <v>498</v>
       </c>
@@ -32594,8 +32604,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="228"/>
-      <c r="B60" s="229"/>
+      <c r="A60" s="231"/>
+      <c r="B60" s="226"/>
       <c r="C60" s="112" t="s">
         <v>498</v>
       </c>
@@ -32604,10 +32614,10 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="225" t="s">
+      <c r="A61" s="222" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="208" t="s">
+      <c r="B61" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C61" s="107" t="s">
@@ -32618,8 +32628,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="226"/>
-      <c r="B62" s="209"/>
+      <c r="A62" s="234"/>
+      <c r="B62" s="213"/>
       <c r="C62" s="136" t="s">
         <v>463</v>
       </c>
@@ -32628,8 +32638,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="227"/>
-      <c r="B63" s="210"/>
+      <c r="A63" s="223"/>
+      <c r="B63" s="214"/>
       <c r="C63" s="137" t="s">
         <v>481</v>
       </c>
@@ -32678,10 +32688,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="228" t="s">
+      <c r="A67" s="231" t="s">
         <v>269</v>
       </c>
-      <c r="B67" s="229" t="s">
+      <c r="B67" s="226" t="s">
         <v>439</v>
       </c>
       <c r="C67" s="106" t="s">
@@ -32692,24 +32702,24 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="228"/>
-      <c r="B68" s="229"/>
+      <c r="A68" s="231"/>
+      <c r="B68" s="226"/>
       <c r="C68" s="106"/>
       <c r="D68" s="80" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="228"/>
-      <c r="B69" s="229"/>
+      <c r="A69" s="231"/>
+      <c r="B69" s="226"/>
       <c r="C69" s="106"/>
       <c r="D69" s="106" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="228"/>
-      <c r="B70" s="229"/>
+      <c r="A70" s="231"/>
+      <c r="B70" s="226"/>
       <c r="C70" s="111" t="s">
         <v>319</v>
       </c>
@@ -32718,8 +32728,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="228"/>
-      <c r="B71" s="229"/>
+      <c r="A71" s="231"/>
+      <c r="B71" s="226"/>
       <c r="C71" s="112" t="s">
         <v>398</v>
       </c>
@@ -32740,10 +32750,10 @@
       <c r="D72" s="106"/>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="234" t="s">
+      <c r="A73" s="227" t="s">
         <v>165</v>
       </c>
-      <c r="B73" s="208" t="s">
+      <c r="B73" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C73" s="106"/>
@@ -32752,8 +32762,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="235"/>
-      <c r="B74" s="209"/>
+      <c r="A74" s="228"/>
+      <c r="B74" s="213"/>
       <c r="C74" s="112" t="s">
         <v>355</v>
       </c>
@@ -32762,8 +32772,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="235"/>
-      <c r="B75" s="209"/>
+      <c r="A75" s="228"/>
+      <c r="B75" s="213"/>
       <c r="C75" s="112" t="s">
         <v>353</v>
       </c>
@@ -32772,8 +32782,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="235"/>
-      <c r="B76" s="209"/>
+      <c r="A76" s="228"/>
+      <c r="B76" s="213"/>
       <c r="C76" s="115" t="s">
         <v>361</v>
       </c>
@@ -32782,8 +32792,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="235"/>
-      <c r="B77" s="209"/>
+      <c r="A77" s="228"/>
+      <c r="B77" s="213"/>
       <c r="C77" s="112" t="s">
         <v>353</v>
       </c>
@@ -32792,8 +32802,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="235"/>
-      <c r="B78" s="209"/>
+      <c r="A78" s="228"/>
+      <c r="B78" s="213"/>
       <c r="C78" s="112" t="s">
         <v>365</v>
       </c>
@@ -32802,8 +32812,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="235"/>
-      <c r="B79" s="209"/>
+      <c r="A79" s="228"/>
+      <c r="B79" s="213"/>
       <c r="C79" s="112" t="s">
         <v>353</v>
       </c>
@@ -32812,8 +32822,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="235"/>
-      <c r="B80" s="209"/>
+      <c r="A80" s="228"/>
+      <c r="B80" s="213"/>
       <c r="C80" s="112" t="s">
         <v>464</v>
       </c>
@@ -32822,8 +32832,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="235"/>
-      <c r="B81" s="209"/>
+      <c r="A81" s="228"/>
+      <c r="B81" s="213"/>
       <c r="C81" s="133" t="s">
         <v>466</v>
       </c>
@@ -32832,8 +32842,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="235"/>
-      <c r="B82" s="209"/>
+      <c r="A82" s="228"/>
+      <c r="B82" s="213"/>
       <c r="C82" s="133" t="s">
         <v>353</v>
       </c>
@@ -32842,8 +32852,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="235"/>
-      <c r="B83" s="209"/>
+      <c r="A83" s="228"/>
+      <c r="B83" s="213"/>
       <c r="C83" s="138" t="s">
         <v>466</v>
       </c>
@@ -32852,8 +32862,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="235"/>
-      <c r="B84" s="209"/>
+      <c r="A84" s="228"/>
+      <c r="B84" s="213"/>
       <c r="C84" s="112" t="s">
         <v>353</v>
       </c>
@@ -32862,8 +32872,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="235"/>
-      <c r="B85" s="209"/>
+      <c r="A85" s="228"/>
+      <c r="B85" s="213"/>
       <c r="C85" s="112" t="s">
         <v>498</v>
       </c>
@@ -32872,8 +32882,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="235"/>
-      <c r="B86" s="209"/>
+      <c r="A86" s="228"/>
+      <c r="B86" s="213"/>
       <c r="C86" s="112" t="s">
         <v>498</v>
       </c>
@@ -32882,8 +32892,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="235"/>
-      <c r="B87" s="209"/>
+      <c r="A87" s="228"/>
+      <c r="B87" s="213"/>
       <c r="C87" s="151" t="s">
         <v>520</v>
       </c>
@@ -32892,8 +32902,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="236"/>
-      <c r="B88" s="210"/>
+      <c r="A88" s="229"/>
+      <c r="B88" s="214"/>
       <c r="C88" s="112" t="s">
         <v>498</v>
       </c>
@@ -32942,10 +32952,10 @@
       <c r="D91" s="113"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="216" t="s">
+      <c r="A92" s="235" t="s">
         <v>363</v>
       </c>
-      <c r="B92" s="208" t="s">
+      <c r="B92" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C92" s="112" t="s">
@@ -32954,8 +32964,8 @@
       <c r="D92" s="113"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="217"/>
-      <c r="B93" s="210"/>
+      <c r="A93" s="239"/>
+      <c r="B93" s="214"/>
       <c r="C93" s="112" t="s">
         <v>398</v>
       </c>
@@ -32972,10 +32982,10 @@
       <c r="D94" s="103"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="216" t="s">
+      <c r="A95" s="235" t="s">
         <v>236</v>
       </c>
-      <c r="B95" s="208" t="s">
+      <c r="B95" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C95" s="106"/>
@@ -32984,24 +32994,24 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="218"/>
-      <c r="B96" s="209"/>
+      <c r="A96" s="236"/>
+      <c r="B96" s="213"/>
       <c r="C96" s="106"/>
       <c r="D96" s="106" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="218"/>
-      <c r="B97" s="209"/>
+      <c r="A97" s="236"/>
+      <c r="B97" s="213"/>
       <c r="C97" s="106"/>
       <c r="D97" s="106" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="218"/>
-      <c r="B98" s="209"/>
+      <c r="A98" s="236"/>
+      <c r="B98" s="213"/>
       <c r="C98" s="106" t="s">
         <v>294</v>
       </c>
@@ -33010,8 +33020,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="218"/>
-      <c r="B99" s="209"/>
+      <c r="A99" s="236"/>
+      <c r="B99" s="213"/>
       <c r="C99" s="106" t="s">
         <v>322</v>
       </c>
@@ -33020,8 +33030,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="218"/>
-      <c r="B100" s="209"/>
+      <c r="A100" s="236"/>
+      <c r="B100" s="213"/>
       <c r="C100" s="106" t="s">
         <v>367</v>
       </c>
@@ -33030,8 +33040,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="218"/>
-      <c r="B101" s="209"/>
+      <c r="A101" s="236"/>
+      <c r="B101" s="213"/>
       <c r="C101" s="119" t="s">
         <v>468</v>
       </c>
@@ -33040,8 +33050,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="218"/>
-      <c r="B102" s="209"/>
+      <c r="A102" s="236"/>
+      <c r="B102" s="213"/>
       <c r="C102" s="58" t="s">
         <v>37</v>
       </c>
@@ -33050,8 +33060,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="218"/>
-      <c r="B103" s="209"/>
+      <c r="A103" s="236"/>
+      <c r="B103" s="213"/>
       <c r="C103" s="130" t="s">
         <v>353</v>
       </c>
@@ -33060,8 +33070,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="218"/>
-      <c r="B104" s="209"/>
+      <c r="A104" s="236"/>
+      <c r="B104" s="213"/>
       <c r="C104" s="130" t="s">
         <v>466</v>
       </c>
@@ -33070,8 +33080,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="218"/>
-      <c r="B105" s="209"/>
+      <c r="A105" s="236"/>
+      <c r="B105" s="213"/>
       <c r="C105" s="130" t="s">
         <v>367</v>
       </c>
@@ -33080,8 +33090,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="218"/>
-      <c r="B106" s="209"/>
+      <c r="A106" s="236"/>
+      <c r="B106" s="213"/>
       <c r="C106" s="130" t="s">
         <v>353</v>
       </c>
@@ -33090,8 +33100,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="218"/>
-      <c r="B107" s="209"/>
+      <c r="A107" s="236"/>
+      <c r="B107" s="213"/>
       <c r="C107" s="130" t="s">
         <v>498</v>
       </c>
@@ -33100,8 +33110,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="218"/>
-      <c r="B108" s="209"/>
+      <c r="A108" s="236"/>
+      <c r="B108" s="213"/>
       <c r="C108" s="109" t="s">
         <v>498</v>
       </c>
@@ -33110,8 +33120,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="218"/>
-      <c r="B109" s="209"/>
+      <c r="A109" s="236"/>
+      <c r="B109" s="213"/>
       <c r="C109" s="151" t="s">
         <v>520</v>
       </c>
@@ -33120,8 +33130,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="217"/>
-      <c r="B110" s="210"/>
+      <c r="A110" s="239"/>
+      <c r="B110" s="214"/>
       <c r="C110" s="109" t="s">
         <v>498</v>
       </c>
@@ -33130,22 +33140,22 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="219" t="s">
+      <c r="A111" s="240" t="s">
         <v>27</v>
       </c>
-      <c r="B111" s="208" t="s">
+      <c r="B111" s="212" t="s">
         <v>439</v>
       </c>
-      <c r="C111" s="242" t="s">
+      <c r="C111" s="157" t="s">
         <v>532</v>
       </c>
-      <c r="D111" s="243" t="s">
+      <c r="D111" s="158" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="220"/>
-      <c r="B112" s="209"/>
+      <c r="A112" s="241"/>
+      <c r="B112" s="213"/>
       <c r="C112" s="106" t="s">
         <v>297</v>
       </c>
@@ -33154,16 +33164,16 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="220"/>
-      <c r="B113" s="209"/>
+      <c r="A113" s="241"/>
+      <c r="B113" s="213"/>
       <c r="C113" s="106"/>
       <c r="D113" s="106" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="220"/>
-      <c r="B114" s="209"/>
+      <c r="A114" s="241"/>
+      <c r="B114" s="213"/>
       <c r="C114" s="117" t="s">
         <v>323</v>
       </c>
@@ -33172,8 +33182,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="220"/>
-      <c r="B115" s="209"/>
+      <c r="A115" s="241"/>
+      <c r="B115" s="213"/>
       <c r="C115" s="117" t="s">
         <v>353</v>
       </c>
@@ -33182,8 +33192,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="220"/>
-      <c r="B116" s="209"/>
+      <c r="A116" s="241"/>
+      <c r="B116" s="213"/>
       <c r="C116" s="117" t="s">
         <v>361</v>
       </c>
@@ -33192,8 +33202,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="220"/>
-      <c r="B117" s="209"/>
+      <c r="A117" s="241"/>
+      <c r="B117" s="213"/>
       <c r="C117" s="117" t="s">
         <v>365</v>
       </c>
@@ -33202,8 +33212,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="220"/>
-      <c r="B118" s="209"/>
+      <c r="A118" s="241"/>
+      <c r="B118" s="213"/>
       <c r="C118" s="117" t="s">
         <v>375</v>
       </c>
@@ -33212,8 +33222,8 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="220"/>
-      <c r="B119" s="209"/>
+      <c r="A119" s="241"/>
+      <c r="B119" s="213"/>
       <c r="C119" s="109" t="s">
         <v>353</v>
       </c>
@@ -33222,8 +33232,8 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="220"/>
-      <c r="B120" s="209"/>
+      <c r="A120" s="241"/>
+      <c r="B120" s="213"/>
       <c r="C120" s="109" t="s">
         <v>464</v>
       </c>
@@ -33232,8 +33242,8 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="220"/>
-      <c r="B121" s="209"/>
+      <c r="A121" s="241"/>
+      <c r="B121" s="213"/>
       <c r="C121" s="130" t="s">
         <v>466</v>
       </c>
@@ -33242,8 +33252,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="220"/>
-      <c r="B122" s="209"/>
+      <c r="A122" s="241"/>
+      <c r="B122" s="213"/>
       <c r="C122" s="130" t="s">
         <v>353</v>
       </c>
@@ -33252,8 +33262,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="220"/>
-      <c r="B123" s="209"/>
+      <c r="A123" s="241"/>
+      <c r="B123" s="213"/>
       <c r="C123" s="130" t="s">
         <v>466</v>
       </c>
@@ -33262,8 +33272,8 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="220"/>
-      <c r="B124" s="209"/>
+      <c r="A124" s="241"/>
+      <c r="B124" s="213"/>
       <c r="C124" s="130" t="s">
         <v>367</v>
       </c>
@@ -33272,8 +33282,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="220"/>
-      <c r="B125" s="209"/>
+      <c r="A125" s="241"/>
+      <c r="B125" s="213"/>
       <c r="C125" s="130" t="s">
         <v>353</v>
       </c>
@@ -33282,8 +33292,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="220"/>
-      <c r="B126" s="209"/>
+      <c r="A126" s="241"/>
+      <c r="B126" s="213"/>
       <c r="C126" s="130" t="s">
         <v>498</v>
       </c>
@@ -33292,8 +33302,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="220"/>
-      <c r="B127" s="209"/>
+      <c r="A127" s="241"/>
+      <c r="B127" s="213"/>
       <c r="C127" s="109" t="s">
         <v>498</v>
       </c>
@@ -33302,8 +33312,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="220"/>
-      <c r="B128" s="209"/>
+      <c r="A128" s="241"/>
+      <c r="B128" s="213"/>
       <c r="C128" s="151" t="s">
         <v>520</v>
       </c>
@@ -33312,8 +33322,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="221"/>
-      <c r="B129" s="210"/>
+      <c r="A129" s="242"/>
+      <c r="B129" s="214"/>
       <c r="C129" s="109" t="s">
         <v>498</v>
       </c>
@@ -33322,13 +33332,13 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="225" t="s">
+      <c r="A130" s="222" t="s">
         <v>222</v>
       </c>
-      <c r="B130" s="208" t="s">
+      <c r="B130" s="212" t="s">
         <v>439</v>
       </c>
-      <c r="C130" s="222" t="s">
+      <c r="C130" s="243" t="s">
         <v>238</v>
       </c>
       <c r="D130" s="96" t="s">
@@ -33336,17 +33346,17 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="226"/>
-      <c r="B131" s="209"/>
-      <c r="C131" s="223"/>
+      <c r="A131" s="234"/>
+      <c r="B131" s="213"/>
+      <c r="C131" s="244"/>
       <c r="D131" s="113" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="226"/>
-      <c r="B132" s="209"/>
-      <c r="C132" s="224" t="s">
+      <c r="A132" s="234"/>
+      <c r="B132" s="213"/>
+      <c r="C132" s="245" t="s">
         <v>239</v>
       </c>
       <c r="D132" s="106" t="s">
@@ -33354,16 +33364,16 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="226"/>
-      <c r="B133" s="209"/>
-      <c r="C133" s="224"/>
+      <c r="A133" s="234"/>
+      <c r="B133" s="213"/>
+      <c r="C133" s="245"/>
       <c r="D133" s="119" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="226"/>
-      <c r="B134" s="209"/>
+      <c r="A134" s="234"/>
+      <c r="B134" s="213"/>
       <c r="C134" s="112" t="s">
         <v>301</v>
       </c>
@@ -33372,8 +33382,8 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="226"/>
-      <c r="B135" s="209"/>
+      <c r="A135" s="234"/>
+      <c r="B135" s="213"/>
       <c r="C135" s="112">
         <v>2.1</v>
       </c>
@@ -33382,8 +33392,8 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="226"/>
-      <c r="B136" s="209"/>
+      <c r="A136" s="234"/>
+      <c r="B136" s="213"/>
       <c r="C136" s="112" t="s">
         <v>238</v>
       </c>
@@ -33392,8 +33402,8 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="226"/>
-      <c r="B137" s="209"/>
+      <c r="A137" s="234"/>
+      <c r="B137" s="213"/>
       <c r="C137" s="112" t="s">
         <v>238</v>
       </c>
@@ -33402,8 +33412,8 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="226"/>
-      <c r="B138" s="209"/>
+      <c r="A138" s="234"/>
+      <c r="B138" s="213"/>
       <c r="C138" s="112" t="s">
         <v>238</v>
       </c>
@@ -33412,8 +33422,8 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="226"/>
-      <c r="B139" s="209"/>
+      <c r="A139" s="234"/>
+      <c r="B139" s="213"/>
       <c r="C139" s="120" t="s">
         <v>372</v>
       </c>
@@ -33422,8 +33432,8 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="226"/>
-      <c r="B140" s="209"/>
+      <c r="A140" s="234"/>
+      <c r="B140" s="213"/>
       <c r="C140" s="112">
         <v>2.1</v>
       </c>
@@ -33432,8 +33442,8 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="226"/>
-      <c r="B141" s="209"/>
+      <c r="A141" s="234"/>
+      <c r="B141" s="213"/>
       <c r="C141" s="112" t="s">
         <v>238</v>
       </c>
@@ -33442,8 +33452,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="226"/>
-      <c r="B142" s="209"/>
+      <c r="A142" s="234"/>
+      <c r="B142" s="213"/>
       <c r="C142" s="112" t="s">
         <v>238</v>
       </c>
@@ -33452,8 +33462,8 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="226"/>
-      <c r="B143" s="209"/>
+      <c r="A143" s="234"/>
+      <c r="B143" s="213"/>
       <c r="C143" s="112">
         <v>2.1</v>
       </c>
@@ -33462,10 +33472,10 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="219" t="s">
+      <c r="A144" s="240" t="s">
         <v>290</v>
       </c>
-      <c r="B144" s="208" t="s">
+      <c r="B144" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C144" s="106" t="s">
@@ -33476,8 +33486,8 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145" s="220"/>
-      <c r="B145" s="209"/>
+      <c r="A145" s="241"/>
+      <c r="B145" s="213"/>
       <c r="C145" s="119" t="s">
         <v>275</v>
       </c>
@@ -33486,8 +33496,8 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="221"/>
-      <c r="B146" s="210"/>
+      <c r="A146" s="242"/>
+      <c r="B146" s="214"/>
       <c r="C146" s="106" t="s">
         <v>344</v>
       </c>
@@ -33496,10 +33506,10 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="216" t="s">
+      <c r="A147" s="235" t="s">
         <v>364</v>
       </c>
-      <c r="B147" s="208" t="s">
+      <c r="B147" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C147" s="112" t="s">
@@ -33508,8 +33518,8 @@
       <c r="D147" s="106"/>
     </row>
     <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="218"/>
-      <c r="B148" s="209"/>
+      <c r="A148" s="236"/>
+      <c r="B148" s="213"/>
       <c r="C148" s="112" t="s">
         <v>372</v>
       </c>
@@ -33518,8 +33528,8 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="218"/>
-      <c r="B149" s="209"/>
+      <c r="A149" s="236"/>
+      <c r="B149" s="213"/>
       <c r="C149" s="112">
         <v>2.1</v>
       </c>
@@ -33528,8 +33538,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="218"/>
-      <c r="B150" s="209"/>
+      <c r="A150" s="236"/>
+      <c r="B150" s="213"/>
       <c r="C150" s="112" t="s">
         <v>239</v>
       </c>
@@ -33538,8 +33548,8 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="218"/>
-      <c r="B151" s="209"/>
+      <c r="A151" s="236"/>
+      <c r="B151" s="213"/>
       <c r="C151" s="112" t="s">
         <v>238</v>
       </c>
@@ -33568,10 +33578,10 @@
       <c r="D153" s="113"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="225" t="s">
+      <c r="A154" s="222" t="s">
         <v>255</v>
       </c>
-      <c r="B154" s="208" t="s">
+      <c r="B154" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C154" s="106"/>
@@ -33580,24 +33590,24 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="226"/>
-      <c r="B155" s="209"/>
+      <c r="A155" s="234"/>
+      <c r="B155" s="213"/>
       <c r="C155" s="106"/>
       <c r="D155" s="106" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="226"/>
-      <c r="B156" s="209"/>
+      <c r="A156" s="234"/>
+      <c r="B156" s="213"/>
       <c r="C156" s="106"/>
       <c r="D156" s="113" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="226"/>
-      <c r="B157" s="209"/>
+      <c r="A157" s="234"/>
+      <c r="B157" s="213"/>
       <c r="C157" s="106" t="s">
         <v>418</v>
       </c>
@@ -33606,8 +33616,8 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="226"/>
-      <c r="B158" s="209"/>
+      <c r="A158" s="234"/>
+      <c r="B158" s="213"/>
       <c r="C158" s="106" t="s">
         <v>423</v>
       </c>
@@ -33616,8 +33626,8 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="226"/>
-      <c r="B159" s="209"/>
+      <c r="A159" s="234"/>
+      <c r="B159" s="213"/>
       <c r="C159" s="106" t="s">
         <v>484</v>
       </c>
@@ -33626,8 +33636,8 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="226"/>
-      <c r="B160" s="209"/>
+      <c r="A160" s="234"/>
+      <c r="B160" s="213"/>
       <c r="C160" s="106" t="s">
         <v>498</v>
       </c>
@@ -33636,10 +33646,10 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="228" t="s">
+      <c r="A161" s="231" t="s">
         <v>328</v>
       </c>
-      <c r="B161" s="229" t="s">
+      <c r="B161" s="226" t="s">
         <v>439</v>
       </c>
       <c r="C161" s="80" t="s">
@@ -33650,8 +33660,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="228"/>
-      <c r="B162" s="229"/>
+      <c r="A162" s="231"/>
+      <c r="B162" s="226"/>
       <c r="C162" s="106" t="s">
         <v>405</v>
       </c>
@@ -33660,42 +33670,42 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="228"/>
-      <c r="B163" s="229"/>
+      <c r="A163" s="231"/>
+      <c r="B163" s="226"/>
       <c r="C163" s="122" t="s">
         <v>408</v>
       </c>
-      <c r="D163" s="211" t="s">
+      <c r="D163" s="237" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A164" s="228"/>
-      <c r="B164" s="229"/>
+      <c r="A164" s="231"/>
+      <c r="B164" s="226"/>
       <c r="C164" s="122" t="s">
         <v>409</v>
       </c>
-      <c r="D164" s="212"/>
+      <c r="D164" s="238"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="228"/>
-      <c r="B165" s="229"/>
+      <c r="A165" s="231"/>
+      <c r="B165" s="226"/>
       <c r="C165" s="122" t="s">
         <v>410</v>
       </c>
-      <c r="D165" s="212"/>
+      <c r="D165" s="238"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="228"/>
-      <c r="B166" s="229"/>
+      <c r="A166" s="231"/>
+      <c r="B166" s="226"/>
       <c r="C166" s="122" t="s">
         <v>411</v>
       </c>
-      <c r="D166" s="212"/>
+      <c r="D166" s="238"/>
     </row>
     <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="228"/>
-      <c r="B167" s="229"/>
+      <c r="A167" s="231"/>
+      <c r="B167" s="226"/>
       <c r="C167" s="122" t="s">
         <v>470</v>
       </c>
@@ -33718,10 +33728,10 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="239" t="s">
+      <c r="A169" s="215" t="s">
         <v>32</v>
       </c>
-      <c r="B169" s="208" t="s">
+      <c r="B169" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C169" s="106" t="s">
@@ -33732,8 +33742,8 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="240"/>
-      <c r="B170" s="209"/>
+      <c r="A170" s="216"/>
+      <c r="B170" s="213"/>
       <c r="C170" s="106" t="s">
         <v>264</v>
       </c>
@@ -33742,8 +33752,8 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="240"/>
-      <c r="B171" s="209"/>
+      <c r="A171" s="216"/>
+      <c r="B171" s="213"/>
       <c r="C171" s="106" t="s">
         <v>263</v>
       </c>
@@ -33752,8 +33762,8 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="240"/>
-      <c r="B172" s="209"/>
+      <c r="A172" s="216"/>
+      <c r="B172" s="213"/>
       <c r="C172" s="113" t="s">
         <v>271</v>
       </c>
@@ -33762,8 +33772,8 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="240"/>
-      <c r="B173" s="209"/>
+      <c r="A173" s="216"/>
+      <c r="B173" s="213"/>
       <c r="C173" s="106" t="s">
         <v>276</v>
       </c>
@@ -33772,8 +33782,8 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="240"/>
-      <c r="B174" s="209"/>
+      <c r="A174" s="216"/>
+      <c r="B174" s="213"/>
       <c r="C174" s="106" t="s">
         <v>277</v>
       </c>
@@ -33782,8 +33792,8 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="240"/>
-      <c r="B175" s="209"/>
+      <c r="A175" s="216"/>
+      <c r="B175" s="213"/>
       <c r="C175" s="113" t="s">
         <v>282</v>
       </c>
@@ -33792,8 +33802,8 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="240"/>
-      <c r="B176" s="209"/>
+      <c r="A176" s="216"/>
+      <c r="B176" s="213"/>
       <c r="C176" s="113" t="s">
         <v>296</v>
       </c>
@@ -33802,8 +33812,8 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="240"/>
-      <c r="B177" s="209"/>
+      <c r="A177" s="216"/>
+      <c r="B177" s="213"/>
       <c r="C177" s="113" t="s">
         <v>283</v>
       </c>
@@ -33812,8 +33822,8 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" s="240"/>
-      <c r="B178" s="209"/>
+      <c r="A178" s="216"/>
+      <c r="B178" s="213"/>
       <c r="C178" s="123" t="s">
         <v>243</v>
       </c>
@@ -33822,8 +33832,8 @@
       </c>
     </row>
     <row r="179" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A179" s="240"/>
-      <c r="B179" s="209"/>
+      <c r="A179" s="216"/>
+      <c r="B179" s="213"/>
       <c r="C179" s="117" t="s">
         <v>305</v>
       </c>
@@ -33832,8 +33842,8 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="240"/>
-      <c r="B180" s="209"/>
+      <c r="A180" s="216"/>
+      <c r="B180" s="213"/>
       <c r="C180" s="106" t="s">
         <v>306</v>
       </c>
@@ -33842,8 +33852,8 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="240"/>
-      <c r="B181" s="209"/>
+      <c r="A181" s="216"/>
+      <c r="B181" s="213"/>
       <c r="C181" s="113" t="s">
         <v>307</v>
       </c>
@@ -33852,8 +33862,8 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="240"/>
-      <c r="B182" s="209"/>
+      <c r="A182" s="216"/>
+      <c r="B182" s="213"/>
       <c r="C182" s="113" t="s">
         <v>309</v>
       </c>
@@ -33862,8 +33872,8 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="240"/>
-      <c r="B183" s="209"/>
+      <c r="A183" s="216"/>
+      <c r="B183" s="213"/>
       <c r="C183" s="113" t="s">
         <v>262</v>
       </c>
@@ -33872,8 +33882,8 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="240"/>
-      <c r="B184" s="209"/>
+      <c r="A184" s="216"/>
+      <c r="B184" s="213"/>
       <c r="C184" s="106" t="s">
         <v>312</v>
       </c>
@@ -33882,8 +33892,8 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="240"/>
-      <c r="B185" s="209"/>
+      <c r="A185" s="216"/>
+      <c r="B185" s="213"/>
       <c r="C185" s="113" t="s">
         <v>277</v>
       </c>
@@ -33892,8 +33902,8 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="240"/>
-      <c r="B186" s="209"/>
+      <c r="A186" s="216"/>
+      <c r="B186" s="213"/>
       <c r="C186" s="113" t="s">
         <v>313</v>
       </c>
@@ -33902,16 +33912,16 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A187" s="240"/>
-      <c r="B187" s="209"/>
+      <c r="A187" s="216"/>
+      <c r="B187" s="213"/>
       <c r="C187" s="106"/>
       <c r="D187" s="97" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="240"/>
-      <c r="B188" s="209"/>
+      <c r="A188" s="216"/>
+      <c r="B188" s="213"/>
       <c r="C188" s="113" t="s">
         <v>316</v>
       </c>
@@ -33920,8 +33930,8 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="240"/>
-      <c r="B189" s="209"/>
+      <c r="A189" s="216"/>
+      <c r="B189" s="213"/>
       <c r="C189" s="113" t="s">
         <v>262</v>
       </c>
@@ -33930,8 +33940,8 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="240"/>
-      <c r="B190" s="209"/>
+      <c r="A190" s="216"/>
+      <c r="B190" s="213"/>
       <c r="C190" s="113" t="s">
         <v>333</v>
       </c>
@@ -33940,8 +33950,8 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="240"/>
-      <c r="B191" s="209"/>
+      <c r="A191" s="216"/>
+      <c r="B191" s="213"/>
       <c r="C191" s="113" t="s">
         <v>334</v>
       </c>
@@ -33950,8 +33960,8 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="240"/>
-      <c r="B192" s="209"/>
+      <c r="A192" s="216"/>
+      <c r="B192" s="213"/>
       <c r="C192" s="113" t="s">
         <v>318</v>
       </c>
@@ -33960,8 +33970,8 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="240"/>
-      <c r="B193" s="209"/>
+      <c r="A193" s="216"/>
+      <c r="B193" s="213"/>
       <c r="C193" s="113" t="s">
         <v>339</v>
       </c>
@@ -33970,8 +33980,8 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="240"/>
-      <c r="B194" s="209"/>
+      <c r="A194" s="216"/>
+      <c r="B194" s="213"/>
       <c r="C194" s="113" t="s">
         <v>332</v>
       </c>
@@ -33980,8 +33990,8 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="240"/>
-      <c r="B195" s="209"/>
+      <c r="A195" s="216"/>
+      <c r="B195" s="213"/>
       <c r="C195" s="113" t="s">
         <v>347</v>
       </c>
@@ -33990,8 +34000,8 @@
       </c>
     </row>
     <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="240"/>
-      <c r="B196" s="209"/>
+      <c r="A196" s="216"/>
+      <c r="B196" s="213"/>
       <c r="C196" s="101" t="s">
         <v>350</v>
       </c>
@@ -34000,8 +34010,8 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="240"/>
-      <c r="B197" s="209"/>
+      <c r="A197" s="216"/>
+      <c r="B197" s="213"/>
       <c r="C197" s="113" t="s">
         <v>351</v>
       </c>
@@ -34010,8 +34020,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="240"/>
-      <c r="B198" s="209"/>
+      <c r="A198" s="216"/>
+      <c r="B198" s="213"/>
       <c r="C198" s="113" t="s">
         <v>352</v>
       </c>
@@ -34020,8 +34030,8 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="240"/>
-      <c r="B199" s="209"/>
+      <c r="A199" s="216"/>
+      <c r="B199" s="213"/>
       <c r="C199" s="113" t="s">
         <v>358</v>
       </c>
@@ -34030,8 +34040,8 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="240"/>
-      <c r="B200" s="209"/>
+      <c r="A200" s="216"/>
+      <c r="B200" s="213"/>
       <c r="C200" s="113" t="s">
         <v>360</v>
       </c>
@@ -34040,8 +34050,8 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="240"/>
-      <c r="B201" s="209"/>
+      <c r="A201" s="216"/>
+      <c r="B201" s="213"/>
       <c r="C201" s="113" t="s">
         <v>366</v>
       </c>
@@ -34050,8 +34060,8 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="240"/>
-      <c r="B202" s="209"/>
+      <c r="A202" s="216"/>
+      <c r="B202" s="213"/>
       <c r="C202" s="113" t="s">
         <v>358</v>
       </c>
@@ -34060,8 +34070,8 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="240"/>
-      <c r="B203" s="209"/>
+      <c r="A203" s="216"/>
+      <c r="B203" s="213"/>
       <c r="C203" s="118" t="s">
         <v>379</v>
       </c>
@@ -34070,8 +34080,8 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="240"/>
-      <c r="B204" s="209"/>
+      <c r="A204" s="216"/>
+      <c r="B204" s="213"/>
       <c r="C204" s="106" t="s">
         <v>383</v>
       </c>
@@ -34080,8 +34090,8 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="240"/>
-      <c r="B205" s="209"/>
+      <c r="A205" s="216"/>
+      <c r="B205" s="213"/>
       <c r="C205" s="106" t="s">
         <v>386</v>
       </c>
@@ -34090,8 +34100,8 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="240"/>
-      <c r="B206" s="209"/>
+      <c r="A206" s="216"/>
+      <c r="B206" s="213"/>
       <c r="C206" s="106" t="s">
         <v>387</v>
       </c>
@@ -34100,8 +34110,8 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="240"/>
-      <c r="B207" s="209"/>
+      <c r="A207" s="216"/>
+      <c r="B207" s="213"/>
       <c r="C207" s="106" t="s">
         <v>388</v>
       </c>
@@ -34110,8 +34120,8 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="240"/>
-      <c r="B208" s="209"/>
+      <c r="A208" s="216"/>
+      <c r="B208" s="213"/>
       <c r="C208" s="106" t="s">
         <v>389</v>
       </c>
@@ -34120,8 +34130,8 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="240"/>
-      <c r="B209" s="209"/>
+      <c r="A209" s="216"/>
+      <c r="B209" s="213"/>
       <c r="C209" s="106" t="s">
         <v>390</v>
       </c>
@@ -34130,8 +34140,8 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="240"/>
-      <c r="B210" s="209"/>
+      <c r="A210" s="216"/>
+      <c r="B210" s="213"/>
       <c r="C210" s="106" t="s">
         <v>393</v>
       </c>
@@ -34140,8 +34150,8 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="240"/>
-      <c r="B211" s="209"/>
+      <c r="A211" s="216"/>
+      <c r="B211" s="213"/>
       <c r="C211" s="106" t="s">
         <v>403</v>
       </c>
@@ -34150,8 +34160,8 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="240"/>
-      <c r="B212" s="209"/>
+      <c r="A212" s="216"/>
+      <c r="B212" s="213"/>
       <c r="C212" s="106" t="s">
         <v>404</v>
       </c>
@@ -34160,8 +34170,8 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="240"/>
-      <c r="B213" s="209"/>
+      <c r="A213" s="216"/>
+      <c r="B213" s="213"/>
       <c r="C213" s="106" t="s">
         <v>421</v>
       </c>
@@ -34170,8 +34180,8 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="240"/>
-      <c r="B214" s="209"/>
+      <c r="A214" s="216"/>
+      <c r="B214" s="213"/>
       <c r="C214" s="106" t="s">
         <v>422</v>
       </c>
@@ -34180,8 +34190,8 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="240"/>
-      <c r="B215" s="209"/>
+      <c r="A215" s="216"/>
+      <c r="B215" s="213"/>
       <c r="C215" s="106" t="s">
         <v>425</v>
       </c>
@@ -34190,8 +34200,8 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="240"/>
-      <c r="B216" s="209"/>
+      <c r="A216" s="216"/>
+      <c r="B216" s="213"/>
       <c r="C216" s="58" t="s">
         <v>471</v>
       </c>
@@ -34200,8 +34210,8 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="240"/>
-      <c r="B217" s="209"/>
+      <c r="A217" s="216"/>
+      <c r="B217" s="213"/>
       <c r="C217" s="58" t="s">
         <v>421</v>
       </c>
@@ -34210,8 +34220,8 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="240"/>
-      <c r="B218" s="209"/>
+      <c r="A218" s="216"/>
+      <c r="B218" s="213"/>
       <c r="C218" s="58" t="s">
         <v>497</v>
       </c>
@@ -34220,8 +34230,8 @@
       </c>
     </row>
     <row r="219" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A219" s="240"/>
-      <c r="B219" s="209"/>
+      <c r="A219" s="216"/>
+      <c r="B219" s="213"/>
       <c r="C219" s="61" t="s">
         <v>522</v>
       </c>
@@ -34230,8 +34240,8 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A220" s="241"/>
-      <c r="B220" s="210"/>
+      <c r="A220" s="217"/>
+      <c r="B220" s="214"/>
       <c r="C220" s="61" t="s">
         <v>332</v>
       </c>
@@ -34240,10 +34250,10 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="239" t="s">
+      <c r="A221" s="215" t="s">
         <v>415</v>
       </c>
-      <c r="B221" s="208" t="s">
+      <c r="B221" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C221" s="106" t="s">
@@ -34254,8 +34264,8 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="240"/>
-      <c r="B222" s="209"/>
+      <c r="A222" s="216"/>
+      <c r="B222" s="213"/>
       <c r="C222" s="118" t="s">
         <v>491</v>
       </c>
@@ -34264,8 +34274,8 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="241"/>
-      <c r="B223" s="210"/>
+      <c r="A223" s="217"/>
+      <c r="B223" s="214"/>
       <c r="C223" s="113" t="s">
         <v>524</v>
       </c>
@@ -34310,10 +34320,10 @@
       <c r="D226" s="104"/>
     </row>
     <row r="227" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="225" t="s">
+      <c r="A227" s="222" t="s">
         <v>84</v>
       </c>
-      <c r="B227" s="208" t="s">
+      <c r="B227" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C227" s="106"/>
@@ -34322,8 +34332,8 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="226"/>
-      <c r="B228" s="209"/>
+      <c r="A228" s="234"/>
+      <c r="B228" s="213"/>
       <c r="C228" s="107" t="s">
         <v>245</v>
       </c>
@@ -34332,8 +34342,8 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="226"/>
-      <c r="B229" s="209"/>
+      <c r="A229" s="234"/>
+      <c r="B229" s="213"/>
       <c r="C229" s="107">
         <v>10.1</v>
       </c>
@@ -34342,8 +34352,8 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="226"/>
-      <c r="B230" s="209"/>
+      <c r="A230" s="234"/>
+      <c r="B230" s="213"/>
       <c r="C230" s="107">
         <v>10.199999999999999</v>
       </c>
@@ -34352,8 +34362,8 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="226"/>
-      <c r="B231" s="209"/>
+      <c r="A231" s="234"/>
+      <c r="B231" s="213"/>
       <c r="C231" s="98" t="s">
         <v>287</v>
       </c>
@@ -34362,8 +34372,8 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="226"/>
-      <c r="B232" s="209"/>
+      <c r="A232" s="234"/>
+      <c r="B232" s="213"/>
       <c r="C232" s="98" t="s">
         <v>369</v>
       </c>
@@ -34372,8 +34382,8 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="226"/>
-      <c r="B233" s="209"/>
+      <c r="A233" s="234"/>
+      <c r="B233" s="213"/>
       <c r="C233" s="98" t="s">
         <v>117</v>
       </c>
@@ -34382,8 +34392,8 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="226"/>
-      <c r="B234" s="209"/>
+      <c r="A234" s="234"/>
+      <c r="B234" s="213"/>
       <c r="C234" s="98" t="s">
         <v>416</v>
       </c>
@@ -34392,8 +34402,8 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="226"/>
-      <c r="B235" s="209"/>
+      <c r="A235" s="234"/>
+      <c r="B235" s="213"/>
       <c r="C235" s="98" t="s">
         <v>17</v>
       </c>
@@ -34402,8 +34412,8 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" s="226"/>
-      <c r="B236" s="209"/>
+      <c r="A236" s="234"/>
+      <c r="B236" s="213"/>
       <c r="C236" s="98" t="s">
         <v>496</v>
       </c>
@@ -34412,8 +34422,8 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A237" s="227"/>
-      <c r="B237" s="210"/>
+      <c r="A237" s="223"/>
+      <c r="B237" s="214"/>
       <c r="C237" s="98" t="s">
         <v>496</v>
       </c>
@@ -34422,10 +34432,10 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="225" t="s">
+      <c r="A238" s="222" t="s">
         <v>246</v>
       </c>
-      <c r="B238" s="208" t="s">
+      <c r="B238" s="212" t="s">
         <v>439</v>
       </c>
       <c r="C238" s="98"/>
@@ -34434,8 +34444,8 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="226"/>
-      <c r="B239" s="209"/>
+      <c r="A239" s="234"/>
+      <c r="B239" s="213"/>
       <c r="C239" s="126" t="s">
         <v>427</v>
       </c>
@@ -34466,10 +34476,10 @@
       <c r="D241" s="127"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="225" t="s">
+      <c r="A242" s="222" t="s">
         <v>58</v>
       </c>
-      <c r="B242" s="208" t="s">
+      <c r="B242" s="212" t="s">
         <v>265</v>
       </c>
       <c r="C242" s="128" t="s">
@@ -34480,8 +34490,8 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="226"/>
-      <c r="B243" s="209"/>
+      <c r="A243" s="234"/>
+      <c r="B243" s="213"/>
       <c r="C243" s="128" t="s">
         <v>259</v>
       </c>
@@ -34490,18 +34500,18 @@
       </c>
     </row>
     <row r="244" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="227"/>
-      <c r="B244" s="210"/>
+      <c r="A244" s="223"/>
+      <c r="B244" s="214"/>
       <c r="C244" s="106"/>
       <c r="D244" s="106" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="245" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A245" s="230" t="s">
+      <c r="A245" s="232" t="s">
         <v>59</v>
       </c>
-      <c r="B245" s="208" t="s">
+      <c r="B245" s="212" t="s">
         <v>265</v>
       </c>
       <c r="C245" s="119" t="s">
@@ -34512,18 +34522,18 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="231"/>
-      <c r="B246" s="210"/>
+      <c r="A246" s="233"/>
+      <c r="B246" s="214"/>
       <c r="C246" s="119"/>
       <c r="D246" s="106" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A247" s="230" t="s">
+      <c r="A247" s="232" t="s">
         <v>285</v>
       </c>
-      <c r="B247" s="208" t="s">
+      <c r="B247" s="212" t="s">
         <v>265</v>
       </c>
       <c r="C247" s="119"/>
@@ -34532,18 +34542,18 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="231"/>
-      <c r="B248" s="210"/>
+      <c r="A248" s="233"/>
+      <c r="B248" s="214"/>
       <c r="C248" s="106"/>
       <c r="D248" s="106" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="230" t="s">
+      <c r="A249" s="232" t="s">
         <v>60</v>
       </c>
-      <c r="B249" s="208" t="s">
+      <c r="B249" s="212" t="s">
         <v>265</v>
       </c>
       <c r="C249" s="119" t="s">
@@ -34554,8 +34564,8 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="231"/>
-      <c r="B250" s="210"/>
+      <c r="A250" s="233"/>
+      <c r="B250" s="214"/>
       <c r="C250" s="106"/>
       <c r="D250" s="106" t="s">
         <v>407</v>
@@ -34613,6 +34623,56 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D163:D166"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A95:A110"/>
+    <mergeCell ref="B95:B110"/>
+    <mergeCell ref="A111:A129"/>
+    <mergeCell ref="B111:B129"/>
+    <mergeCell ref="C130:C131"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="B144:B146"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="A227:A237"/>
+    <mergeCell ref="B227:B237"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B130:B143"/>
+    <mergeCell ref="A154:A160"/>
+    <mergeCell ref="B154:B160"/>
+    <mergeCell ref="A130:A143"/>
+    <mergeCell ref="A242:A244"/>
+    <mergeCell ref="B242:B244"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="B238:B239"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="A249:A250"/>
+    <mergeCell ref="B249:B250"/>
+    <mergeCell ref="A245:A246"/>
+    <mergeCell ref="B245:B246"/>
+    <mergeCell ref="A247:A248"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A73:A88"/>
+    <mergeCell ref="B73:B88"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A55:A60"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B221:B223"/>
@@ -34629,58 +34689,65 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A73:A88"/>
-    <mergeCell ref="B73:B88"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A249:A250"/>
-    <mergeCell ref="B249:B250"/>
-    <mergeCell ref="A245:A246"/>
-    <mergeCell ref="B245:B246"/>
-    <mergeCell ref="A247:A248"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="A242:A244"/>
-    <mergeCell ref="B242:B244"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="B238:B239"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="A147:A151"/>
-    <mergeCell ref="B147:B151"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="A227:A237"/>
-    <mergeCell ref="B227:B237"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B130:B143"/>
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="B154:B160"/>
-    <mergeCell ref="A130:A143"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="D163:D166"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A95:A110"/>
-    <mergeCell ref="B95:B110"/>
-    <mergeCell ref="A111:A129"/>
-    <mergeCell ref="B111:B129"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="A144:A146"/>
-    <mergeCell ref="B144:B146"/>
-    <mergeCell ref="A61:A63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DBC65A-63D2-46B3-B8B5-A94A70B9EDFE}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>430</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="104"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="109" t="s">
+        <v>534</v>
+      </c>
+      <c r="B3" s="112" t="s">
+        <v>439</v>
+      </c>
+      <c r="C3" s="156" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="155" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ERR - updating pit4 changelog
</commit_message>
<xml_diff>
--- a/PIT4/Schema Publication Changelog.xlsx
+++ b/PIT4/Schema Publication Changelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwalsh06\IdeaProjects\paye-employers-documentation\src\main\resources\PIT4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\paye-employers-documentation\src\main\resources\PIT4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF58CF23-56E8-4E81-8CE4-33ACCAD7E735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDB739B-8A3D-4160-8CFE-4492D22CFFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,9 +24,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="571">
   <si>
     <t>Document</t>
   </si>
@@ -3559,9 +3559,6 @@
     <t>New file</t>
   </si>
   <si>
-    <t xml:space="preserve">SOAP Reference </t>
-  </si>
-  <si>
     <t>Added Enhanced Reporting Check
 Run and Check Submission Web
 Services</t>
@@ -3582,9 +3579,6 @@
     <t>ERN Schema</t>
   </si>
   <si>
-    <t>Added Enhanced Reporting and ERN Web Services and Schemas</t>
-  </si>
-  <si>
     <t>1, 2.1, 3.8, 3.9</t>
   </si>
   <si>
@@ -3601,6 +3595,9 @@
   </si>
   <si>
     <t>1, 2.1, 3.10</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Validation Rules</t>
   </si>
 </sst>
 </file>
@@ -4700,38 +4697,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4754,6 +4721,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4775,36 +4802,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4823,14 +4820,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4841,61 +4835,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4915,6 +4861,57 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5937,7 +5934,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5947,7 +5944,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -6057,10 +6054,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="179" t="s">
+      <c r="A7" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="180" t="s">
+      <c r="B7" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -6071,8 +6068,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="179"/>
-      <c r="B8" s="180"/>
+      <c r="A8" s="194"/>
+      <c r="B8" s="193"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -6081,8 +6078,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="179"/>
-      <c r="B9" s="180"/>
+      <c r="A9" s="194"/>
+      <c r="B9" s="193"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -6091,8 +6088,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="179"/>
-      <c r="B10" s="180"/>
+      <c r="A10" s="194"/>
+      <c r="B10" s="193"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -6101,8 +6098,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="179"/>
-      <c r="B11" s="180"/>
+      <c r="A11" s="194"/>
+      <c r="B11" s="193"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -6111,8 +6108,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="179"/>
-      <c r="B12" s="180"/>
+      <c r="A12" s="194"/>
+      <c r="B12" s="193"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -6121,10 +6118,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="182" t="s">
+      <c r="A13" s="196" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="180" t="s">
+      <c r="B13" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -6135,8 +6132,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="182"/>
-      <c r="B14" s="180"/>
+      <c r="A14" s="196"/>
+      <c r="B14" s="193"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -6145,8 +6142,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="182"/>
-      <c r="B15" s="180"/>
+      <c r="A15" s="196"/>
+      <c r="B15" s="193"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -6155,10 +6152,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="183" t="s">
+      <c r="A16" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="184" t="s">
+      <c r="B16" s="188" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -6169,8 +6166,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="183"/>
-      <c r="B17" s="184"/>
+      <c r="A17" s="179"/>
+      <c r="B17" s="188"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -6179,8 +6176,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="183"/>
-      <c r="B18" s="184"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="188"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -6189,8 +6186,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="183"/>
-      <c r="B19" s="184"/>
+      <c r="A19" s="179"/>
+      <c r="B19" s="188"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -6199,8 +6196,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183"/>
-      <c r="B20" s="184"/>
+      <c r="A20" s="179"/>
+      <c r="B20" s="188"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -6209,8 +6206,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="183"/>
-      <c r="B21" s="184"/>
+      <c r="A21" s="179"/>
+      <c r="B21" s="188"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -6219,8 +6216,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="183"/>
-      <c r="B22" s="184"/>
+      <c r="A22" s="179"/>
+      <c r="B22" s="188"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -6229,8 +6226,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="183"/>
-      <c r="B23" s="184"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="188"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -6239,26 +6236,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="183"/>
-      <c r="B24" s="184"/>
-      <c r="C24" s="183" t="s">
+      <c r="A24" s="179"/>
+      <c r="B24" s="188"/>
+      <c r="C24" s="179" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="190" t="s">
+      <c r="D24" s="180" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="183"/>
-      <c r="B25" s="184"/>
-      <c r="C25" s="183"/>
-      <c r="D25" s="190"/>
+      <c r="A25" s="179"/>
+      <c r="B25" s="188"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="180"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="179" t="s">
+      <c r="A26" s="194" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="180" t="s">
+      <c r="B26" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -6269,8 +6266,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="179"/>
-      <c r="B27" s="180"/>
+      <c r="A27" s="194"/>
+      <c r="B27" s="193"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -6297,28 +6294,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="181" t="s">
+      <c r="A30" s="195" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="180" t="s">
+      <c r="B30" s="193" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="183" t="s">
+      <c r="C30" s="179" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="193" t="s">
+      <c r="D30" s="183" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="181"/>
-      <c r="B31" s="180"/>
-      <c r="C31" s="183"/>
-      <c r="D31" s="193"/>
+      <c r="A31" s="195"/>
+      <c r="B31" s="193"/>
+      <c r="C31" s="179"/>
+      <c r="D31" s="183"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="181"/>
-      <c r="B32" s="180"/>
+      <c r="A32" s="195"/>
+      <c r="B32" s="193"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -6327,8 +6324,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="181"/>
-      <c r="B33" s="180"/>
+      <c r="A33" s="195"/>
+      <c r="B33" s="193"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -6337,8 +6334,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="181"/>
-      <c r="B34" s="180"/>
+      <c r="A34" s="195"/>
+      <c r="B34" s="193"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -6347,8 +6344,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="181"/>
-      <c r="B35" s="180"/>
+      <c r="A35" s="195"/>
+      <c r="B35" s="193"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -6357,8 +6354,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="181"/>
-      <c r="B36" s="180"/>
+      <c r="A36" s="195"/>
+      <c r="B36" s="193"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -6367,26 +6364,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="181"/>
-      <c r="B37" s="180"/>
-      <c r="C37" s="194" t="s">
+      <c r="A37" s="195"/>
+      <c r="B37" s="193"/>
+      <c r="C37" s="184" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="196" t="s">
+      <c r="D37" s="186" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="181"/>
-      <c r="B38" s="180"/>
-      <c r="C38" s="195"/>
-      <c r="D38" s="196"/>
+      <c r="A38" s="195"/>
+      <c r="B38" s="193"/>
+      <c r="C38" s="185"/>
+      <c r="D38" s="186"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="179" t="s">
+      <c r="A39" s="194" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6397,8 +6394,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="179"/>
-      <c r="B40" s="180"/>
+      <c r="A40" s="194"/>
+      <c r="B40" s="193"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6425,10 +6422,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="181" t="s">
+      <c r="A43" s="195" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="180" t="s">
+      <c r="B43" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6437,8 +6434,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="181"/>
-      <c r="B44" s="180"/>
+      <c r="A44" s="195"/>
+      <c r="B44" s="193"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6447,10 +6444,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="187" t="s">
+      <c r="A45" s="190" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="180" t="s">
+      <c r="B45" s="193" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6459,8 +6456,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="188"/>
-      <c r="B46" s="180"/>
+      <c r="A46" s="191"/>
+      <c r="B46" s="193"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6469,8 +6466,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="188"/>
-      <c r="B47" s="180"/>
+      <c r="A47" s="191"/>
+      <c r="B47" s="193"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6479,8 +6476,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="189"/>
-      <c r="B48" s="180"/>
+      <c r="A48" s="192"/>
+      <c r="B48" s="193"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -6489,10 +6486,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="184" t="s">
+      <c r="A49" s="188" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="184" t="s">
+      <c r="B49" s="188" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10596,8 +10593,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="184"/>
-      <c r="B50" s="184"/>
+      <c r="A50" s="188"/>
+      <c r="B50" s="188"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14701,8 +14698,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="184"/>
-      <c r="B51" s="184"/>
+      <c r="A51" s="188"/>
+      <c r="B51" s="188"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18806,8 +18803,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="184"/>
-      <c r="B52" s="184"/>
+      <c r="A52" s="188"/>
+      <c r="B52" s="188"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22911,12 +22908,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="184"/>
-      <c r="B53" s="184"/>
-      <c r="C53" s="192" t="s">
+      <c r="A53" s="188"/>
+      <c r="B53" s="188"/>
+      <c r="C53" s="182" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="193" t="s">
+      <c r="D53" s="183" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -27016,10 +27013,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="184"/>
-      <c r="B54" s="184"/>
-      <c r="C54" s="192"/>
-      <c r="D54" s="193"/>
+      <c r="A54" s="188"/>
+      <c r="B54" s="188"/>
+      <c r="C54" s="182"/>
+      <c r="D54" s="183"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -31137,10 +31134,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="185" t="s">
+      <c r="A57" s="187" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="184" t="s">
+      <c r="B57" s="188" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -31151,8 +31148,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="185"/>
-      <c r="B58" s="184"/>
+      <c r="A58" s="187"/>
+      <c r="B58" s="188"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -31161,8 +31158,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="185"/>
-      <c r="B59" s="184"/>
+      <c r="A59" s="187"/>
+      <c r="B59" s="188"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -31171,8 +31168,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="185"/>
-      <c r="B60" s="184"/>
+      <c r="A60" s="187"/>
+      <c r="B60" s="188"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -31181,8 +31178,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="185"/>
-      <c r="B61" s="184"/>
+      <c r="A61" s="187"/>
+      <c r="B61" s="188"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -31191,8 +31188,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="185"/>
-      <c r="B62" s="184"/>
+      <c r="A62" s="187"/>
+      <c r="B62" s="188"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -31201,8 +31198,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="185"/>
-      <c r="B63" s="184"/>
+      <c r="A63" s="187"/>
+      <c r="B63" s="188"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -31211,16 +31208,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="185"/>
-      <c r="B64" s="184"/>
+      <c r="A64" s="187"/>
+      <c r="B64" s="188"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="185"/>
-      <c r="B65" s="184"/>
+      <c r="A65" s="187"/>
+      <c r="B65" s="188"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -31229,16 +31226,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="185"/>
-      <c r="B66" s="184"/>
+      <c r="A66" s="187"/>
+      <c r="B66" s="188"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="185"/>
-      <c r="B67" s="184"/>
+      <c r="A67" s="187"/>
+      <c r="B67" s="188"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -31247,8 +31244,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="185"/>
-      <c r="B68" s="184"/>
+      <c r="A68" s="187"/>
+      <c r="B68" s="188"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -31257,8 +31254,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="185"/>
-      <c r="B69" s="184"/>
+      <c r="A69" s="187"/>
+      <c r="B69" s="188"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -31267,8 +31264,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="185"/>
-      <c r="B70" s="184"/>
+      <c r="A70" s="187"/>
+      <c r="B70" s="188"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -31277,8 +31274,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="185"/>
-      <c r="B71" s="184"/>
+      <c r="A71" s="187"/>
+      <c r="B71" s="188"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -31287,8 +31284,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="185"/>
-      <c r="B72" s="184"/>
+      <c r="A72" s="187"/>
+      <c r="B72" s="188"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -31297,16 +31294,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="185"/>
-      <c r="B73" s="184"/>
+      <c r="A73" s="187"/>
+      <c r="B73" s="188"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="185"/>
-      <c r="B74" s="184"/>
+      <c r="A74" s="187"/>
+      <c r="B74" s="188"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -31315,18 +31312,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="185"/>
-      <c r="B75" s="184"/>
-      <c r="C75" s="191"/>
-      <c r="D75" s="186" t="s">
+      <c r="A75" s="187"/>
+      <c r="B75" s="188"/>
+      <c r="C75" s="181"/>
+      <c r="D75" s="189" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="185"/>
-      <c r="B76" s="184"/>
-      <c r="C76" s="191"/>
-      <c r="D76" s="186"/>
+      <c r="A76" s="187"/>
+      <c r="B76" s="188"/>
+      <c r="C76" s="181"/>
+      <c r="D76" s="189"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -31350,8 +31347,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -31360,29 +31357,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -31397,6 +31378,22 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -31450,10 +31447,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="179" t="s">
+      <c r="A4" s="194" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31464,133 +31461,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="179"/>
-      <c r="B5" s="180"/>
-      <c r="C5" s="206" t="s">
+      <c r="A5" s="194"/>
+      <c r="B5" s="193"/>
+      <c r="C5" s="204" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="205" t="s">
+      <c r="D5" s="203" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="179"/>
-      <c r="B6" s="180"/>
-      <c r="C6" s="206"/>
-      <c r="D6" s="205"/>
+      <c r="A6" s="194"/>
+      <c r="B6" s="193"/>
+      <c r="C6" s="204"/>
+      <c r="D6" s="203"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="179"/>
-      <c r="B7" s="180"/>
+      <c r="A7" s="194"/>
+      <c r="B7" s="193"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="179"/>
-      <c r="B8" s="180"/>
+      <c r="A8" s="194"/>
+      <c r="B8" s="193"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="179"/>
-      <c r="B9" s="180"/>
+      <c r="A9" s="194"/>
+      <c r="B9" s="193"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="182" t="s">
+      <c r="A10" s="196" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="180" t="s">
+      <c r="B10" s="193" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="204"/>
-      <c r="D10" s="205" t="s">
+      <c r="C10" s="206"/>
+      <c r="D10" s="203" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="182"/>
-      <c r="B11" s="180"/>
-      <c r="C11" s="204"/>
-      <c r="D11" s="205"/>
+      <c r="A11" s="196"/>
+      <c r="B11" s="193"/>
+      <c r="C11" s="206"/>
+      <c r="D11" s="203"/>
     </row>
     <row r="12" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="182"/>
-      <c r="B12" s="180"/>
-      <c r="C12" s="204"/>
-      <c r="D12" s="205"/>
+      <c r="A12" s="196"/>
+      <c r="B12" s="193"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="203"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="183" t="s">
+      <c r="A13" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="184" t="s">
+      <c r="B13" s="188" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="207"/>
-      <c r="D13" s="205" t="s">
+      <c r="C13" s="205"/>
+      <c r="D13" s="203" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="183"/>
-      <c r="B14" s="184"/>
-      <c r="C14" s="207"/>
-      <c r="D14" s="205"/>
+      <c r="A14" s="179"/>
+      <c r="B14" s="188"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="203"/>
     </row>
     <row r="15" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="183"/>
-      <c r="B15" s="184"/>
-      <c r="C15" s="207"/>
+      <c r="A15" s="179"/>
+      <c r="B15" s="188"/>
+      <c r="C15" s="205"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="183"/>
-      <c r="B16" s="184"/>
-      <c r="C16" s="207"/>
+      <c r="A16" s="179"/>
+      <c r="B16" s="188"/>
+      <c r="C16" s="205"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="183"/>
-      <c r="B17" s="184"/>
-      <c r="C17" s="207"/>
+      <c r="A17" s="179"/>
+      <c r="B17" s="188"/>
+      <c r="C17" s="205"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="183"/>
-      <c r="B18" s="184"/>
-      <c r="C18" s="207"/>
+      <c r="A18" s="179"/>
+      <c r="B18" s="188"/>
+      <c r="C18" s="205"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="183"/>
-      <c r="B19" s="184"/>
-      <c r="C19" s="207"/>
+      <c r="A19" s="179"/>
+      <c r="B19" s="188"/>
+      <c r="C19" s="205"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="183"/>
-      <c r="B20" s="184"/>
-      <c r="C20" s="207"/>
+      <c r="A20" s="179"/>
+      <c r="B20" s="188"/>
+      <c r="C20" s="205"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="183"/>
-      <c r="B21" s="184"/>
-      <c r="C21" s="207"/>
+      <c r="A21" s="179"/>
+      <c r="B21" s="188"/>
+      <c r="C21" s="205"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="183"/>
-      <c r="B22" s="184"/>
-      <c r="C22" s="207"/>
+      <c r="A22" s="179"/>
+      <c r="B22" s="188"/>
+      <c r="C22" s="205"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="183"/>
-      <c r="B23" s="184"/>
-      <c r="C23" s="207"/>
+      <c r="A23" s="179"/>
+      <c r="B23" s="188"/>
+      <c r="C23" s="205"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31688,10 +31685,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="208" t="s">
+      <c r="A32" s="197" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="211" t="s">
+      <c r="B32" s="200" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31702,26 +31699,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="209"/>
-      <c r="B33" s="212"/>
+      <c r="A33" s="198"/>
+      <c r="B33" s="201"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="209"/>
-      <c r="B34" s="212"/>
+      <c r="A34" s="198"/>
+      <c r="B34" s="201"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="209"/>
-      <c r="B35" s="212"/>
+      <c r="A35" s="198"/>
+      <c r="B35" s="201"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="210"/>
-      <c r="B36" s="213"/>
+      <c r="A36" s="199"/>
+      <c r="B36" s="202"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31750,10 +31747,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="181" t="s">
+      <c r="A39" s="195" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="180" t="s">
+      <c r="B39" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31764,8 +31761,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="181"/>
-      <c r="B40" s="180"/>
+      <c r="A40" s="195"/>
+      <c r="B40" s="193"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31774,84 +31771,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="179" t="s">
+      <c r="A41" s="194" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="180" t="s">
+      <c r="B41" s="193" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="204" t="s">
+      <c r="C41" s="206" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="183" t="s">
+      <c r="D41" s="179" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="179"/>
-      <c r="B42" s="180"/>
-      <c r="C42" s="204"/>
-      <c r="D42" s="183"/>
+      <c r="A42" s="194"/>
+      <c r="B42" s="193"/>
+      <c r="C42" s="206"/>
+      <c r="D42" s="179"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="179"/>
-      <c r="B43" s="180"/>
-      <c r="C43" s="204" t="s">
+      <c r="A43" s="194"/>
+      <c r="B43" s="193"/>
+      <c r="C43" s="206" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="186" t="s">
+      <c r="D43" s="189" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="179"/>
-      <c r="B44" s="180"/>
-      <c r="C44" s="204"/>
-      <c r="D44" s="186"/>
+      <c r="A44" s="194"/>
+      <c r="B44" s="193"/>
+      <c r="C44" s="206"/>
+      <c r="D44" s="189"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="185" t="s">
+      <c r="A45" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="184" t="s">
+      <c r="B45" s="188" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="200"/>
+      <c r="C45" s="210"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="185"/>
-      <c r="B46" s="184"/>
-      <c r="C46" s="201"/>
-      <c r="D46" s="197" t="s">
+      <c r="A46" s="187"/>
+      <c r="B46" s="188"/>
+      <c r="C46" s="211"/>
+      <c r="D46" s="207" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="185"/>
-      <c r="B47" s="184"/>
-      <c r="C47" s="201"/>
-      <c r="D47" s="198"/>
+      <c r="A47" s="187"/>
+      <c r="B47" s="188"/>
+      <c r="C47" s="211"/>
+      <c r="D47" s="208"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="185"/>
-      <c r="B48" s="184"/>
-      <c r="C48" s="202"/>
-      <c r="D48" s="198"/>
+      <c r="A48" s="187"/>
+      <c r="B48" s="188"/>
+      <c r="C48" s="212"/>
+      <c r="D48" s="208"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="185"/>
-      <c r="B49" s="184"/>
-      <c r="C49" s="192"/>
-      <c r="D49" s="198"/>
+      <c r="A49" s="187"/>
+      <c r="B49" s="188"/>
+      <c r="C49" s="182"/>
+      <c r="D49" s="208"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="185"/>
-      <c r="B50" s="184"/>
-      <c r="C50" s="192"/>
-      <c r="D50" s="199"/>
+      <c r="A50" s="187"/>
+      <c r="B50" s="188"/>
+      <c r="C50" s="182"/>
+      <c r="D50" s="209"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31874,10 +31871,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="184" t="s">
+      <c r="A53" s="188" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="184" t="s">
+      <c r="B53" s="188" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31888,8 +31885,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="184"/>
-      <c r="B54" s="184"/>
+      <c r="A54" s="188"/>
+      <c r="B54" s="188"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31898,8 +31895,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="184"/>
-      <c r="B55" s="184"/>
+      <c r="A55" s="188"/>
+      <c r="B55" s="188"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31908,9 +31905,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="184"/>
-      <c r="B56" s="184"/>
-      <c r="C56" s="203" t="s">
+      <c r="A56" s="188"/>
+      <c r="B56" s="188"/>
+      <c r="C56" s="213" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31918,16 +31915,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="184"/>
-      <c r="B57" s="184"/>
-      <c r="C57" s="203"/>
+      <c r="A57" s="188"/>
+      <c r="B57" s="188"/>
+      <c r="C57" s="213"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="184"/>
-      <c r="B58" s="184"/>
+      <c r="A58" s="188"/>
+      <c r="B58" s="188"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31936,8 +31933,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="184"/>
-      <c r="B59" s="184"/>
+      <c r="A59" s="188"/>
+      <c r="B59" s="188"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31946,9 +31943,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="184"/>
-      <c r="B60" s="184"/>
-      <c r="C60" s="203" t="s">
+      <c r="A60" s="188"/>
+      <c r="B60" s="188"/>
+      <c r="C60" s="213" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31956,25 +31953,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="184"/>
-      <c r="B61" s="184"/>
-      <c r="C61" s="203"/>
+      <c r="A61" s="188"/>
+      <c r="B61" s="188"/>
+      <c r="C61" s="213"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="184"/>
-      <c r="B62" s="184"/>
-      <c r="C62" s="203"/>
+      <c r="A62" s="188"/>
+      <c r="B62" s="188"/>
+      <c r="C62" s="213"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="184"/>
-      <c r="B63" s="184"/>
-      <c r="C63" s="204" t="s">
+      <c r="A63" s="188"/>
+      <c r="B63" s="188"/>
+      <c r="C63" s="206" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31982,30 +31979,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="184"/>
-      <c r="B64" s="184"/>
-      <c r="C64" s="204"/>
-      <c r="D64" s="186" t="s">
+      <c r="A64" s="188"/>
+      <c r="B64" s="188"/>
+      <c r="C64" s="206"/>
+      <c r="D64" s="189" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="184"/>
-      <c r="B65" s="184"/>
-      <c r="C65" s="204"/>
-      <c r="D65" s="186"/>
+      <c r="A65" s="188"/>
+      <c r="B65" s="188"/>
+      <c r="C65" s="206"/>
+      <c r="D65" s="189"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="184"/>
-      <c r="B66" s="184"/>
-      <c r="C66" s="204"/>
-      <c r="D66" s="186"/>
+      <c r="A66" s="188"/>
+      <c r="B66" s="188"/>
+      <c r="C66" s="206"/>
+      <c r="D66" s="189"/>
     </row>
     <row r="67" spans="1:4" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="184"/>
-      <c r="B67" s="184"/>
-      <c r="C67" s="204"/>
-      <c r="D67" s="186"/>
+      <c r="A67" s="188"/>
+      <c r="B67" s="188"/>
+      <c r="C67" s="206"/>
+      <c r="D67" s="189"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -32061,23 +32058,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -32094,6 +32074,23 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -32173,7 +32170,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="223" t="s">
+      <c r="A6" s="222" t="s">
         <v>438</v>
       </c>
       <c r="B6" s="217" t="s">
@@ -32185,7 +32182,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="224"/>
+      <c r="A7" s="223"/>
       <c r="B7" s="218"/>
       <c r="C7" s="100"/>
       <c r="D7" s="58" t="s">
@@ -32193,7 +32190,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="224"/>
+      <c r="A8" s="223"/>
       <c r="B8" s="218"/>
       <c r="C8" s="100"/>
       <c r="D8" s="140" t="s">
@@ -32201,7 +32198,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="224"/>
+      <c r="A9" s="223"/>
       <c r="B9" s="218"/>
       <c r="C9" s="100"/>
       <c r="D9" s="140" t="s">
@@ -32209,7 +32206,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="225"/>
+      <c r="A10" s="224"/>
       <c r="B10" s="219"/>
       <c r="C10" s="100" t="s">
         <v>498</v>
@@ -32261,7 +32258,7 @@
       <c r="D14" s="104"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="227" t="s">
+      <c r="A15" s="234" t="s">
         <v>247</v>
       </c>
       <c r="B15" s="217" t="s">
@@ -32275,7 +32272,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="228"/>
+      <c r="A16" s="236"/>
       <c r="B16" s="219"/>
       <c r="C16" s="128" t="s">
         <v>474</v>
@@ -32415,7 +32412,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="223" t="s">
+      <c r="A29" s="222" t="s">
         <v>452</v>
       </c>
       <c r="B29" s="217" t="s">
@@ -32429,7 +32426,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="224"/>
+      <c r="A30" s="223"/>
       <c r="B30" s="218"/>
       <c r="C30" s="100" t="s">
         <v>453</v>
@@ -32439,7 +32436,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="224"/>
+      <c r="A31" s="223"/>
       <c r="B31" s="218"/>
       <c r="C31" s="100">
         <v>3.3</v>
@@ -32449,7 +32446,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="224"/>
+      <c r="A32" s="223"/>
       <c r="B32" s="218"/>
       <c r="C32" s="130">
         <v>3</v>
@@ -32459,7 +32456,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="225"/>
+      <c r="A33" s="224"/>
       <c r="B33" s="219"/>
       <c r="C33" s="130">
         <v>3.5</v>
@@ -32469,7 +32466,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="223" t="s">
+      <c r="A34" s="222" t="s">
         <v>457</v>
       </c>
       <c r="B34" s="217" t="s">
@@ -32481,7 +32478,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="225"/>
+      <c r="A35" s="224"/>
       <c r="B35" s="219"/>
       <c r="C35" s="100"/>
       <c r="D35" s="67" t="s">
@@ -32489,7 +32486,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="226" t="s">
+      <c r="A36" s="246" t="s">
         <v>501</v>
       </c>
       <c r="B36" s="217" t="s">
@@ -32500,7 +32497,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="226"/>
+      <c r="A37" s="246"/>
       <c r="B37" s="218"/>
       <c r="C37" s="144" t="s">
         <v>508</v>
@@ -32510,7 +32507,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="226"/>
+      <c r="A38" s="246"/>
       <c r="B38" s="218"/>
       <c r="C38" s="58" t="s">
         <v>506</v>
@@ -32520,7 +32517,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="226"/>
+      <c r="A39" s="246"/>
       <c r="B39" s="218"/>
       <c r="C39" s="61" t="s">
         <v>509</v>
@@ -32586,7 +32583,7 @@
       <c r="B45" s="217" t="s">
         <v>439</v>
       </c>
-      <c r="C45" s="229"/>
+      <c r="C45" s="241"/>
       <c r="D45" s="145" t="s">
         <v>510</v>
       </c>
@@ -32594,7 +32591,7 @@
     <row r="46" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="216"/>
       <c r="B46" s="219"/>
-      <c r="C46" s="230"/>
+      <c r="C46" s="242"/>
       <c r="D46" s="145" t="s">
         <v>518</v>
       </c>
@@ -32644,10 +32641,10 @@
       <c r="D50" s="104"/>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="226" t="s">
+      <c r="A51" s="246" t="s">
         <v>336</v>
       </c>
-      <c r="B51" s="235" t="s">
+      <c r="B51" s="247" t="s">
         <v>439</v>
       </c>
       <c r="C51" s="100" t="s">
@@ -32658,8 +32655,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="226"/>
-      <c r="B52" s="235"/>
+      <c r="A52" s="246"/>
+      <c r="B52" s="247"/>
       <c r="C52" s="100" t="s">
         <v>341</v>
       </c>
@@ -32668,8 +32665,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="226"/>
-      <c r="B53" s="235"/>
+      <c r="A53" s="246"/>
+      <c r="B53" s="247"/>
       <c r="C53" s="100" t="s">
         <v>337</v>
       </c>
@@ -32686,10 +32683,10 @@
       <c r="D54" s="104"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="236" t="s">
+      <c r="A55" s="237" t="s">
         <v>3</v>
       </c>
-      <c r="B55" s="231" t="s">
+      <c r="B55" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C55" s="106"/>
@@ -32698,8 +32695,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="236"/>
-      <c r="B56" s="231"/>
+      <c r="A56" s="237"/>
+      <c r="B56" s="238"/>
       <c r="C56" s="136" t="s">
         <v>234</v>
       </c>
@@ -32708,8 +32705,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="236"/>
-      <c r="B57" s="231"/>
+      <c r="A57" s="237"/>
+      <c r="B57" s="238"/>
       <c r="C57" s="139" t="s">
         <v>484</v>
       </c>
@@ -32718,8 +32715,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="236"/>
-      <c r="B58" s="231"/>
+      <c r="A58" s="237"/>
+      <c r="B58" s="238"/>
       <c r="C58" s="141" t="s">
         <v>484</v>
       </c>
@@ -32728,8 +32725,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="236"/>
-      <c r="B59" s="231"/>
+      <c r="A59" s="237"/>
+      <c r="B59" s="238"/>
       <c r="C59" s="139" t="s">
         <v>498</v>
       </c>
@@ -32738,8 +32735,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="236"/>
-      <c r="B60" s="231"/>
+      <c r="A60" s="237"/>
+      <c r="B60" s="238"/>
       <c r="C60" s="112" t="s">
         <v>498</v>
       </c>
@@ -32748,7 +32745,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="227" t="s">
+      <c r="A61" s="234" t="s">
         <v>74</v>
       </c>
       <c r="B61" s="217" t="s">
@@ -32762,7 +32759,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="239"/>
+      <c r="A62" s="235"/>
       <c r="B62" s="218"/>
       <c r="C62" s="136" t="s">
         <v>463</v>
@@ -32772,7 +32769,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="228"/>
+      <c r="A63" s="236"/>
       <c r="B63" s="219"/>
       <c r="C63" s="137" t="s">
         <v>481</v>
@@ -32822,10 +32819,10 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="236" t="s">
+      <c r="A67" s="237" t="s">
         <v>269</v>
       </c>
-      <c r="B67" s="231" t="s">
+      <c r="B67" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C67" s="106" t="s">
@@ -32836,24 +32833,24 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="236"/>
-      <c r="B68" s="231"/>
+      <c r="A68" s="237"/>
+      <c r="B68" s="238"/>
       <c r="C68" s="106"/>
       <c r="D68" s="80" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="236"/>
-      <c r="B69" s="231"/>
+      <c r="A69" s="237"/>
+      <c r="B69" s="238"/>
       <c r="C69" s="106"/>
       <c r="D69" s="106" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="236"/>
-      <c r="B70" s="231"/>
+      <c r="A70" s="237"/>
+      <c r="B70" s="238"/>
       <c r="C70" s="111" t="s">
         <v>319</v>
       </c>
@@ -32862,8 +32859,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="236"/>
-      <c r="B71" s="231"/>
+      <c r="A71" s="237"/>
+      <c r="B71" s="238"/>
       <c r="C71" s="112" t="s">
         <v>398</v>
       </c>
@@ -32884,7 +32881,7 @@
       <c r="D72" s="106"/>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="232" t="s">
+      <c r="A73" s="243" t="s">
         <v>165</v>
       </c>
       <c r="B73" s="217" t="s">
@@ -32896,7 +32893,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="233"/>
+      <c r="A74" s="244"/>
       <c r="B74" s="218"/>
       <c r="C74" s="112" t="s">
         <v>355</v>
@@ -32906,7 +32903,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="233"/>
+      <c r="A75" s="244"/>
       <c r="B75" s="218"/>
       <c r="C75" s="112" t="s">
         <v>353</v>
@@ -32916,7 +32913,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="233"/>
+      <c r="A76" s="244"/>
       <c r="B76" s="218"/>
       <c r="C76" s="115" t="s">
         <v>361</v>
@@ -32926,7 +32923,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="233"/>
+      <c r="A77" s="244"/>
       <c r="B77" s="218"/>
       <c r="C77" s="112" t="s">
         <v>353</v>
@@ -32936,7 +32933,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="233"/>
+      <c r="A78" s="244"/>
       <c r="B78" s="218"/>
       <c r="C78" s="112" t="s">
         <v>365</v>
@@ -32946,7 +32943,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="233"/>
+      <c r="A79" s="244"/>
       <c r="B79" s="218"/>
       <c r="C79" s="112" t="s">
         <v>353</v>
@@ -32956,7 +32953,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="233"/>
+      <c r="A80" s="244"/>
       <c r="B80" s="218"/>
       <c r="C80" s="112" t="s">
         <v>464</v>
@@ -32966,7 +32963,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="233"/>
+      <c r="A81" s="244"/>
       <c r="B81" s="218"/>
       <c r="C81" s="133" t="s">
         <v>466</v>
@@ -32976,7 +32973,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="233"/>
+      <c r="A82" s="244"/>
       <c r="B82" s="218"/>
       <c r="C82" s="133" t="s">
         <v>353</v>
@@ -32986,7 +32983,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="233"/>
+      <c r="A83" s="244"/>
       <c r="B83" s="218"/>
       <c r="C83" s="138" t="s">
         <v>466</v>
@@ -32996,7 +32993,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="233"/>
+      <c r="A84" s="244"/>
       <c r="B84" s="218"/>
       <c r="C84" s="112" t="s">
         <v>353</v>
@@ -33006,7 +33003,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="233"/>
+      <c r="A85" s="244"/>
       <c r="B85" s="218"/>
       <c r="C85" s="112" t="s">
         <v>498</v>
@@ -33016,7 +33013,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="233"/>
+      <c r="A86" s="244"/>
       <c r="B86" s="218"/>
       <c r="C86" s="112" t="s">
         <v>498</v>
@@ -33026,7 +33023,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="233"/>
+      <c r="A87" s="244"/>
       <c r="B87" s="218"/>
       <c r="C87" s="151" t="s">
         <v>520</v>
@@ -33036,7 +33033,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="234"/>
+      <c r="A88" s="245"/>
       <c r="B88" s="219"/>
       <c r="C88" s="112" t="s">
         <v>498</v>
@@ -33086,7 +33083,7 @@
       <c r="D91" s="113"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="240" t="s">
+      <c r="A92" s="225" t="s">
         <v>363</v>
       </c>
       <c r="B92" s="217" t="s">
@@ -33098,7 +33095,7 @@
       <c r="D92" s="113"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="244"/>
+      <c r="A93" s="226"/>
       <c r="B93" s="219"/>
       <c r="C93" s="112" t="s">
         <v>398</v>
@@ -33116,7 +33113,7 @@
       <c r="D94" s="103"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="240" t="s">
+      <c r="A95" s="225" t="s">
         <v>236</v>
       </c>
       <c r="B95" s="217" t="s">
@@ -33128,7 +33125,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="241"/>
+      <c r="A96" s="227"/>
       <c r="B96" s="218"/>
       <c r="C96" s="106"/>
       <c r="D96" s="106" t="s">
@@ -33136,7 +33133,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="241"/>
+      <c r="A97" s="227"/>
       <c r="B97" s="218"/>
       <c r="C97" s="106"/>
       <c r="D97" s="106" t="s">
@@ -33144,7 +33141,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="241"/>
+      <c r="A98" s="227"/>
       <c r="B98" s="218"/>
       <c r="C98" s="106" t="s">
         <v>294</v>
@@ -33154,7 +33151,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="241"/>
+      <c r="A99" s="227"/>
       <c r="B99" s="218"/>
       <c r="C99" s="106" t="s">
         <v>322</v>
@@ -33164,7 +33161,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="241"/>
+      <c r="A100" s="227"/>
       <c r="B100" s="218"/>
       <c r="C100" s="106" t="s">
         <v>367</v>
@@ -33174,7 +33171,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="241"/>
+      <c r="A101" s="227"/>
       <c r="B101" s="218"/>
       <c r="C101" s="119" t="s">
         <v>468</v>
@@ -33184,7 +33181,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="241"/>
+      <c r="A102" s="227"/>
       <c r="B102" s="218"/>
       <c r="C102" s="58" t="s">
         <v>37</v>
@@ -33194,7 +33191,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="241"/>
+      <c r="A103" s="227"/>
       <c r="B103" s="218"/>
       <c r="C103" s="130" t="s">
         <v>353</v>
@@ -33204,7 +33201,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="241"/>
+      <c r="A104" s="227"/>
       <c r="B104" s="218"/>
       <c r="C104" s="130" t="s">
         <v>466</v>
@@ -33214,7 +33211,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="241"/>
+      <c r="A105" s="227"/>
       <c r="B105" s="218"/>
       <c r="C105" s="130" t="s">
         <v>367</v>
@@ -33224,7 +33221,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="241"/>
+      <c r="A106" s="227"/>
       <c r="B106" s="218"/>
       <c r="C106" s="130" t="s">
         <v>353</v>
@@ -33234,7 +33231,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="241"/>
+      <c r="A107" s="227"/>
       <c r="B107" s="218"/>
       <c r="C107" s="130" t="s">
         <v>498</v>
@@ -33244,7 +33241,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="241"/>
+      <c r="A108" s="227"/>
       <c r="B108" s="218"/>
       <c r="C108" s="109" t="s">
         <v>498</v>
@@ -33254,7 +33251,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="241"/>
+      <c r="A109" s="227"/>
       <c r="B109" s="218"/>
       <c r="C109" s="151" t="s">
         <v>520</v>
@@ -33264,7 +33261,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="244"/>
+      <c r="A110" s="226"/>
       <c r="B110" s="219"/>
       <c r="C110" s="109" t="s">
         <v>498</v>
@@ -33274,7 +33271,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="245" t="s">
+      <c r="A111" s="228" t="s">
         <v>27</v>
       </c>
       <c r="B111" s="217" t="s">
@@ -33288,7 +33285,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="246"/>
+      <c r="A112" s="229"/>
       <c r="B112" s="218"/>
       <c r="C112" s="106" t="s">
         <v>297</v>
@@ -33298,7 +33295,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="246"/>
+      <c r="A113" s="229"/>
       <c r="B113" s="218"/>
       <c r="C113" s="106"/>
       <c r="D113" s="106" t="s">
@@ -33306,7 +33303,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="246"/>
+      <c r="A114" s="229"/>
       <c r="B114" s="218"/>
       <c r="C114" s="117" t="s">
         <v>323</v>
@@ -33316,7 +33313,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="246"/>
+      <c r="A115" s="229"/>
       <c r="B115" s="218"/>
       <c r="C115" s="117" t="s">
         <v>353</v>
@@ -33326,7 +33323,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="246"/>
+      <c r="A116" s="229"/>
       <c r="B116" s="218"/>
       <c r="C116" s="117" t="s">
         <v>361</v>
@@ -33336,7 +33333,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="246"/>
+      <c r="A117" s="229"/>
       <c r="B117" s="218"/>
       <c r="C117" s="117" t="s">
         <v>365</v>
@@ -33346,7 +33343,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="246"/>
+      <c r="A118" s="229"/>
       <c r="B118" s="218"/>
       <c r="C118" s="117" t="s">
         <v>375</v>
@@ -33356,7 +33353,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="246"/>
+      <c r="A119" s="229"/>
       <c r="B119" s="218"/>
       <c r="C119" s="109" t="s">
         <v>353</v>
@@ -33366,7 +33363,7 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="246"/>
+      <c r="A120" s="229"/>
       <c r="B120" s="218"/>
       <c r="C120" s="109" t="s">
         <v>464</v>
@@ -33376,7 +33373,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="246"/>
+      <c r="A121" s="229"/>
       <c r="B121" s="218"/>
       <c r="C121" s="130" t="s">
         <v>466</v>
@@ -33386,7 +33383,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="246"/>
+      <c r="A122" s="229"/>
       <c r="B122" s="218"/>
       <c r="C122" s="130" t="s">
         <v>353</v>
@@ -33396,7 +33393,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="246"/>
+      <c r="A123" s="229"/>
       <c r="B123" s="218"/>
       <c r="C123" s="130" t="s">
         <v>466</v>
@@ -33406,7 +33403,7 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="246"/>
+      <c r="A124" s="229"/>
       <c r="B124" s="218"/>
       <c r="C124" s="130" t="s">
         <v>367</v>
@@ -33416,7 +33413,7 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="246"/>
+      <c r="A125" s="229"/>
       <c r="B125" s="218"/>
       <c r="C125" s="130" t="s">
         <v>353</v>
@@ -33426,7 +33423,7 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="246"/>
+      <c r="A126" s="229"/>
       <c r="B126" s="218"/>
       <c r="C126" s="130" t="s">
         <v>498</v>
@@ -33436,7 +33433,7 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="246"/>
+      <c r="A127" s="229"/>
       <c r="B127" s="218"/>
       <c r="C127" s="109" t="s">
         <v>498</v>
@@ -33446,7 +33443,7 @@
       </c>
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="246"/>
+      <c r="A128" s="229"/>
       <c r="B128" s="218"/>
       <c r="C128" s="151" t="s">
         <v>520</v>
@@ -33456,7 +33453,7 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="247"/>
+      <c r="A129" s="230"/>
       <c r="B129" s="219"/>
       <c r="C129" s="109" t="s">
         <v>498</v>
@@ -33466,13 +33463,13 @@
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="227" t="s">
+      <c r="A130" s="234" t="s">
         <v>222</v>
       </c>
       <c r="B130" s="217" t="s">
         <v>439</v>
       </c>
-      <c r="C130" s="248" t="s">
+      <c r="C130" s="231" t="s">
         <v>238</v>
       </c>
       <c r="D130" s="96" t="s">
@@ -33480,17 +33477,17 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="239"/>
+      <c r="A131" s="235"/>
       <c r="B131" s="218"/>
-      <c r="C131" s="249"/>
+      <c r="C131" s="232"/>
       <c r="D131" s="113" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="239"/>
+      <c r="A132" s="235"/>
       <c r="B132" s="218"/>
-      <c r="C132" s="250" t="s">
+      <c r="C132" s="233" t="s">
         <v>239</v>
       </c>
       <c r="D132" s="106" t="s">
@@ -33498,15 +33495,15 @@
       </c>
     </row>
     <row r="133" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="239"/>
+      <c r="A133" s="235"/>
       <c r="B133" s="218"/>
-      <c r="C133" s="250"/>
+      <c r="C133" s="233"/>
       <c r="D133" s="119" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="239"/>
+      <c r="A134" s="235"/>
       <c r="B134" s="218"/>
       <c r="C134" s="112" t="s">
         <v>301</v>
@@ -33516,7 +33513,7 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="239"/>
+      <c r="A135" s="235"/>
       <c r="B135" s="218"/>
       <c r="C135" s="112">
         <v>2.1</v>
@@ -33526,7 +33523,7 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="239"/>
+      <c r="A136" s="235"/>
       <c r="B136" s="218"/>
       <c r="C136" s="112" t="s">
         <v>238</v>
@@ -33536,7 +33533,7 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="239"/>
+      <c r="A137" s="235"/>
       <c r="B137" s="218"/>
       <c r="C137" s="112" t="s">
         <v>238</v>
@@ -33546,7 +33543,7 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="239"/>
+      <c r="A138" s="235"/>
       <c r="B138" s="218"/>
       <c r="C138" s="112" t="s">
         <v>238</v>
@@ -33556,7 +33553,7 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="239"/>
+      <c r="A139" s="235"/>
       <c r="B139" s="218"/>
       <c r="C139" s="120" t="s">
         <v>372</v>
@@ -33566,7 +33563,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="239"/>
+      <c r="A140" s="235"/>
       <c r="B140" s="218"/>
       <c r="C140" s="112">
         <v>2.1</v>
@@ -33576,7 +33573,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="239"/>
+      <c r="A141" s="235"/>
       <c r="B141" s="218"/>
       <c r="C141" s="112" t="s">
         <v>238</v>
@@ -33586,7 +33583,7 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="239"/>
+      <c r="A142" s="235"/>
       <c r="B142" s="218"/>
       <c r="C142" s="112" t="s">
         <v>238</v>
@@ -33596,7 +33593,7 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="239"/>
+      <c r="A143" s="235"/>
       <c r="B143" s="218"/>
       <c r="C143" s="112">
         <v>2.1</v>
@@ -33606,7 +33603,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="245" t="s">
+      <c r="A144" s="228" t="s">
         <v>290</v>
       </c>
       <c r="B144" s="217" t="s">
@@ -33620,7 +33617,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145" s="246"/>
+      <c r="A145" s="229"/>
       <c r="B145" s="218"/>
       <c r="C145" s="119" t="s">
         <v>275</v>
@@ -33630,7 +33627,7 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="247"/>
+      <c r="A146" s="230"/>
       <c r="B146" s="219"/>
       <c r="C146" s="106" t="s">
         <v>344</v>
@@ -33640,7 +33637,7 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="240" t="s">
+      <c r="A147" s="225" t="s">
         <v>364</v>
       </c>
       <c r="B147" s="217" t="s">
@@ -33652,7 +33649,7 @@
       <c r="D147" s="106"/>
     </row>
     <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="241"/>
+      <c r="A148" s="227"/>
       <c r="B148" s="218"/>
       <c r="C148" s="112" t="s">
         <v>372</v>
@@ -33662,7 +33659,7 @@
       </c>
     </row>
     <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="241"/>
+      <c r="A149" s="227"/>
       <c r="B149" s="218"/>
       <c r="C149" s="112">
         <v>2.1</v>
@@ -33672,7 +33669,7 @@
       </c>
     </row>
     <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="241"/>
+      <c r="A150" s="227"/>
       <c r="B150" s="218"/>
       <c r="C150" s="112" t="s">
         <v>239</v>
@@ -33682,7 +33679,7 @@
       </c>
     </row>
     <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="241"/>
+      <c r="A151" s="227"/>
       <c r="B151" s="218"/>
       <c r="C151" s="112" t="s">
         <v>238</v>
@@ -33712,7 +33709,7 @@
       <c r="D153" s="113"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="227" t="s">
+      <c r="A154" s="234" t="s">
         <v>255</v>
       </c>
       <c r="B154" s="217" t="s">
@@ -33724,7 +33721,7 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="239"/>
+      <c r="A155" s="235"/>
       <c r="B155" s="218"/>
       <c r="C155" s="106"/>
       <c r="D155" s="106" t="s">
@@ -33732,7 +33729,7 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="239"/>
+      <c r="A156" s="235"/>
       <c r="B156" s="218"/>
       <c r="C156" s="106"/>
       <c r="D156" s="113" t="s">
@@ -33740,7 +33737,7 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="239"/>
+      <c r="A157" s="235"/>
       <c r="B157" s="218"/>
       <c r="C157" s="106" t="s">
         <v>418</v>
@@ -33750,7 +33747,7 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="239"/>
+      <c r="A158" s="235"/>
       <c r="B158" s="218"/>
       <c r="C158" s="106" t="s">
         <v>423</v>
@@ -33760,7 +33757,7 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="239"/>
+      <c r="A159" s="235"/>
       <c r="B159" s="218"/>
       <c r="C159" s="106" t="s">
         <v>484</v>
@@ -33770,7 +33767,7 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="239"/>
+      <c r="A160" s="235"/>
       <c r="B160" s="218"/>
       <c r="C160" s="106" t="s">
         <v>498</v>
@@ -33780,10 +33777,10 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="236" t="s">
+      <c r="A161" s="237" t="s">
         <v>328</v>
       </c>
-      <c r="B161" s="231" t="s">
+      <c r="B161" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C161" s="80" t="s">
@@ -33794,8 +33791,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="236"/>
-      <c r="B162" s="231"/>
+      <c r="A162" s="237"/>
+      <c r="B162" s="238"/>
       <c r="C162" s="106" t="s">
         <v>405</v>
       </c>
@@ -33804,42 +33801,42 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="236"/>
-      <c r="B163" s="231"/>
+      <c r="A163" s="237"/>
+      <c r="B163" s="238"/>
       <c r="C163" s="122" t="s">
         <v>408</v>
       </c>
-      <c r="D163" s="242" t="s">
+      <c r="D163" s="220" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A164" s="236"/>
-      <c r="B164" s="231"/>
+      <c r="A164" s="237"/>
+      <c r="B164" s="238"/>
       <c r="C164" s="122" t="s">
         <v>409</v>
       </c>
-      <c r="D164" s="243"/>
+      <c r="D164" s="221"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="236"/>
-      <c r="B165" s="231"/>
+      <c r="A165" s="237"/>
+      <c r="B165" s="238"/>
       <c r="C165" s="122" t="s">
         <v>410</v>
       </c>
-      <c r="D165" s="243"/>
+      <c r="D165" s="221"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="236"/>
-      <c r="B166" s="231"/>
+      <c r="A166" s="237"/>
+      <c r="B166" s="238"/>
       <c r="C166" s="122" t="s">
         <v>411</v>
       </c>
-      <c r="D166" s="243"/>
+      <c r="D166" s="221"/>
     </row>
     <row r="167" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="236"/>
-      <c r="B167" s="231"/>
+      <c r="A167" s="237"/>
+      <c r="B167" s="238"/>
       <c r="C167" s="122" t="s">
         <v>470</v>
       </c>
@@ -33862,7 +33859,7 @@
       </c>
     </row>
     <row r="169" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="220" t="s">
+      <c r="A169" s="248" t="s">
         <v>32</v>
       </c>
       <c r="B169" s="217" t="s">
@@ -33876,7 +33873,7 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="221"/>
+      <c r="A170" s="249"/>
       <c r="B170" s="218"/>
       <c r="C170" s="106" t="s">
         <v>264</v>
@@ -33886,7 +33883,7 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="221"/>
+      <c r="A171" s="249"/>
       <c r="B171" s="218"/>
       <c r="C171" s="106" t="s">
         <v>263</v>
@@ -33896,7 +33893,7 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="221"/>
+      <c r="A172" s="249"/>
       <c r="B172" s="218"/>
       <c r="C172" s="113" t="s">
         <v>271</v>
@@ -33906,7 +33903,7 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="221"/>
+      <c r="A173" s="249"/>
       <c r="B173" s="218"/>
       <c r="C173" s="106" t="s">
         <v>276</v>
@@ -33916,7 +33913,7 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="221"/>
+      <c r="A174" s="249"/>
       <c r="B174" s="218"/>
       <c r="C174" s="106" t="s">
         <v>277</v>
@@ -33926,7 +33923,7 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="221"/>
+      <c r="A175" s="249"/>
       <c r="B175" s="218"/>
       <c r="C175" s="113" t="s">
         <v>282</v>
@@ -33936,7 +33933,7 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="221"/>
+      <c r="A176" s="249"/>
       <c r="B176" s="218"/>
       <c r="C176" s="113" t="s">
         <v>296</v>
@@ -33946,7 +33943,7 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="221"/>
+      <c r="A177" s="249"/>
       <c r="B177" s="218"/>
       <c r="C177" s="113" t="s">
         <v>283</v>
@@ -33956,7 +33953,7 @@
       </c>
     </row>
     <row r="178" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" s="221"/>
+      <c r="A178" s="249"/>
       <c r="B178" s="218"/>
       <c r="C178" s="123" t="s">
         <v>243</v>
@@ -33966,7 +33963,7 @@
       </c>
     </row>
     <row r="179" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A179" s="221"/>
+      <c r="A179" s="249"/>
       <c r="B179" s="218"/>
       <c r="C179" s="117" t="s">
         <v>305</v>
@@ -33976,7 +33973,7 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="221"/>
+      <c r="A180" s="249"/>
       <c r="B180" s="218"/>
       <c r="C180" s="106" t="s">
         <v>306</v>
@@ -33986,7 +33983,7 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="221"/>
+      <c r="A181" s="249"/>
       <c r="B181" s="218"/>
       <c r="C181" s="113" t="s">
         <v>307</v>
@@ -33996,7 +33993,7 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="221"/>
+      <c r="A182" s="249"/>
       <c r="B182" s="218"/>
       <c r="C182" s="113" t="s">
         <v>309</v>
@@ -34006,7 +34003,7 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="221"/>
+      <c r="A183" s="249"/>
       <c r="B183" s="218"/>
       <c r="C183" s="113" t="s">
         <v>262</v>
@@ -34016,7 +34013,7 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="221"/>
+      <c r="A184" s="249"/>
       <c r="B184" s="218"/>
       <c r="C184" s="106" t="s">
         <v>312</v>
@@ -34026,7 +34023,7 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="221"/>
+      <c r="A185" s="249"/>
       <c r="B185" s="218"/>
       <c r="C185" s="113" t="s">
         <v>277</v>
@@ -34036,7 +34033,7 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="221"/>
+      <c r="A186" s="249"/>
       <c r="B186" s="218"/>
       <c r="C186" s="113" t="s">
         <v>313</v>
@@ -34046,7 +34043,7 @@
       </c>
     </row>
     <row r="187" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A187" s="221"/>
+      <c r="A187" s="249"/>
       <c r="B187" s="218"/>
       <c r="C187" s="106"/>
       <c r="D187" s="97" t="s">
@@ -34054,7 +34051,7 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="221"/>
+      <c r="A188" s="249"/>
       <c r="B188" s="218"/>
       <c r="C188" s="113" t="s">
         <v>316</v>
@@ -34064,7 +34061,7 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="221"/>
+      <c r="A189" s="249"/>
       <c r="B189" s="218"/>
       <c r="C189" s="113" t="s">
         <v>262</v>
@@ -34074,7 +34071,7 @@
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="221"/>
+      <c r="A190" s="249"/>
       <c r="B190" s="218"/>
       <c r="C190" s="113" t="s">
         <v>333</v>
@@ -34084,7 +34081,7 @@
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="221"/>
+      <c r="A191" s="249"/>
       <c r="B191" s="218"/>
       <c r="C191" s="113" t="s">
         <v>334</v>
@@ -34094,7 +34091,7 @@
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="221"/>
+      <c r="A192" s="249"/>
       <c r="B192" s="218"/>
       <c r="C192" s="113" t="s">
         <v>318</v>
@@ -34104,7 +34101,7 @@
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="221"/>
+      <c r="A193" s="249"/>
       <c r="B193" s="218"/>
       <c r="C193" s="113" t="s">
         <v>339</v>
@@ -34114,7 +34111,7 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="221"/>
+      <c r="A194" s="249"/>
       <c r="B194" s="218"/>
       <c r="C194" s="113" t="s">
         <v>332</v>
@@ -34124,7 +34121,7 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="221"/>
+      <c r="A195" s="249"/>
       <c r="B195" s="218"/>
       <c r="C195" s="113" t="s">
         <v>347</v>
@@ -34134,7 +34131,7 @@
       </c>
     </row>
     <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="221"/>
+      <c r="A196" s="249"/>
       <c r="B196" s="218"/>
       <c r="C196" s="101" t="s">
         <v>350</v>
@@ -34144,7 +34141,7 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="221"/>
+      <c r="A197" s="249"/>
       <c r="B197" s="218"/>
       <c r="C197" s="113" t="s">
         <v>351</v>
@@ -34154,7 +34151,7 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="221"/>
+      <c r="A198" s="249"/>
       <c r="B198" s="218"/>
       <c r="C198" s="113" t="s">
         <v>352</v>
@@ -34164,7 +34161,7 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="221"/>
+      <c r="A199" s="249"/>
       <c r="B199" s="218"/>
       <c r="C199" s="113" t="s">
         <v>358</v>
@@ -34174,7 +34171,7 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="221"/>
+      <c r="A200" s="249"/>
       <c r="B200" s="218"/>
       <c r="C200" s="113" t="s">
         <v>360</v>
@@ -34184,7 +34181,7 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="221"/>
+      <c r="A201" s="249"/>
       <c r="B201" s="218"/>
       <c r="C201" s="113" t="s">
         <v>366</v>
@@ -34194,7 +34191,7 @@
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="221"/>
+      <c r="A202" s="249"/>
       <c r="B202" s="218"/>
       <c r="C202" s="113" t="s">
         <v>358</v>
@@ -34204,7 +34201,7 @@
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="221"/>
+      <c r="A203" s="249"/>
       <c r="B203" s="218"/>
       <c r="C203" s="118" t="s">
         <v>379</v>
@@ -34214,7 +34211,7 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="221"/>
+      <c r="A204" s="249"/>
       <c r="B204" s="218"/>
       <c r="C204" s="106" t="s">
         <v>383</v>
@@ -34224,7 +34221,7 @@
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="221"/>
+      <c r="A205" s="249"/>
       <c r="B205" s="218"/>
       <c r="C205" s="106" t="s">
         <v>386</v>
@@ -34234,7 +34231,7 @@
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="221"/>
+      <c r="A206" s="249"/>
       <c r="B206" s="218"/>
       <c r="C206" s="106" t="s">
         <v>387</v>
@@ -34244,7 +34241,7 @@
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="221"/>
+      <c r="A207" s="249"/>
       <c r="B207" s="218"/>
       <c r="C207" s="106" t="s">
         <v>388</v>
@@ -34254,7 +34251,7 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="221"/>
+      <c r="A208" s="249"/>
       <c r="B208" s="218"/>
       <c r="C208" s="106" t="s">
         <v>389</v>
@@ -34264,7 +34261,7 @@
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="221"/>
+      <c r="A209" s="249"/>
       <c r="B209" s="218"/>
       <c r="C209" s="106" t="s">
         <v>390</v>
@@ -34274,7 +34271,7 @@
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="221"/>
+      <c r="A210" s="249"/>
       <c r="B210" s="218"/>
       <c r="C210" s="106" t="s">
         <v>393</v>
@@ -34284,7 +34281,7 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="221"/>
+      <c r="A211" s="249"/>
       <c r="B211" s="218"/>
       <c r="C211" s="106" t="s">
         <v>403</v>
@@ -34294,7 +34291,7 @@
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="221"/>
+      <c r="A212" s="249"/>
       <c r="B212" s="218"/>
       <c r="C212" s="106" t="s">
         <v>404</v>
@@ -34304,7 +34301,7 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="221"/>
+      <c r="A213" s="249"/>
       <c r="B213" s="218"/>
       <c r="C213" s="106" t="s">
         <v>421</v>
@@ -34314,7 +34311,7 @@
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="221"/>
+      <c r="A214" s="249"/>
       <c r="B214" s="218"/>
       <c r="C214" s="106" t="s">
         <v>422</v>
@@ -34324,7 +34321,7 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="221"/>
+      <c r="A215" s="249"/>
       <c r="B215" s="218"/>
       <c r="C215" s="106" t="s">
         <v>425</v>
@@ -34334,7 +34331,7 @@
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="221"/>
+      <c r="A216" s="249"/>
       <c r="B216" s="218"/>
       <c r="C216" s="58" t="s">
         <v>471</v>
@@ -34344,7 +34341,7 @@
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="221"/>
+      <c r="A217" s="249"/>
       <c r="B217" s="218"/>
       <c r="C217" s="58" t="s">
         <v>421</v>
@@ -34354,7 +34351,7 @@
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="221"/>
+      <c r="A218" s="249"/>
       <c r="B218" s="218"/>
       <c r="C218" s="58" t="s">
         <v>497</v>
@@ -34364,7 +34361,7 @@
       </c>
     </row>
     <row r="219" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A219" s="221"/>
+      <c r="A219" s="249"/>
       <c r="B219" s="218"/>
       <c r="C219" s="61" t="s">
         <v>522</v>
@@ -34374,7 +34371,7 @@
       </c>
     </row>
     <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A220" s="222"/>
+      <c r="A220" s="250"/>
       <c r="B220" s="219"/>
       <c r="C220" s="61" t="s">
         <v>332</v>
@@ -34384,7 +34381,7 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="220" t="s">
+      <c r="A221" s="248" t="s">
         <v>415</v>
       </c>
       <c r="B221" s="217" t="s">
@@ -34398,7 +34395,7 @@
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="221"/>
+      <c r="A222" s="249"/>
       <c r="B222" s="218"/>
       <c r="C222" s="118" t="s">
         <v>491</v>
@@ -34408,7 +34405,7 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="222"/>
+      <c r="A223" s="250"/>
       <c r="B223" s="219"/>
       <c r="C223" s="113" t="s">
         <v>524</v>
@@ -34454,7 +34451,7 @@
       <c r="D226" s="104"/>
     </row>
     <row r="227" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="227" t="s">
+      <c r="A227" s="234" t="s">
         <v>84</v>
       </c>
       <c r="B227" s="217" t="s">
@@ -34466,7 +34463,7 @@
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="239"/>
+      <c r="A228" s="235"/>
       <c r="B228" s="218"/>
       <c r="C228" s="107" t="s">
         <v>245</v>
@@ -34476,7 +34473,7 @@
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="239"/>
+      <c r="A229" s="235"/>
       <c r="B229" s="218"/>
       <c r="C229" s="107">
         <v>10.1</v>
@@ -34486,7 +34483,7 @@
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="239"/>
+      <c r="A230" s="235"/>
       <c r="B230" s="218"/>
       <c r="C230" s="107">
         <v>10.199999999999999</v>
@@ -34496,7 +34493,7 @@
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="239"/>
+      <c r="A231" s="235"/>
       <c r="B231" s="218"/>
       <c r="C231" s="98" t="s">
         <v>287</v>
@@ -34506,7 +34503,7 @@
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="239"/>
+      <c r="A232" s="235"/>
       <c r="B232" s="218"/>
       <c r="C232" s="98" t="s">
         <v>369</v>
@@ -34516,7 +34513,7 @@
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A233" s="239"/>
+      <c r="A233" s="235"/>
       <c r="B233" s="218"/>
       <c r="C233" s="98" t="s">
         <v>117</v>
@@ -34526,7 +34523,7 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A234" s="239"/>
+      <c r="A234" s="235"/>
       <c r="B234" s="218"/>
       <c r="C234" s="98" t="s">
         <v>416</v>
@@ -34536,7 +34533,7 @@
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A235" s="239"/>
+      <c r="A235" s="235"/>
       <c r="B235" s="218"/>
       <c r="C235" s="98" t="s">
         <v>17</v>
@@ -34546,7 +34543,7 @@
       </c>
     </row>
     <row r="236" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" s="239"/>
+      <c r="A236" s="235"/>
       <c r="B236" s="218"/>
       <c r="C236" s="98" t="s">
         <v>496</v>
@@ -34556,7 +34553,7 @@
       </c>
     </row>
     <row r="237" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A237" s="228"/>
+      <c r="A237" s="236"/>
       <c r="B237" s="219"/>
       <c r="C237" s="98" t="s">
         <v>496</v>
@@ -34566,7 +34563,7 @@
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A238" s="227" t="s">
+      <c r="A238" s="234" t="s">
         <v>246</v>
       </c>
       <c r="B238" s="217" t="s">
@@ -34578,7 +34575,7 @@
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A239" s="239"/>
+      <c r="A239" s="235"/>
       <c r="B239" s="218"/>
       <c r="C239" s="126" t="s">
         <v>427</v>
@@ -34610,7 +34607,7 @@
       <c r="D241" s="127"/>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A242" s="227" t="s">
+      <c r="A242" s="234" t="s">
         <v>58</v>
       </c>
       <c r="B242" s="217" t="s">
@@ -34624,7 +34621,7 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A243" s="239"/>
+      <c r="A243" s="235"/>
       <c r="B243" s="218"/>
       <c r="C243" s="128" t="s">
         <v>259</v>
@@ -34634,7 +34631,7 @@
       </c>
     </row>
     <row r="244" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="228"/>
+      <c r="A244" s="236"/>
       <c r="B244" s="219"/>
       <c r="C244" s="106"/>
       <c r="D244" s="106" t="s">
@@ -34642,7 +34639,7 @@
       </c>
     </row>
     <row r="245" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A245" s="237" t="s">
+      <c r="A245" s="239" t="s">
         <v>59</v>
       </c>
       <c r="B245" s="217" t="s">
@@ -34656,7 +34653,7 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A246" s="238"/>
+      <c r="A246" s="240"/>
       <c r="B246" s="219"/>
       <c r="C246" s="119"/>
       <c r="D246" s="106" t="s">
@@ -34664,7 +34661,7 @@
       </c>
     </row>
     <row r="247" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A247" s="237" t="s">
+      <c r="A247" s="239" t="s">
         <v>285</v>
       </c>
       <c r="B247" s="217" t="s">
@@ -34676,7 +34673,7 @@
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A248" s="238"/>
+      <c r="A248" s="240"/>
       <c r="B248" s="219"/>
       <c r="C248" s="106"/>
       <c r="D248" s="106" t="s">
@@ -34684,7 +34681,7 @@
       </c>
     </row>
     <row r="249" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="237" t="s">
+      <c r="A249" s="239" t="s">
         <v>60</v>
       </c>
       <c r="B249" s="217" t="s">
@@ -34698,7 +34695,7 @@
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A250" s="238"/>
+      <c r="A250" s="240"/>
       <c r="B250" s="219"/>
       <c r="C250" s="106"/>
       <c r="D250" s="106" t="s">
@@ -34757,6 +34754,56 @@
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B221:B223"/>
+    <mergeCell ref="A221:A223"/>
+    <mergeCell ref="B169:B220"/>
+    <mergeCell ref="A169:A220"/>
+    <mergeCell ref="A19:A28"/>
+    <mergeCell ref="B19:B28"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="A73:A88"/>
+    <mergeCell ref="B73:B88"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="A249:A250"/>
+    <mergeCell ref="B249:B250"/>
+    <mergeCell ref="A245:A246"/>
+    <mergeCell ref="B245:B246"/>
+    <mergeCell ref="A247:A248"/>
+    <mergeCell ref="B247:B248"/>
+    <mergeCell ref="A242:A244"/>
+    <mergeCell ref="B242:B244"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="B238:B239"/>
+    <mergeCell ref="B161:B167"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A161:A167"/>
+    <mergeCell ref="A227:A237"/>
+    <mergeCell ref="B227:B237"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B130:B143"/>
+    <mergeCell ref="A154:A160"/>
+    <mergeCell ref="B154:B160"/>
+    <mergeCell ref="A130:A143"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="D163:D166"/>
@@ -34773,56 +34820,6 @@
     <mergeCell ref="A144:A146"/>
     <mergeCell ref="B144:B146"/>
     <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A147:A151"/>
-    <mergeCell ref="B147:B151"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A161:A167"/>
-    <mergeCell ref="A227:A237"/>
-    <mergeCell ref="B227:B237"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B130:B143"/>
-    <mergeCell ref="A154:A160"/>
-    <mergeCell ref="B154:B160"/>
-    <mergeCell ref="A130:A143"/>
-    <mergeCell ref="A242:A244"/>
-    <mergeCell ref="B242:B244"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="B238:B239"/>
-    <mergeCell ref="B161:B167"/>
-    <mergeCell ref="A249:A250"/>
-    <mergeCell ref="B249:B250"/>
-    <mergeCell ref="A245:A246"/>
-    <mergeCell ref="B245:B246"/>
-    <mergeCell ref="A247:A248"/>
-    <mergeCell ref="B247:B248"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="A73:A88"/>
-    <mergeCell ref="B73:B88"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B221:B223"/>
-    <mergeCell ref="A221:A223"/>
-    <mergeCell ref="B169:B220"/>
-    <mergeCell ref="A169:A220"/>
-    <mergeCell ref="A19:A28"/>
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34831,10 +34828,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DBC65A-63D2-46B3-B8B5-A94A70B9EDFE}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34860,7 +34857,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="242" t="s">
+      <c r="A2" s="220" t="s">
         <v>236</v>
       </c>
       <c r="B2" s="217" t="s">
@@ -34874,7 +34871,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="243"/>
+      <c r="A3" s="221"/>
       <c r="B3" s="218"/>
       <c r="C3" s="58" t="s">
         <v>540</v>
@@ -34884,7 +34881,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="243"/>
+      <c r="A4" s="221"/>
       <c r="B4" s="218"/>
       <c r="C4" s="58" t="s">
         <v>541</v>
@@ -34894,7 +34891,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="243"/>
+      <c r="A5" s="221"/>
       <c r="B5" s="218"/>
       <c r="C5" s="58" t="s">
         <v>542</v>
@@ -34904,7 +34901,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="243"/>
+      <c r="A6" s="221"/>
       <c r="B6" s="218"/>
       <c r="C6" s="58" t="s">
         <v>543</v>
@@ -34914,7 +34911,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="243"/>
+      <c r="A7" s="221"/>
       <c r="B7" s="218"/>
       <c r="C7" s="58" t="s">
         <v>537</v>
@@ -34924,7 +34921,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="243"/>
+      <c r="A8" s="221"/>
       <c r="B8" s="218"/>
       <c r="C8" s="58" t="s">
         <v>544</v>
@@ -34934,7 +34931,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="243"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="218"/>
       <c r="C9" s="58" t="s">
         <v>545</v>
@@ -34944,7 +34941,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="243"/>
+      <c r="A10" s="221"/>
       <c r="B10" s="218"/>
       <c r="C10" s="58" t="s">
         <v>546</v>
@@ -34954,7 +34951,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="243"/>
+      <c r="A11" s="221"/>
       <c r="B11" s="218"/>
       <c r="C11" s="58" t="s">
         <v>547</v>
@@ -34964,7 +34961,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="243"/>
+      <c r="A12" s="221"/>
       <c r="B12" s="218"/>
       <c r="C12" s="58" t="s">
         <v>548</v>
@@ -34974,7 +34971,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="243"/>
+      <c r="A13" s="221"/>
       <c r="B13" s="218"/>
       <c r="C13" s="58" t="s">
         <v>539</v>
@@ -34984,7 +34981,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="243"/>
+      <c r="A14" s="221"/>
       <c r="B14" s="218"/>
       <c r="C14" s="58" t="s">
         <v>538</v>
@@ -34994,7 +34991,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="243"/>
+      <c r="A15" s="221"/>
       <c r="B15" s="218"/>
       <c r="C15" s="106" t="s">
         <v>552</v>
@@ -35004,30 +35001,30 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="243"/>
+      <c r="A16" s="221"/>
       <c r="B16" s="218"/>
       <c r="C16" s="58" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D16" s="119" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="243"/>
+      <c r="A17" s="221"/>
       <c r="B17" s="218"/>
       <c r="C17" s="119" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D17" s="119" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="243"/>
+      <c r="A18" s="221"/>
       <c r="B18" s="218"/>
       <c r="C18" s="58" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D18" s="119" t="s">
         <v>549</v>
@@ -35037,7 +35034,7 @@
       <c r="A19" s="251"/>
       <c r="B19" s="219"/>
       <c r="C19" s="119" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D19" s="119" t="s">
         <v>549</v>
@@ -35047,7 +35044,7 @@
       <c r="A20" s="252" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="231" t="s">
+      <c r="B20" s="238" t="s">
         <v>439</v>
       </c>
       <c r="C20" s="106" t="s">
@@ -35059,7 +35056,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="252"/>
-      <c r="B21" s="231"/>
+      <c r="B21" s="238"/>
       <c r="C21" s="58" t="s">
         <v>540</v>
       </c>
@@ -35069,7 +35066,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="252"/>
-      <c r="B22" s="231"/>
+      <c r="B22" s="238"/>
       <c r="C22" s="58" t="s">
         <v>541</v>
       </c>
@@ -35079,7 +35076,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="252"/>
-      <c r="B23" s="231"/>
+      <c r="B23" s="238"/>
       <c r="C23" s="58" t="s">
         <v>542</v>
       </c>
@@ -35089,7 +35086,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="252"/>
-      <c r="B24" s="231"/>
+      <c r="B24" s="238"/>
       <c r="C24" s="58" t="s">
         <v>543</v>
       </c>
@@ -35099,7 +35096,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="252"/>
-      <c r="B25" s="231"/>
+      <c r="B25" s="238"/>
       <c r="C25" s="58" t="s">
         <v>537</v>
       </c>
@@ -35109,7 +35106,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="252"/>
-      <c r="B26" s="231"/>
+      <c r="B26" s="238"/>
       <c r="C26" s="58" t="s">
         <v>544</v>
       </c>
@@ -35119,7 +35116,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="252"/>
-      <c r="B27" s="231"/>
+      <c r="B27" s="238"/>
       <c r="C27" s="58" t="s">
         <v>545</v>
       </c>
@@ -35129,7 +35126,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="252"/>
-      <c r="B28" s="231"/>
+      <c r="B28" s="238"/>
       <c r="C28" s="58" t="s">
         <v>546</v>
       </c>
@@ -35139,7 +35136,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="252"/>
-      <c r="B29" s="231"/>
+      <c r="B29" s="238"/>
       <c r="C29" s="58" t="s">
         <v>547</v>
       </c>
@@ -35149,7 +35146,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="252"/>
-      <c r="B30" s="231"/>
+      <c r="B30" s="238"/>
       <c r="C30" s="58" t="s">
         <v>548</v>
       </c>
@@ -35159,7 +35156,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="252"/>
-      <c r="B31" s="231"/>
+      <c r="B31" s="238"/>
       <c r="C31" s="58" t="s">
         <v>539</v>
       </c>
@@ -35169,7 +35166,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="252"/>
-      <c r="B32" s="231"/>
+      <c r="B32" s="238"/>
       <c r="C32" s="58" t="s">
         <v>538</v>
       </c>
@@ -35179,7 +35176,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="252"/>
-      <c r="B33" s="231"/>
+      <c r="B33" s="238"/>
       <c r="C33" s="106" t="s">
         <v>552</v>
       </c>
@@ -35189,9 +35186,9 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="252"/>
-      <c r="B34" s="231"/>
+      <c r="B34" s="238"/>
       <c r="C34" s="58" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D34" s="119" t="s">
         <v>549</v>
@@ -35199,9 +35196,9 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="252"/>
-      <c r="B35" s="231"/>
+      <c r="B35" s="238"/>
       <c r="C35" s="119" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D35" s="119" t="s">
         <v>549</v>
@@ -35209,9 +35206,9 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="252"/>
-      <c r="B36" s="231"/>
+      <c r="B36" s="238"/>
       <c r="C36" s="58" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D36" s="119" t="s">
         <v>549</v>
@@ -35219,9 +35216,9 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="252"/>
-      <c r="B37" s="231"/>
+      <c r="B37" s="238"/>
       <c r="C37" s="119" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D37" s="119" t="s">
         <v>549</v>
@@ -35245,20 +35242,20 @@
       <c r="A39" s="218"/>
       <c r="B39" s="218"/>
       <c r="C39" s="106" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D39" s="159" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="253"/>
       <c r="B40" s="253"/>
       <c r="C40" s="106" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D40" s="159" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -35268,9 +35265,7 @@
       <c r="B41" s="112" t="s">
         <v>439</v>
       </c>
-      <c r="C41" s="156" t="s">
-        <v>22</v>
-      </c>
+      <c r="C41" s="156"/>
       <c r="D41" s="155" t="s">
         <v>30</v>
       </c>
@@ -35293,20 +35288,20 @@
       <c r="A43" s="218"/>
       <c r="B43" s="218"/>
       <c r="C43" s="109" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D43" s="159" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="219"/>
       <c r="B44" s="219"/>
       <c r="C44" s="109" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D44" s="159" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -35347,7 +35342,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="126" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B48" s="162" t="s">
         <v>439</v>
@@ -35359,7 +35354,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="126" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B49" s="162" t="s">
         <v>439</v>
@@ -35370,26 +35365,14 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="126" t="s">
-        <v>558</v>
-      </c>
-      <c r="B50" s="161" t="s">
+      <c r="A50" s="131" t="s">
+        <v>570</v>
+      </c>
+      <c r="B50" s="163" t="s">
         <v>439</v>
       </c>
       <c r="C50" s="109"/>
-      <c r="D50" s="160" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="131" t="s">
-        <v>536</v>
-      </c>
-      <c r="B51" s="163" t="s">
-        <v>439</v>
-      </c>
-      <c r="C51" s="109"/>
-      <c r="D51" s="159" t="s">
+      <c r="D50" s="159" t="s">
         <v>557</v>
       </c>
     </row>

</xml_diff>